<commit_message>
Can now reverse the sort order.
Former-commit-id: d27d550c599f903707cab360b818688160108b14
</commit_message>
<xml_diff>
--- a/resources/modules-config-details-setup.xlsx
+++ b/resources/modules-config-details-setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\IdeaProjects\MakeMyManual\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70CE7370-5D84-4714-B62F-B9E6FA7ABF6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55954212-7916-41E2-B2D8-6D41D2A95E97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="407">
   <si>
     <t>Colour Flash</t>
   </si>
@@ -1212,6 +1212,48 @@
   </si>
   <si>
     <t>2017-07-02</t>
+  </si>
+  <si>
+    <t>German Button</t>
+  </si>
+  <si>
+    <t>BigButtonTranslated</t>
+  </si>
+  <si>
+    <t>./resources/modules/German Button.pdf</t>
+  </si>
+  <si>
+    <t>Malde, Tharagon</t>
+  </si>
+  <si>
+    <t>2017-01-25</t>
+  </si>
+  <si>
+    <t>German Morse Code</t>
+  </si>
+  <si>
+    <t>MorseCodeTranslated</t>
+  </si>
+  <si>
+    <t>./resources/modules/German Morse Code.pdf</t>
+  </si>
+  <si>
+    <t>German Password</t>
+  </si>
+  <si>
+    <t>PasswordsTranslated</t>
+  </si>
+  <si>
+    <t>./resources/modules/German Password.pdf</t>
+  </si>
+  <si>
+    <t>German Who's On First</t>
+  </si>
+  <si>
+    <t>WhosOnFirstTranslated</t>
+  </si>
+  <si>
+    <t>./resources/modules/German Who's On First.pdf</t>
   </si>
 </sst>
 </file>
@@ -1564,23 +1606,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC09710-E84E-49A6-94A5-EB5A61B7898A}">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="72" workbookViewId="0">
+      <selection activeCell="K91" sqref="K91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="1.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1599,8 +1642,11 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1619,8 +1665,11 @@
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1639,8 +1688,11 @@
       <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1659,8 +1711,11 @@
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1679,8 +1734,11 @@
       <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1699,8 +1757,11 @@
       <c r="F6" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1719,8 +1780,11 @@
       <c r="F7" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1739,8 +1803,11 @@
       <c r="F8" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1759,8 +1826,11 @@
       <c r="F9" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1779,8 +1849,11 @@
       <c r="F10" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1799,8 +1872,11 @@
       <c r="F11" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1819,8 +1895,11 @@
       <c r="F12" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1839,8 +1918,11 @@
       <c r="F13" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -1859,8 +1941,11 @@
       <c r="F14" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -1879,8 +1964,11 @@
       <c r="F15" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -1899,8 +1987,11 @@
       <c r="F16" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -1919,8 +2010,11 @@
       <c r="F17" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -1939,8 +2033,11 @@
       <c r="F18" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -1959,8 +2056,11 @@
       <c r="F19" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -1979,8 +2079,11 @@
       <c r="F20" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -1999,8 +2102,11 @@
       <c r="F21" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -2019,8 +2125,11 @@
       <c r="F22" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>86</v>
       </c>
@@ -2039,8 +2148,11 @@
       <c r="F23" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -2059,8 +2171,11 @@
       <c r="F24" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>90</v>
       </c>
@@ -2079,8 +2194,11 @@
       <c r="F25" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>96</v>
       </c>
@@ -2099,8 +2217,11 @@
       <c r="F26" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -2119,8 +2240,11 @@
       <c r="F27" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -2139,8 +2263,11 @@
       <c r="F28" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -2159,8 +2286,11 @@
       <c r="F29" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -2179,8 +2309,11 @@
       <c r="F30" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>116</v>
       </c>
@@ -2199,8 +2332,11 @@
       <c r="F31" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>120</v>
       </c>
@@ -2219,8 +2355,11 @@
       <c r="F32" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>123</v>
       </c>
@@ -2239,8 +2378,11 @@
       <c r="F33" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>127</v>
       </c>
@@ -2259,8 +2401,11 @@
       <c r="F34" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>132</v>
       </c>
@@ -2279,8 +2424,11 @@
       <c r="F35" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>136</v>
       </c>
@@ -2299,8 +2447,11 @@
       <c r="F36" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>195</v>
       </c>
@@ -2319,8 +2470,11 @@
       <c r="F37" s="1" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>199</v>
       </c>
@@ -2339,8 +2493,11 @@
       <c r="F38" s="1" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>200</v>
       </c>
@@ -2359,8 +2516,11 @@
       <c r="F39" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>211</v>
       </c>
@@ -2379,8 +2539,11 @@
       <c r="F40" s="1" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>141</v>
       </c>
@@ -2399,8 +2562,11 @@
       <c r="F41" s="1" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>196</v>
       </c>
@@ -2419,8 +2585,11 @@
       <c r="F42" s="1" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>220</v>
       </c>
@@ -2439,8 +2608,11 @@
       <c r="F43" s="1" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>265</v>
       </c>
@@ -2459,8 +2631,11 @@
       <c r="F44" s="1" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>221</v>
       </c>
@@ -2479,8 +2654,11 @@
       <c r="F45" s="1" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>222</v>
       </c>
@@ -2499,8 +2677,11 @@
       <c r="F46" s="1" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>223</v>
       </c>
@@ -2519,8 +2700,11 @@
       <c r="F47" s="1" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>224</v>
       </c>
@@ -2539,8 +2723,11 @@
       <c r="F48" s="1" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>225</v>
       </c>
@@ -2559,8 +2746,11 @@
       <c r="F49" s="1" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>217</v>
       </c>
@@ -2579,8 +2769,11 @@
       <c r="F50" s="1" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>201</v>
       </c>
@@ -2599,8 +2792,11 @@
       <c r="F51" s="1" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>212</v>
       </c>
@@ -2619,8 +2815,11 @@
       <c r="F52" s="1" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>213</v>
       </c>
@@ -2639,8 +2838,11 @@
       <c r="F53" s="1" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>226</v>
       </c>
@@ -2659,8 +2861,11 @@
       <c r="F54" s="1" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>227</v>
       </c>
@@ -2679,8 +2884,11 @@
       <c r="F55" s="1" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>228</v>
       </c>
@@ -2699,8 +2907,11 @@
       <c r="F56" s="1" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>202</v>
       </c>
@@ -2719,8 +2930,11 @@
       <c r="F57" s="1" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>203</v>
       </c>
@@ -2739,8 +2953,11 @@
       <c r="F58" s="1" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>214</v>
       </c>
@@ -2759,8 +2976,11 @@
       <c r="F59" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>229</v>
       </c>
@@ -2779,8 +2999,11 @@
       <c r="F60" s="1" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>204</v>
       </c>
@@ -2799,8 +3022,11 @@
       <c r="F61" s="1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>205</v>
       </c>
@@ -2819,8 +3045,11 @@
       <c r="F62" s="1" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>206</v>
       </c>
@@ -2839,8 +3068,11 @@
       <c r="F63" s="1" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>230</v>
       </c>
@@ -2859,8 +3091,11 @@
       <c r="F64" s="1" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>231</v>
       </c>
@@ -2879,8 +3114,11 @@
       <c r="F65" s="1" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>232</v>
       </c>
@@ -2899,8 +3137,11 @@
       <c r="F66" s="1" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>215</v>
       </c>
@@ -2919,8 +3160,11 @@
       <c r="F67" s="1" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>233</v>
       </c>
@@ -2939,8 +3183,11 @@
       <c r="F68" s="1" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>207</v>
       </c>
@@ -2959,8 +3206,11 @@
       <c r="F69" s="1" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>234</v>
       </c>
@@ -2979,8 +3229,11 @@
       <c r="F70" s="1" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>208</v>
       </c>
@@ -2999,8 +3252,11 @@
       <c r="F71" s="1" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>235</v>
       </c>
@@ -3019,8 +3275,11 @@
       <c r="F72" s="1" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>209</v>
       </c>
@@ -3039,8 +3298,11 @@
       <c r="F73" s="1" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>236</v>
       </c>
@@ -3059,8 +3321,11 @@
       <c r="F74" s="1" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>237</v>
       </c>
@@ -3079,8 +3344,11 @@
       <c r="F75" s="1" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>210</v>
       </c>
@@ -3099,8 +3367,11 @@
       <c r="F76" s="1" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>218</v>
       </c>
@@ -3119,8 +3390,11 @@
       <c r="F77" s="1" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>238</v>
       </c>
@@ -3139,8 +3413,11 @@
       <c r="F78" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>216</v>
       </c>
@@ -3159,8 +3436,11 @@
       <c r="F79" s="1" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>239</v>
       </c>
@@ -3179,8 +3459,11 @@
       <c r="F80" s="1" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>240</v>
       </c>
@@ -3199,8 +3482,11 @@
       <c r="F81" s="1" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>241</v>
       </c>
@@ -3219,8 +3505,11 @@
       <c r="F82" s="1" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>242</v>
       </c>
@@ -3239,8 +3528,11 @@
       <c r="F83" s="1" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>243</v>
       </c>
@@ -3259,8 +3551,11 @@
       <c r="F84" s="1" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>244</v>
       </c>
@@ -3279,8 +3574,11 @@
       <c r="F85" s="1" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>245</v>
       </c>
@@ -3299,8 +3597,11 @@
       <c r="F86" s="1" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>246</v>
       </c>
@@ -3319,8 +3620,11 @@
       <c r="F87" s="1" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>247</v>
       </c>
@@ -3339,8 +3643,11 @@
       <c r="F88" s="1" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>248</v>
       </c>
@@ -3359,8 +3666,11 @@
       <c r="F89" s="1" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>249</v>
       </c>
@@ -3379,8 +3689,11 @@
       <c r="F90" s="1" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>250</v>
       </c>
@@ -3399,8 +3712,11 @@
       <c r="F91" s="1" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>251</v>
       </c>
@@ -3419,8 +3735,11 @@
       <c r="F92" s="1" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>219</v>
       </c>
@@ -3439,8 +3758,11 @@
       <c r="F93" s="1" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>252</v>
       </c>
@@ -3458,6 +3780,101 @@
       </c>
       <c r="F94" s="1" t="s">
         <v>392</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>393</v>
+      </c>
+      <c r="B95" t="s">
+        <v>394</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95" t="s">
+        <v>395</v>
+      </c>
+      <c r="E95" t="s">
+        <v>396</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="G95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>398</v>
+      </c>
+      <c r="B96" t="s">
+        <v>399</v>
+      </c>
+      <c r="C96">
+        <v>2</v>
+      </c>
+      <c r="D96" t="s">
+        <v>400</v>
+      </c>
+      <c r="E96" t="s">
+        <v>396</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>401</v>
+      </c>
+      <c r="B97" t="s">
+        <v>402</v>
+      </c>
+      <c r="C97">
+        <v>2</v>
+      </c>
+      <c r="D97" t="s">
+        <v>403</v>
+      </c>
+      <c r="E97" t="s">
+        <v>396</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>404</v>
+      </c>
+      <c r="B98" t="s">
+        <v>405</v>
+      </c>
+      <c r="C98">
+        <v>2</v>
+      </c>
+      <c r="D98" t="s">
+        <v>406</v>
+      </c>
+      <c r="E98" t="s">
+        <v>396</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Can now export to .tex, very limited.
Former-commit-id: 4ecbf4c54021322f0a7e39ec91aa41bdf4e48b09
Former-commit-id: 555b9eb406aa88d24c9fcb341604c2dae6bb1899
</commit_message>
<xml_diff>
--- a/resources/modules-config-details-setup.xlsx
+++ b/resources/modules-config-details-setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\IdeaProjects\MakeMyManual\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55954212-7916-41E2-B2D8-6D41D2A95E97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBF696A-1D1E-473F-9E54-1E1E64D79FE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>ColourFlash</t>
   </si>
   <si>
-    <t>./resources/modules/Colour Flash.pdf</t>
-  </si>
-  <si>
     <t>Bashly</t>
   </si>
   <si>
@@ -56,27 +53,18 @@
     <t>PianoKeys</t>
   </si>
   <si>
-    <t>./resources/modules/Piano Keys.pdf</t>
-  </si>
-  <si>
     <t>2016-06-26</t>
   </si>
   <si>
     <t>Semaphore</t>
   </si>
   <si>
-    <t>./resources/modules/Semaphore.pdf</t>
-  </si>
-  <si>
     <t>2016-07-13</t>
   </si>
   <si>
     <t>Emoji Math</t>
   </si>
   <si>
-    <t>./resources/modules/Emoji Math.pdf</t>
-  </si>
-  <si>
     <t>Mock Army</t>
   </si>
   <si>
@@ -89,9 +77,6 @@
     <t>switchModule</t>
   </si>
   <si>
-    <t>./resources/modules/Switches.pdf</t>
-  </si>
-  <si>
     <t>Brian Fetter</t>
   </si>
   <si>
@@ -104,9 +89,6 @@
     <t>TwoBits</t>
   </si>
   <si>
-    <t>./resources/modules/Two Bits.pdf</t>
-  </si>
-  <si>
     <t>kaneb</t>
   </si>
   <si>
@@ -125,12 +107,6 @@
     <t>WordScrambleModule</t>
   </si>
   <si>
-    <t>./resources/modules/Anagrams.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Word Scramble.pdf</t>
-  </si>
-  <si>
     <t>2016-07-28</t>
   </si>
   <si>
@@ -140,9 +116,6 @@
     <t>combinationLock</t>
   </si>
   <si>
-    <t>./resources/modules/Combination Lock.pdf</t>
-  </si>
-  <si>
     <t>2016-08-03</t>
   </si>
   <si>
@@ -152,9 +125,6 @@
     <t>ButtonV2</t>
   </si>
   <si>
-    <t>./resources/modules/Square Button.pdf</t>
-  </si>
-  <si>
     <t>Hexicube</t>
   </si>
   <si>
@@ -167,24 +137,15 @@
     <t>SimonV2</t>
   </si>
   <si>
-    <t>./resources/modules/Simon States.pdf</t>
-  </si>
-  <si>
     <t>Round Keypad</t>
   </si>
   <si>
     <t>KeypadV2</t>
   </si>
   <si>
-    <t>./resources/modules/Round Keypad.pdf</t>
-  </si>
-  <si>
     <t>Listening</t>
   </si>
   <si>
-    <t>./resources/modules/Listening.pdf</t>
-  </si>
-  <si>
     <t>Perky</t>
   </si>
   <si>
@@ -194,18 +155,12 @@
     <t>ForeignExchangeRates</t>
   </si>
   <si>
-    <t>./resources/modules/Foreign Exchange Rates.pdf</t>
-  </si>
-  <si>
     <t>Orientation Cube</t>
   </si>
   <si>
     <t>OrientationCube</t>
   </si>
   <si>
-    <t>./resources/modules/Orientation Cube.pdf</t>
-  </si>
-  <si>
     <t>2016-08-14</t>
   </si>
   <si>
@@ -215,18 +170,12 @@
     <t>MorseV2</t>
   </si>
   <si>
-    <t>./resources/modules/Morsematics.pdf</t>
-  </si>
-  <si>
     <t>Connection Check</t>
   </si>
   <si>
     <t>graphModule</t>
   </si>
   <si>
-    <t>./resources/modules/Connection Check.pdf</t>
-  </si>
-  <si>
     <t>clutterArranger</t>
   </si>
   <si>
@@ -236,9 +185,6 @@
     <t>LetterKeys</t>
   </si>
   <si>
-    <t>./resources/modules/Letter Keys.pdf</t>
-  </si>
-  <si>
     <t>Mage of R. Jelly</t>
   </si>
   <si>
@@ -251,18 +197,12 @@
     <t>MemoryV2</t>
   </si>
   <si>
-    <t>./resources/modules/Forget Me Not.pdf</t>
-  </si>
-  <si>
     <t>Astrology</t>
   </si>
   <si>
     <t>spwizAstrology</t>
   </si>
   <si>
-    <t>./resources/modules/Astrology.pdf</t>
-  </si>
-  <si>
     <t>Spare Wizard</t>
   </si>
   <si>
@@ -272,9 +212,6 @@
     <t>Logic</t>
   </si>
   <si>
-    <t>./resources/modules/Logic.pdf</t>
-  </si>
-  <si>
     <t>SL7205</t>
   </si>
   <si>
@@ -287,9 +224,6 @@
     <t>CrazyTalk</t>
   </si>
   <si>
-    <t>./resources/modules/Crazy Talk.pdf</t>
-  </si>
-  <si>
     <t>2016-08-19</t>
   </si>
   <si>
@@ -299,9 +233,6 @@
     <t>spwizAdventureGame</t>
   </si>
   <si>
-    <t>./resources/modules/Adventure Game.pdf</t>
-  </si>
-  <si>
     <t>Turn The Key</t>
   </si>
   <si>
@@ -314,12 +245,6 @@
     <t>TurnTheKeyAdvanced</t>
   </si>
   <si>
-    <t>./resources/modules/Turn The Key.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Turn The Keys.pdf</t>
-  </si>
-  <si>
     <t>2016-08-20</t>
   </si>
   <si>
@@ -329,9 +254,6 @@
     <t>MysticSquareModule</t>
   </si>
   <si>
-    <t>./resources/modules/Mystic Square.pdf</t>
-  </si>
-  <si>
     <t>Konqi</t>
   </si>
   <si>
@@ -341,9 +263,6 @@
     <t>MazeV2</t>
   </si>
   <si>
-    <t>./resources/modules/Plumbing.pdf</t>
-  </si>
-  <si>
     <t>2016-08-21</t>
   </si>
   <si>
@@ -353,9 +272,6 @@
     <t>PasswordV2</t>
   </si>
   <si>
-    <t>./resources/modules/Safety Safe.pdf</t>
-  </si>
-  <si>
     <t>2016-08-22</t>
   </si>
   <si>
@@ -365,9 +281,6 @@
     <t>CryptModule</t>
   </si>
   <si>
-    <t>./resources/modules/Cryptography.pdf</t>
-  </si>
-  <si>
     <t>2016-08-24</t>
   </si>
   <si>
@@ -377,9 +290,6 @@
     <t>ChessModule</t>
   </si>
   <si>
-    <t>./resources/modules/Chess.pdf</t>
-  </si>
-  <si>
     <t>MoMo, Flamanis</t>
   </si>
   <si>
@@ -389,9 +299,6 @@
     <t>MouseInTheMaze</t>
   </si>
   <si>
-    <t>./resources/modules/Mouse In The Maze.pdf</t>
-  </si>
-  <si>
     <t>2016-08-26</t>
   </si>
   <si>
@@ -401,18 +308,12 @@
     <t>spwiz3DMaze</t>
   </si>
   <si>
-    <t>./resources/modules/3D Maze.pdf</t>
-  </si>
-  <si>
     <t>Silly Slots</t>
   </si>
   <si>
     <t>SillySlots</t>
   </si>
   <si>
-    <t>./resources/modules/Silly Slots.pdf</t>
-  </si>
-  <si>
     <t>2016-08-29</t>
   </si>
   <si>
@@ -422,9 +323,6 @@
     <t>NumberPad</t>
   </si>
   <si>
-    <t>./resources/modules/Number Pad.pdf</t>
-  </si>
-  <si>
     <t>mitterdoo</t>
   </si>
   <si>
@@ -434,9 +332,6 @@
     <t>Laundry</t>
   </si>
   <si>
-    <t>./resources/modules/Laundry.pdf</t>
-  </si>
-  <si>
     <t>Hendruid, AcrylicStain, Flamanis</t>
   </si>
   <si>
@@ -626,12 +521,6 @@
     <t>Murder</t>
   </si>
   <si>
-    <t>./resources/modules/Resistors.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Probing.pdf</t>
-  </si>
-  <si>
     <t>Skewed Slots</t>
   </si>
   <si>
@@ -782,478 +671,589 @@
     <t>Binary LEDs</t>
   </si>
   <si>
+    <t>Point Of Order</t>
+  </si>
+  <si>
+    <t>Ice Cream</t>
+  </si>
+  <si>
+    <t>Yahtzee</t>
+  </si>
+  <si>
+    <t>Tic-Tac-Toe</t>
+  </si>
+  <si>
+    <t>2016-09-02</t>
+  </si>
+  <si>
+    <t>Onyxite</t>
+  </si>
+  <si>
+    <t>2016-09-12</t>
+  </si>
+  <si>
+    <t>samfun123</t>
+  </si>
+  <si>
+    <t>2016-09-15</t>
+  </si>
+  <si>
+    <t>Eluminate</t>
+  </si>
+  <si>
+    <t>2016-09-18</t>
+  </si>
+  <si>
+    <t>2016-09-24</t>
+  </si>
+  <si>
+    <t>Flush</t>
+  </si>
+  <si>
+    <t>Asimir</t>
+  </si>
+  <si>
+    <t>2016-09-26</t>
+  </si>
+  <si>
+    <t>theFIZZYnator, samfun123</t>
+  </si>
+  <si>
+    <t>2016-10-06</t>
+  </si>
+  <si>
+    <t>Moon, Timwi</t>
+  </si>
+  <si>
+    <t>2016-10-07</t>
+  </si>
+  <si>
+    <t>2016-10-08</t>
+  </si>
+  <si>
+    <t>2016-10-10</t>
+  </si>
+  <si>
+    <t>TheAuthorOfOZ, Timwi</t>
+  </si>
+  <si>
+    <t>2016-10-18</t>
+  </si>
+  <si>
+    <t>Timwi</t>
+  </si>
+  <si>
+    <t>2016-10-24</t>
+  </si>
+  <si>
+    <t>2016-10-28</t>
+  </si>
+  <si>
+    <t>2016-10-30</t>
+  </si>
+  <si>
+    <t>2016-11-03</t>
+  </si>
+  <si>
+    <t>2016-11-06</t>
+  </si>
+  <si>
+    <t>theFIZZYnator, Lupo511</t>
+  </si>
+  <si>
+    <t>2016-11-12</t>
+  </si>
+  <si>
+    <t>2016-11-21</t>
+  </si>
+  <si>
+    <t>Timwi, Lumbud84</t>
+  </si>
+  <si>
+    <t>2016-11-23</t>
+  </si>
+  <si>
+    <t>2016-11-24</t>
+  </si>
+  <si>
+    <t>Lumbud84, Timwi</t>
+  </si>
+  <si>
+    <t>2016-11-25</t>
+  </si>
+  <si>
+    <t>2016-11-27</t>
+  </si>
+  <si>
+    <t>Timwi, Andrio Celos</t>
+  </si>
+  <si>
+    <t>2016-12-02</t>
+  </si>
+  <si>
+    <t>2016-12-07</t>
+  </si>
+  <si>
+    <t>2016-12-12</t>
+  </si>
+  <si>
+    <t>2016-12-20</t>
+  </si>
+  <si>
+    <t>catnip, Flamanis</t>
+  </si>
+  <si>
+    <t>2016-12-24</t>
+  </si>
+  <si>
+    <t>ZekNikZ</t>
+  </si>
+  <si>
+    <t>2016-12-31</t>
+  </si>
+  <si>
+    <t>2017-01-03</t>
+  </si>
+  <si>
+    <t>2017-01-05</t>
+  </si>
+  <si>
+    <t>2017-01-06</t>
+  </si>
+  <si>
+    <t>2017-01-15</t>
+  </si>
+  <si>
+    <t>2017-01-16</t>
+  </si>
+  <si>
+    <t>2017-01-20</t>
+  </si>
+  <si>
+    <t>Rexkix, Timwi</t>
+  </si>
+  <si>
+    <t>2017-01-23</t>
+  </si>
+  <si>
+    <t>Riverbui, Trainzack</t>
+  </si>
+  <si>
+    <t>2017-03-05</t>
+  </si>
+  <si>
+    <t>2017-03-17</t>
+  </si>
+  <si>
+    <t>Nanthelas, SL7205</t>
+  </si>
+  <si>
+    <t>2017-03-23</t>
+  </si>
+  <si>
+    <t>theFIZZYnator, SL7205</t>
+  </si>
+  <si>
+    <t>2017-04-03</t>
+  </si>
+  <si>
+    <t>2017-04-07</t>
+  </si>
+  <si>
+    <t>Grybo, samfun123</t>
+  </si>
+  <si>
+    <t>2017-04-17</t>
+  </si>
+  <si>
+    <t>Timwi, Freelancer1025</t>
+  </si>
+  <si>
+    <t>2017-04-30</t>
+  </si>
+  <si>
+    <t>2017-05-10</t>
+  </si>
+  <si>
+    <t>2017-05-11</t>
+  </si>
+  <si>
+    <t>Virepri</t>
+  </si>
+  <si>
+    <t>2017-05-12</t>
+  </si>
+  <si>
+    <t>2017-05-14</t>
+  </si>
+  <si>
+    <t>LeGeND, SL7205</t>
+  </si>
+  <si>
+    <t>2017-05-25</t>
+  </si>
+  <si>
+    <t>2017-06-12</t>
+  </si>
+  <si>
+    <t>2017-06-13</t>
+  </si>
+  <si>
+    <t>Willowyn</t>
+  </si>
+  <si>
+    <t>2017-06-25</t>
+  </si>
+  <si>
+    <t>2017-06-18</t>
+  </si>
+  <si>
+    <t>2017-06-22</t>
+  </si>
+  <si>
+    <t>SKIPP, LeGeND, ZekNikZ</t>
+  </si>
+  <si>
+    <t>2017-06-26</t>
+  </si>
+  <si>
+    <t>Ezekiel, SL7205</t>
+  </si>
+  <si>
+    <t>2017-07-01</t>
+  </si>
+  <si>
+    <t>Timwi, Rexkix</t>
+  </si>
+  <si>
+    <t>2017-07-02</t>
+  </si>
+  <si>
+    <t>German Button</t>
+  </si>
+  <si>
+    <t>BigButtonTranslated</t>
+  </si>
+  <si>
+    <t>Malde, Tharagon</t>
+  </si>
+  <si>
+    <t>2017-01-25</t>
+  </si>
+  <si>
+    <t>German Morse Code</t>
+  </si>
+  <si>
+    <t>MorseCodeTranslated</t>
+  </si>
+  <si>
+    <t>German Password</t>
+  </si>
+  <si>
+    <t>PasswordsTranslated</t>
+  </si>
+  <si>
+    <t>German Who's On First</t>
+  </si>
+  <si>
+    <t>WhosOnFirstTranslated</t>
+  </si>
+  <si>
+    <t>modules/Colour Flash.pdf</t>
+  </si>
+  <si>
+    <t>modules/Piano Keys.pdf</t>
+  </si>
+  <si>
+    <t>modules/Semaphore.pdf</t>
+  </si>
+  <si>
+    <t>modules/Emoji Math.pdf</t>
+  </si>
+  <si>
+    <t>modules/Switches.pdf</t>
+  </si>
+  <si>
+    <t>modules/Two Bits.pdf</t>
+  </si>
+  <si>
+    <t>modules/Anagrams.pdf</t>
+  </si>
+  <si>
+    <t>modules/Word Scramble.pdf</t>
+  </si>
+  <si>
+    <t>modules/Combination Lock.pdf</t>
+  </si>
+  <si>
+    <t>modules/Square Button.pdf</t>
+  </si>
+  <si>
+    <t>modules/Simon States.pdf</t>
+  </si>
+  <si>
+    <t>modules/Round Keypad.pdf</t>
+  </si>
+  <si>
+    <t>modules/Listening.pdf</t>
+  </si>
+  <si>
+    <t>modules/Foreign Exchange Rates.pdf</t>
+  </si>
+  <si>
+    <t>modules/Orientation Cube.pdf</t>
+  </si>
+  <si>
+    <t>modules/Morsematics.pdf</t>
+  </si>
+  <si>
+    <t>modules/Connection Check.pdf</t>
+  </si>
+  <si>
+    <t>modules/Letter Keys.pdf</t>
+  </si>
+  <si>
+    <t>modules/Forget Me Not.pdf</t>
+  </si>
+  <si>
+    <t>modules/Astrology.pdf</t>
+  </si>
+  <si>
+    <t>modules/Logic.pdf</t>
+  </si>
+  <si>
+    <t>modules/Crazy Talk.pdf</t>
+  </si>
+  <si>
+    <t>modules/Adventure Game.pdf</t>
+  </si>
+  <si>
+    <t>modules/Turn The Key.pdf</t>
+  </si>
+  <si>
+    <t>modules/Turn The Keys.pdf</t>
+  </si>
+  <si>
+    <t>modules/Mystic Square.pdf</t>
+  </si>
+  <si>
+    <t>modules/Plumbing.pdf</t>
+  </si>
+  <si>
+    <t>modules/Safety Safe.pdf</t>
+  </si>
+  <si>
+    <t>modules/Cryptography.pdf</t>
+  </si>
+  <si>
+    <t>modules/Chess.pdf</t>
+  </si>
+  <si>
+    <t>modules/Mouse In The Maze.pdf</t>
+  </si>
+  <si>
+    <t>modules/3D Maze.pdf</t>
+  </si>
+  <si>
+    <t>modules/Silly Slots.pdf</t>
+  </si>
+  <si>
+    <t>modules/Number Pad.pdf</t>
+  </si>
+  <si>
+    <t>modules/Laundry.pdf</t>
+  </si>
+  <si>
+    <t>modules/Probing.pdf</t>
+  </si>
+  <si>
+    <t>modules/Resistors.pdf</t>
+  </si>
+  <si>
+    <t>modules/Skewed Slots.pdf</t>
+  </si>
+  <si>
+    <t>modules/Caesar Cipher.pdf</t>
+  </si>
+  <si>
+    <t>modules/Perspective Pegs.pdf</t>
+  </si>
+  <si>
+    <t>modules/Microcontroller.pdf</t>
+  </si>
+  <si>
+    <t>modules/Murder.pdf</t>
+  </si>
+  <si>
+    <t>modules/Tic-Tac-Toe.pdf</t>
+  </si>
+  <si>
+    <t>modules/Shape Shift.pdf</t>
+  </si>
+  <si>
+    <t>modules/Follow The Leader.pdf</t>
+  </si>
+  <si>
+    <t>modules/Friendship.pdf</t>
+  </si>
+  <si>
+    <t>modules/The Bulb.pdf</t>
+  </si>
+  <si>
+    <t>modules/Alphabet.pdf</t>
+  </si>
+  <si>
+    <t>modules/Blind Alley.pdf</t>
+  </si>
+  <si>
+    <t>modules/Sea Shells.pdf</t>
+  </si>
+  <si>
+    <t>modules/English Test.pdf</t>
+  </si>
+  <si>
+    <t>modules/Rock-Paper-Scissors-Lizard-Spock.pdf</t>
+  </si>
+  <si>
+    <t>modules/Hexamaze.pdf</t>
+  </si>
+  <si>
+    <t>modules/Bitmaps.pdf</t>
+  </si>
+  <si>
+    <t>modules/Colored Squares.pdf</t>
+  </si>
+  <si>
+    <t>modules/Adjacent Letters.pdf</t>
+  </si>
+  <si>
+    <t>modules/Third Base.pdf</t>
+  </si>
+  <si>
+    <t>modules/Souvenir.pdf</t>
+  </si>
+  <si>
+    <t>modules/Word Search.pdf</t>
+  </si>
+  <si>
+    <t>modules/Broken Buttons.pdf</t>
+  </si>
+  <si>
+    <t>modules/Simon Screams.pdf</t>
+  </si>
+  <si>
+    <t>modules/Modules Against Humanity.pdf</t>
+  </si>
+  <si>
+    <t>modules/Complicated Buttons.pdf</t>
+  </si>
+  <si>
+    <t>modules/Battleship.pdf</t>
+  </si>
+  <si>
+    <t>modules/Text Field.pdf</t>
+  </si>
+  <si>
+    <t>modules/Symbolic Password.pdf</t>
+  </si>
+  <si>
+    <t>modules/Wire Placement.pdf</t>
+  </si>
+  <si>
+    <t>modules/Double-Oh.pdf</t>
+  </si>
+  <si>
+    <t>modules/Cheap Checkout.pdf</t>
+  </si>
+  <si>
+    <t>modules/Coordinates.pdf</t>
+  </si>
+  <si>
+    <t>modules/Light Cycle.pdf</t>
+  </si>
+  <si>
+    <t>modules/Rhythms.pdf</t>
+  </si>
+  <si>
+    <t>modules/Color Math.pdf</t>
+  </si>
+  <si>
+    <t>modules/Only Connect.pdf</t>
+  </si>
+  <si>
+    <t>modules/Neutralization.pdf</t>
+  </si>
+  <si>
+    <t>modules/Web Design.pdf</t>
+  </si>
+  <si>
+    <t>modules/Chord Qualities.pdf</t>
+  </si>
+  <si>
+    <t>modules/Creation.pdf</t>
+  </si>
+  <si>
+    <t>modules/Rubik's Cube.pdf</t>
+  </si>
+  <si>
+    <t>modules/FizzBuzz.pdf</t>
+  </si>
+  <si>
+    <t>modules/The Clock.pdf</t>
+  </si>
+  <si>
+    <t>modules/LED Encryption.pdf</t>
+  </si>
+  <si>
+    <t>modules/Bitwise Operations.pdf</t>
+  </si>
+  <si>
+    <t>modules/Fast Math.pdf</t>
+  </si>
+  <si>
+    <t>modules/Minesweeper.pdf</t>
+  </si>
+  <si>
+    <t>modules/Zoo.pdf</t>
+  </si>
+  <si>
+    <t>modules/Binary LEDs.pdf</t>
+  </si>
+  <si>
+    <t>modules/Point Of Order.pdf</t>
+  </si>
+  <si>
+    <t>modules/Ice Cream.pdf</t>
+  </si>
+  <si>
+    <t>modules/The Screw.pdf</t>
+  </si>
+  <si>
+    <t>modules/Yahtzee.pdf</t>
+  </si>
+  <si>
+    <t>modules/German Button.pdf</t>
+  </si>
+  <si>
+    <t>modules/German Morse Code.pdf</t>
+  </si>
+  <si>
+    <t>modules/German Password.pdf</t>
+  </si>
+  <si>
+    <t>modules/German Who's On First.pdf</t>
+  </si>
+  <si>
     <t>Boolean Venn Diagrams</t>
   </si>
   <si>
-    <t>Point Of Order</t>
-  </si>
-  <si>
-    <t>Ice Cream</t>
-  </si>
-  <si>
-    <t>Yahtzee</t>
-  </si>
-  <si>
-    <t>./resources/modules/Skewed Slots.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Gamepad.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Follow The Leader.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Friendship.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Caesar Cipher.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Perspective Pegs.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Monsplode, Fight!.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Shape Shift.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Alphabet.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Microcontroller.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Murder.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Tic-Tac-Toe.pdf</t>
-  </si>
-  <si>
-    <t>Tic-Tac-Toe</t>
-  </si>
-  <si>
-    <t>./resources/modules/The Bulb.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Sea Shells.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/English Test.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Rock-Paper-Scissors-Lizard-Spock.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Hexamaze.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Bitmaps.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Third Base.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Souvenir.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Battleship.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Text Field.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Coordinates.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Rhythms.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Color Math.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Neutralization.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Blind Alley.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Colored Squares.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Adjacent Letters.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Word Search.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Broken Buttons.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Simon Screams.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Wire Placement.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Cheap Checkout.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Light Cycle.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Only Connect.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Symbolic Password.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Double-Oh.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Web Design.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Chord Qualities.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Creation.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Rubik's Cube.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/FizzBuzz.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/LED Encryption.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Bitwise Operations.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Fast Math.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Minesweeper.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Modules Against Humanity.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Complicated Buttons.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Zoo.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Binary LEDs.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Boolean Venn Diagrams.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Point Of Order.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Ice Cream.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/Yahtzee.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/The Clock.pdf</t>
-  </si>
-  <si>
-    <t>./resources/modules/The Screw.pdf</t>
-  </si>
-  <si>
-    <t>2016-09-02</t>
-  </si>
-  <si>
-    <t>Onyxite</t>
-  </si>
-  <si>
-    <t>2016-09-12</t>
-  </si>
-  <si>
-    <t>samfun123</t>
-  </si>
-  <si>
-    <t>2016-09-15</t>
-  </si>
-  <si>
-    <t>Eluminate</t>
-  </si>
-  <si>
-    <t>2016-09-18</t>
-  </si>
-  <si>
-    <t>2016-09-24</t>
-  </si>
-  <si>
-    <t>Flush</t>
-  </si>
-  <si>
-    <t>Asimir</t>
-  </si>
-  <si>
-    <t>2016-09-26</t>
-  </si>
-  <si>
-    <t>theFIZZYnator, samfun123</t>
-  </si>
-  <si>
-    <t>2016-10-06</t>
-  </si>
-  <si>
-    <t>Moon, Timwi</t>
-  </si>
-  <si>
-    <t>2016-10-07</t>
-  </si>
-  <si>
-    <t>2016-10-08</t>
-  </si>
-  <si>
-    <t>2016-10-10</t>
-  </si>
-  <si>
-    <t>TheAuthorOfOZ, Timwi</t>
-  </si>
-  <si>
-    <t>2016-10-18</t>
-  </si>
-  <si>
-    <t>Timwi</t>
-  </si>
-  <si>
-    <t>2016-10-24</t>
-  </si>
-  <si>
-    <t>2016-10-28</t>
-  </si>
-  <si>
-    <t>2016-10-30</t>
-  </si>
-  <si>
-    <t>2016-11-03</t>
-  </si>
-  <si>
-    <t>2016-11-06</t>
-  </si>
-  <si>
-    <t>theFIZZYnator, Lupo511</t>
-  </si>
-  <si>
-    <t>2016-11-12</t>
-  </si>
-  <si>
-    <t>2016-11-21</t>
-  </si>
-  <si>
-    <t>Timwi, Lumbud84</t>
-  </si>
-  <si>
-    <t>2016-11-23</t>
-  </si>
-  <si>
-    <t>2016-11-24</t>
-  </si>
-  <si>
-    <t>Lumbud84, Timwi</t>
-  </si>
-  <si>
-    <t>2016-11-25</t>
-  </si>
-  <si>
-    <t>2016-11-27</t>
-  </si>
-  <si>
-    <t>Timwi, Andrio Celos</t>
-  </si>
-  <si>
-    <t>2016-12-02</t>
-  </si>
-  <si>
-    <t>2016-12-07</t>
-  </si>
-  <si>
-    <t>2016-12-12</t>
-  </si>
-  <si>
-    <t>2016-12-20</t>
-  </si>
-  <si>
-    <t>catnip, Flamanis</t>
-  </si>
-  <si>
-    <t>2016-12-24</t>
-  </si>
-  <si>
-    <t>ZekNikZ</t>
-  </si>
-  <si>
-    <t>2016-12-31</t>
-  </si>
-  <si>
-    <t>2017-01-03</t>
-  </si>
-  <si>
-    <t>2017-01-05</t>
-  </si>
-  <si>
-    <t>2017-01-06</t>
-  </si>
-  <si>
-    <t>2017-01-15</t>
-  </si>
-  <si>
-    <t>2017-01-16</t>
-  </si>
-  <si>
-    <t>2017-01-20</t>
-  </si>
-  <si>
-    <t>Rexkix, Timwi</t>
-  </si>
-  <si>
-    <t>2017-01-23</t>
-  </si>
-  <si>
-    <t>Riverbui, Trainzack</t>
-  </si>
-  <si>
-    <t>2017-03-05</t>
-  </si>
-  <si>
-    <t>2017-03-17</t>
-  </si>
-  <si>
-    <t>Nanthelas, SL7205</t>
-  </si>
-  <si>
-    <t>2017-03-23</t>
-  </si>
-  <si>
-    <t>theFIZZYnator, SL7205</t>
-  </si>
-  <si>
-    <t>2017-04-03</t>
-  </si>
-  <si>
-    <t>2017-04-07</t>
-  </si>
-  <si>
-    <t>Grybo, samfun123</t>
-  </si>
-  <si>
-    <t>2017-04-17</t>
-  </si>
-  <si>
-    <t>Timwi, Freelancer1025</t>
-  </si>
-  <si>
-    <t>2017-04-30</t>
-  </si>
-  <si>
-    <t>2017-05-10</t>
-  </si>
-  <si>
-    <t>2017-05-11</t>
-  </si>
-  <si>
-    <t>Virepri</t>
-  </si>
-  <si>
-    <t>2017-05-12</t>
-  </si>
-  <si>
-    <t>2017-05-14</t>
-  </si>
-  <si>
-    <t>LeGeND, SL7205</t>
-  </si>
-  <si>
-    <t>2017-05-25</t>
-  </si>
-  <si>
-    <t>2017-06-12</t>
-  </si>
-  <si>
-    <t>2017-06-13</t>
-  </si>
-  <si>
-    <t>Willowyn</t>
-  </si>
-  <si>
-    <t>2017-06-25</t>
-  </si>
-  <si>
-    <t>2017-06-18</t>
-  </si>
-  <si>
-    <t>2017-06-22</t>
-  </si>
-  <si>
-    <t>SKIPP, LeGeND, ZekNikZ</t>
-  </si>
-  <si>
-    <t>2017-06-26</t>
-  </si>
-  <si>
-    <t>Ezekiel, SL7205</t>
-  </si>
-  <si>
-    <t>2017-07-01</t>
-  </si>
-  <si>
-    <t>Timwi, Rexkix</t>
-  </si>
-  <si>
-    <t>2017-07-02</t>
-  </si>
-  <si>
-    <t>German Button</t>
-  </si>
-  <si>
-    <t>BigButtonTranslated</t>
-  </si>
-  <si>
-    <t>./resources/modules/German Button.pdf</t>
-  </si>
-  <si>
-    <t>Malde, Tharagon</t>
-  </si>
-  <si>
-    <t>2017-01-25</t>
-  </si>
-  <si>
-    <t>German Morse Code</t>
-  </si>
-  <si>
-    <t>MorseCodeTranslated</t>
-  </si>
-  <si>
-    <t>./resources/modules/German Morse Code.pdf</t>
-  </si>
-  <si>
-    <t>German Password</t>
-  </si>
-  <si>
-    <t>PasswordsTranslated</t>
-  </si>
-  <si>
-    <t>./resources/modules/German Password.pdf</t>
-  </si>
-  <si>
-    <t>German Who's On First</t>
-  </si>
-  <si>
-    <t>WhosOnFirstTranslated</t>
-  </si>
-  <si>
-    <t>./resources/modules/German Who's On First.pdf</t>
+    <t>modules/Boolean Venn Diagram.pdf</t>
+  </si>
+  <si>
+    <t>modules/The Gamepad.pdf</t>
+  </si>
+  <si>
+    <t>modules/Monsplode Fight.pdf</t>
   </si>
 </sst>
 </file>
@@ -1608,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC09710-E84E-49A6-94A5-EB5A61B7898A}">
   <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="72" workbookViewId="0">
-      <selection activeCell="K91" sqref="K91"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="72" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1634,13 +1634,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="G1">
         <v>1</v>
@@ -1648,22 +1648,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>309</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1671,22 +1671,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>310</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -1694,22 +1694,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>311</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1717,22 +1717,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>312</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1740,22 +1740,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>313</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -1763,22 +1763,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>314</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1786,22 +1786,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>315</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -1809,22 +1809,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>316</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1832,22 +1832,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>317</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1855,22 +1855,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>318</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1878,22 +1878,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>319</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1901,22 +1901,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>320</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1924,22 +1924,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>321</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -1947,22 +1947,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>322</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1970,22 +1970,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>323</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1993,22 +1993,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
+        <v>324</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -2016,22 +2016,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>325</v>
       </c>
       <c r="E18" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -2039,22 +2039,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
+        <v>326</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -2062,22 +2062,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="C20">
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>327</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -2085,22 +2085,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>328</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -2108,22 +2108,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>329</v>
       </c>
       <c r="E22" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -2131,22 +2131,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="C23">
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
+        <v>330</v>
       </c>
       <c r="E23" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -2154,22 +2154,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>93</v>
+        <v>331</v>
       </c>
       <c r="E24" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -2177,22 +2177,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="C25">
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>94</v>
+        <v>332</v>
       </c>
       <c r="E25" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -2200,22 +2200,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="C26">
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>98</v>
+        <v>333</v>
       </c>
       <c r="E26" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -2223,22 +2223,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>102</v>
+        <v>334</v>
       </c>
       <c r="E27" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -2246,22 +2246,22 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="C28">
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>106</v>
+        <v>335</v>
       </c>
       <c r="E28" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -2269,22 +2269,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="C29">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>110</v>
+        <v>336</v>
       </c>
       <c r="E29" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -2292,22 +2292,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="C30">
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>114</v>
+        <v>337</v>
       </c>
       <c r="E30" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -2315,22 +2315,22 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="C31">
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>118</v>
+        <v>338</v>
       </c>
       <c r="E31" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -2338,22 +2338,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="B32" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="C32">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>122</v>
+        <v>339</v>
       </c>
       <c r="E32" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -2361,22 +2361,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="B33" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="C33">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>125</v>
+        <v>340</v>
       </c>
       <c r="E33" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -2384,22 +2384,22 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="B34" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
       <c r="C34">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>129</v>
+        <v>341</v>
       </c>
       <c r="E34" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -2407,22 +2407,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
       <c r="B35" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
       <c r="C35">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>133</v>
+        <v>342</v>
       </c>
       <c r="E35" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -2430,22 +2430,22 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
       <c r="B36" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
       <c r="C36">
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>198</v>
+        <v>343</v>
       </c>
       <c r="E36" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>311</v>
+        <v>216</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -2453,22 +2453,22 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>195</v>
+        <v>160</v>
       </c>
       <c r="B37" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="C37">
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>197</v>
+        <v>344</v>
       </c>
       <c r="E37" t="s">
-        <v>312</v>
+        <v>217</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>313</v>
+        <v>218</v>
       </c>
       <c r="G37">
         <v>1</v>
@@ -2476,22 +2476,22 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="B38" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="C38">
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>253</v>
+        <v>345</v>
       </c>
       <c r="E38" t="s">
-        <v>314</v>
+        <v>219</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>315</v>
+        <v>220</v>
       </c>
       <c r="G38">
         <v>1</v>
@@ -2499,22 +2499,22 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>200</v>
+        <v>163</v>
       </c>
       <c r="B39" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>257</v>
+        <v>346</v>
       </c>
       <c r="E39" t="s">
-        <v>316</v>
+        <v>221</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>317</v>
+        <v>222</v>
       </c>
       <c r="G39">
         <v>1</v>
@@ -2522,22 +2522,22 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>211</v>
+        <v>174</v>
       </c>
       <c r="B40" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="C40">
         <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>258</v>
+        <v>347</v>
       </c>
       <c r="E40" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>318</v>
+        <v>223</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -2545,22 +2545,22 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="B41" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="C41">
         <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>262</v>
+        <v>348</v>
       </c>
       <c r="E41" t="s">
-        <v>319</v>
+        <v>224</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>318</v>
+        <v>223</v>
       </c>
       <c r="G41">
         <v>1</v>
@@ -2568,22 +2568,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>196</v>
+        <v>161</v>
       </c>
       <c r="B42" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="C42">
         <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>263</v>
+        <v>349</v>
       </c>
       <c r="E42" t="s">
-        <v>320</v>
+        <v>225</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>321</v>
+        <v>226</v>
       </c>
       <c r="G42">
         <v>1</v>
@@ -2591,22 +2591,22 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>220</v>
+        <v>183</v>
       </c>
       <c r="B43" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="C43">
         <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>254</v>
+        <v>405</v>
       </c>
       <c r="E43" t="s">
-        <v>322</v>
+        <v>227</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>323</v>
+        <v>228</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -2614,22 +2614,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>265</v>
+        <v>215</v>
       </c>
       <c r="B44" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="C44">
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>264</v>
+        <v>350</v>
       </c>
       <c r="E44" t="s">
-        <v>324</v>
+        <v>229</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>325</v>
+        <v>230</v>
       </c>
       <c r="G44">
         <v>1</v>
@@ -2637,22 +2637,22 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>221</v>
+        <v>184</v>
       </c>
       <c r="B45" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="C45">
         <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>259</v>
+        <v>406</v>
       </c>
       <c r="E45" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>326</v>
+        <v>231</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -2660,22 +2660,22 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>222</v>
+        <v>185</v>
       </c>
       <c r="B46" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
       <c r="C46">
         <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>260</v>
+        <v>351</v>
       </c>
       <c r="E46" t="s">
-        <v>320</v>
+        <v>225</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>327</v>
+        <v>232</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -2683,22 +2683,22 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>223</v>
+        <v>186</v>
       </c>
       <c r="B47" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="C47">
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>255</v>
+        <v>352</v>
       </c>
       <c r="E47" t="s">
-        <v>328</v>
+        <v>233</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>329</v>
+        <v>234</v>
       </c>
       <c r="G47">
         <v>1</v>
@@ -2706,22 +2706,22 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>224</v>
+        <v>187</v>
       </c>
       <c r="B48" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="C48">
         <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>256</v>
+        <v>353</v>
       </c>
       <c r="E48" t="s">
-        <v>330</v>
+        <v>235</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>331</v>
+        <v>236</v>
       </c>
       <c r="G48">
         <v>1</v>
@@ -2729,22 +2729,22 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>225</v>
+        <v>188</v>
       </c>
       <c r="B49" t="s">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="C49">
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>266</v>
+        <v>354</v>
       </c>
       <c r="E49" t="s">
-        <v>330</v>
+        <v>235</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>332</v>
+        <v>237</v>
       </c>
       <c r="G49">
         <v>1</v>
@@ -2752,22 +2752,22 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>217</v>
+        <v>180</v>
       </c>
       <c r="B50" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>261</v>
+        <v>355</v>
       </c>
       <c r="E50" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>333</v>
+        <v>238</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -2775,22 +2775,22 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>201</v>
+        <v>164</v>
       </c>
       <c r="B51" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="C51">
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>280</v>
+        <v>356</v>
       </c>
       <c r="E51" t="s">
-        <v>330</v>
+        <v>235</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>334</v>
+        <v>239</v>
       </c>
       <c r="G51">
         <v>1</v>
@@ -2798,22 +2798,22 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>212</v>
+        <v>175</v>
       </c>
       <c r="B52" t="s">
-        <v>152</v>
+        <v>117</v>
       </c>
       <c r="C52">
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>267</v>
+        <v>357</v>
       </c>
       <c r="E52" t="s">
-        <v>320</v>
+        <v>225</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>335</v>
+        <v>240</v>
       </c>
       <c r="G52">
         <v>1</v>
@@ -2821,22 +2821,22 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>213</v>
+        <v>176</v>
       </c>
       <c r="B53" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>268</v>
+        <v>358</v>
       </c>
       <c r="E53" t="s">
-        <v>336</v>
+        <v>241</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>335</v>
+        <v>240</v>
       </c>
       <c r="G53">
         <v>1</v>
@@ -2844,22 +2844,22 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>226</v>
+        <v>189</v>
       </c>
       <c r="B54" t="s">
-        <v>154</v>
+        <v>119</v>
       </c>
       <c r="C54">
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>269</v>
+        <v>359</v>
       </c>
       <c r="E54" t="s">
-        <v>330</v>
+        <v>235</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>337</v>
+        <v>242</v>
       </c>
       <c r="G54">
         <v>1</v>
@@ -2867,22 +2867,22 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="B55" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="C55">
         <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>270</v>
+        <v>360</v>
       </c>
       <c r="E55" t="s">
-        <v>330</v>
+        <v>235</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>338</v>
+        <v>243</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -2890,22 +2890,22 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>228</v>
+        <v>191</v>
       </c>
       <c r="B56" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="C56">
         <v>4</v>
       </c>
       <c r="D56" t="s">
-        <v>271</v>
+        <v>361</v>
       </c>
       <c r="E56" t="s">
-        <v>339</v>
+        <v>244</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>340</v>
+        <v>245</v>
       </c>
       <c r="G56">
         <v>1</v>
@@ -2913,22 +2913,22 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="B57" t="s">
-        <v>157</v>
+        <v>122</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>281</v>
+        <v>362</v>
       </c>
       <c r="E57" t="s">
-        <v>328</v>
+        <v>233</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>341</v>
+        <v>246</v>
       </c>
       <c r="G57">
         <v>1</v>
@@ -2936,22 +2936,22 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>203</v>
+        <v>166</v>
       </c>
       <c r="B58" t="s">
-        <v>158</v>
+        <v>123</v>
       </c>
       <c r="C58">
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>282</v>
+        <v>363</v>
       </c>
       <c r="E58" t="s">
-        <v>342</v>
+        <v>247</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>343</v>
+        <v>248</v>
       </c>
       <c r="G58">
         <v>1</v>
@@ -2959,22 +2959,22 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>214</v>
+        <v>177</v>
       </c>
       <c r="B59" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="C59">
         <v>4</v>
       </c>
       <c r="D59" t="s">
-        <v>272</v>
+        <v>364</v>
       </c>
       <c r="E59" t="s">
-        <v>320</v>
+        <v>225</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>344</v>
+        <v>249</v>
       </c>
       <c r="G59">
         <v>1</v>
@@ -2982,22 +2982,22 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>229</v>
+        <v>192</v>
       </c>
       <c r="B60" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="C60">
         <v>4</v>
       </c>
       <c r="D60" t="s">
-        <v>273</v>
+        <v>365</v>
       </c>
       <c r="E60" t="s">
-        <v>345</v>
+        <v>250</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>346</v>
+        <v>251</v>
       </c>
       <c r="G60">
         <v>1</v>
@@ -3005,22 +3005,22 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>204</v>
+        <v>167</v>
       </c>
       <c r="B61" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="C61">
         <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>283</v>
+        <v>366</v>
       </c>
       <c r="E61" t="s">
-        <v>328</v>
+        <v>233</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>347</v>
+        <v>252</v>
       </c>
       <c r="G61">
         <v>1</v>
@@ -3028,22 +3028,22 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>205</v>
+        <v>168</v>
       </c>
       <c r="B62" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="C62">
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>284</v>
+        <v>367</v>
       </c>
       <c r="E62" t="s">
-        <v>314</v>
+        <v>219</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>348</v>
+        <v>253</v>
       </c>
       <c r="G62">
         <v>1</v>
@@ -3051,22 +3051,22 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>206</v>
+        <v>169</v>
       </c>
       <c r="B63" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="C63">
         <v>4</v>
       </c>
       <c r="D63" t="s">
-        <v>285</v>
+        <v>368</v>
       </c>
       <c r="E63" t="s">
-        <v>330</v>
+        <v>235</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>349</v>
+        <v>254</v>
       </c>
       <c r="G63">
         <v>1</v>
@@ -3074,22 +3074,22 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>230</v>
+        <v>193</v>
       </c>
       <c r="B64" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="C64">
         <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
       <c r="E64" t="s">
-        <v>350</v>
+        <v>255</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>351</v>
+        <v>256</v>
       </c>
       <c r="G64">
         <v>1</v>
@@ -3097,22 +3097,22 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>231</v>
+        <v>194</v>
       </c>
       <c r="B65" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="C65">
         <v>2</v>
       </c>
       <c r="D65" t="s">
-        <v>302</v>
+        <v>370</v>
       </c>
       <c r="E65" t="s">
-        <v>352</v>
+        <v>257</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>353</v>
+        <v>258</v>
       </c>
       <c r="G65">
         <v>1</v>
@@ -3120,22 +3120,22 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>232</v>
+        <v>195</v>
       </c>
       <c r="B66" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="C66">
         <v>4</v>
       </c>
       <c r="D66" t="s">
-        <v>274</v>
+        <v>371</v>
       </c>
       <c r="E66" t="s">
-        <v>330</v>
+        <v>235</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>354</v>
+        <v>259</v>
       </c>
       <c r="G66">
         <v>1</v>
@@ -3143,22 +3143,22 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>215</v>
+        <v>178</v>
       </c>
       <c r="B67" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="C67">
         <v>2</v>
       </c>
       <c r="D67" t="s">
-        <v>275</v>
+        <v>372</v>
       </c>
       <c r="E67" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>355</v>
+        <v>260</v>
       </c>
       <c r="G67">
         <v>1</v>
@@ -3166,22 +3166,22 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>233</v>
+        <v>196</v>
       </c>
       <c r="B68" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="C68">
         <v>2</v>
       </c>
       <c r="D68" t="s">
-        <v>290</v>
+        <v>373</v>
       </c>
       <c r="E68" t="s">
-        <v>352</v>
+        <v>257</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>355</v>
+        <v>260</v>
       </c>
       <c r="G68">
         <v>1</v>
@@ -3189,22 +3189,22 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>207</v>
+        <v>170</v>
       </c>
       <c r="B69" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="C69">
         <v>2</v>
       </c>
       <c r="D69" t="s">
-        <v>286</v>
+        <v>374</v>
       </c>
       <c r="E69" t="s">
-        <v>342</v>
+        <v>247</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>356</v>
+        <v>261</v>
       </c>
       <c r="G69">
         <v>1</v>
@@ -3212,22 +3212,22 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>234</v>
+        <v>197</v>
       </c>
       <c r="B70" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="C70">
         <v>2</v>
       </c>
       <c r="D70" t="s">
-        <v>291</v>
+        <v>375</v>
       </c>
       <c r="E70" t="s">
-        <v>352</v>
+        <v>257</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>357</v>
+        <v>262</v>
       </c>
       <c r="G70">
         <v>1</v>
@@ -3235,22 +3235,22 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
       <c r="B71" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="C71">
         <v>4</v>
       </c>
       <c r="D71" t="s">
-        <v>287</v>
+        <v>376</v>
       </c>
       <c r="E71" t="s">
-        <v>314</v>
+        <v>219</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>358</v>
+        <v>263</v>
       </c>
       <c r="G71">
         <v>1</v>
@@ -3258,22 +3258,22 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>235</v>
+        <v>198</v>
       </c>
       <c r="B72" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="C72">
         <v>4</v>
       </c>
       <c r="D72" t="s">
-        <v>276</v>
+        <v>377</v>
       </c>
       <c r="E72" t="s">
-        <v>330</v>
+        <v>235</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>359</v>
+        <v>264</v>
       </c>
       <c r="G72">
         <v>1</v>
@@ -3281,22 +3281,22 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="B73" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="C73">
         <v>4</v>
       </c>
       <c r="D73" t="s">
-        <v>288</v>
+        <v>378</v>
       </c>
       <c r="E73" t="s">
-        <v>360</v>
+        <v>265</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>361</v>
+        <v>266</v>
       </c>
       <c r="G73">
         <v>1</v>
@@ -3304,22 +3304,22 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="B74" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="C74">
         <v>3</v>
       </c>
       <c r="D74" t="s">
-        <v>277</v>
+        <v>379</v>
       </c>
       <c r="E74" t="s">
-        <v>362</v>
+        <v>267</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>363</v>
+        <v>268</v>
       </c>
       <c r="G74">
         <v>1</v>
@@ -3327,22 +3327,22 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>237</v>
+        <v>200</v>
       </c>
       <c r="B75" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="C75">
         <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>278</v>
+        <v>380</v>
       </c>
       <c r="E75" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>363</v>
+        <v>268</v>
       </c>
       <c r="G75">
         <v>1</v>
@@ -3350,22 +3350,22 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>210</v>
+        <v>173</v>
       </c>
       <c r="B76" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="C76">
         <v>4</v>
       </c>
       <c r="D76" t="s">
-        <v>289</v>
+        <v>381</v>
       </c>
       <c r="E76" t="s">
-        <v>330</v>
+        <v>235</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>364</v>
+        <v>269</v>
       </c>
       <c r="G76">
         <v>1</v>
@@ -3373,22 +3373,22 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>218</v>
+        <v>181</v>
       </c>
       <c r="B77" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="C77">
         <v>4</v>
       </c>
       <c r="D77" t="s">
-        <v>279</v>
+        <v>382</v>
       </c>
       <c r="E77" t="s">
-        <v>365</v>
+        <v>270</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>366</v>
+        <v>271</v>
       </c>
       <c r="G77">
         <v>1</v>
@@ -3396,22 +3396,22 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
       <c r="B78" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="C78">
         <v>4</v>
       </c>
       <c r="D78" t="s">
-        <v>292</v>
+        <v>383</v>
       </c>
       <c r="E78" t="s">
-        <v>367</v>
+        <v>272</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>368</v>
+        <v>273</v>
       </c>
       <c r="G78">
         <v>1</v>
@@ -3419,22 +3419,22 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>216</v>
+        <v>179</v>
       </c>
       <c r="B79" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="C79">
         <v>4</v>
       </c>
       <c r="D79" t="s">
-        <v>293</v>
+        <v>384</v>
       </c>
       <c r="E79" t="s">
-        <v>362</v>
+        <v>267</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>369</v>
+        <v>274</v>
       </c>
       <c r="G79">
         <v>1</v>
@@ -3442,22 +3442,22 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>239</v>
+        <v>202</v>
       </c>
       <c r="B80" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="C80">
         <v>3</v>
       </c>
       <c r="D80" t="s">
-        <v>294</v>
+        <v>385</v>
       </c>
       <c r="E80" t="s">
-        <v>370</v>
+        <v>275</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>371</v>
+        <v>276</v>
       </c>
       <c r="G80">
         <v>1</v>
@@ -3465,22 +3465,22 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>240</v>
+        <v>203</v>
       </c>
       <c r="B81" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="C81">
         <v>4</v>
       </c>
       <c r="D81" t="s">
-        <v>295</v>
+        <v>386</v>
       </c>
       <c r="E81" t="s">
-        <v>372</v>
+        <v>277</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>373</v>
+        <v>278</v>
       </c>
       <c r="G81">
         <v>1</v>
@@ -3488,22 +3488,22 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>241</v>
+        <v>204</v>
       </c>
       <c r="B82" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="C82">
         <v>4</v>
       </c>
       <c r="D82" t="s">
-        <v>296</v>
+        <v>387</v>
       </c>
       <c r="E82" t="s">
-        <v>352</v>
+        <v>257</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>374</v>
+        <v>279</v>
       </c>
       <c r="G82">
         <v>1</v>
@@ -3511,22 +3511,22 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>242</v>
+        <v>205</v>
       </c>
       <c r="B83" t="s">
-        <v>183</v>
+        <v>148</v>
       </c>
       <c r="C83">
         <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>309</v>
+        <v>388</v>
       </c>
       <c r="E83" t="s">
-        <v>328</v>
+        <v>233</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>375</v>
+        <v>280</v>
       </c>
       <c r="G83">
         <v>1</v>
@@ -3534,22 +3534,22 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>243</v>
+        <v>206</v>
       </c>
       <c r="B84" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="C84">
         <v>3</v>
       </c>
       <c r="D84" t="s">
-        <v>297</v>
+        <v>389</v>
       </c>
       <c r="E84" t="s">
-        <v>376</v>
+        <v>281</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>377</v>
+        <v>282</v>
       </c>
       <c r="G84">
         <v>1</v>
@@ -3557,22 +3557,22 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>244</v>
+        <v>207</v>
       </c>
       <c r="B85" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
       <c r="C85">
         <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>298</v>
+        <v>390</v>
       </c>
       <c r="E85" t="s">
-        <v>376</v>
+        <v>281</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>378</v>
+        <v>283</v>
       </c>
       <c r="G85">
         <v>1</v>
@@ -3580,22 +3580,22 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>245</v>
+        <v>208</v>
       </c>
       <c r="B86" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
       <c r="C86">
         <v>4</v>
       </c>
       <c r="D86" t="s">
-        <v>299</v>
+        <v>391</v>
       </c>
       <c r="E86" t="s">
-        <v>379</v>
+        <v>284</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>380</v>
+        <v>285</v>
       </c>
       <c r="G86">
         <v>1</v>
@@ -3603,22 +3603,22 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>246</v>
+        <v>209</v>
       </c>
       <c r="B87" t="s">
-        <v>187</v>
+        <v>152</v>
       </c>
       <c r="C87">
         <v>2</v>
       </c>
       <c r="D87" t="s">
-        <v>300</v>
+        <v>392</v>
       </c>
       <c r="E87" t="s">
-        <v>314</v>
+        <v>219</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>381</v>
+        <v>286</v>
       </c>
       <c r="G87">
         <v>1</v>
@@ -3626,22 +3626,22 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>247</v>
+        <v>210</v>
       </c>
       <c r="B88" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="C88">
         <v>4</v>
       </c>
       <c r="D88" t="s">
-        <v>303</v>
+        <v>393</v>
       </c>
       <c r="E88" t="s">
-        <v>330</v>
+        <v>235</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>382</v>
+        <v>287</v>
       </c>
       <c r="G88">
         <v>1</v>
@@ -3649,22 +3649,22 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>248</v>
+        <v>211</v>
       </c>
       <c r="B89" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
       <c r="C89">
         <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>304</v>
+        <v>394</v>
       </c>
       <c r="E89" t="s">
-        <v>383</v>
+        <v>288</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>385</v>
+        <v>290</v>
       </c>
       <c r="G89">
         <v>1</v>
@@ -3672,22 +3672,22 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>249</v>
+        <v>403</v>
       </c>
       <c r="B90" t="s">
-        <v>190</v>
+        <v>155</v>
       </c>
       <c r="C90">
         <v>4</v>
       </c>
       <c r="D90" t="s">
-        <v>305</v>
+        <v>404</v>
       </c>
       <c r="E90" t="s">
-        <v>352</v>
+        <v>257</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>386</v>
+        <v>291</v>
       </c>
       <c r="G90">
         <v>1</v>
@@ -3695,22 +3695,22 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>250</v>
+        <v>212</v>
       </c>
       <c r="B91" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="C91">
         <v>4</v>
       </c>
       <c r="D91" t="s">
-        <v>306</v>
+        <v>395</v>
       </c>
       <c r="E91" t="s">
-        <v>330</v>
+        <v>235</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>384</v>
+        <v>289</v>
       </c>
       <c r="G91">
         <v>1</v>
@@ -3718,22 +3718,22 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>251</v>
+        <v>213</v>
       </c>
       <c r="B92" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
       <c r="C92">
         <v>3</v>
       </c>
       <c r="D92" t="s">
-        <v>307</v>
+        <v>396</v>
       </c>
       <c r="E92" t="s">
-        <v>387</v>
+        <v>292</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>388</v>
+        <v>293</v>
       </c>
       <c r="G92">
         <v>1</v>
@@ -3741,22 +3741,22 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>219</v>
+        <v>182</v>
       </c>
       <c r="B93" t="s">
-        <v>193</v>
+        <v>158</v>
       </c>
       <c r="C93">
         <v>3</v>
       </c>
       <c r="D93" t="s">
-        <v>310</v>
+        <v>397</v>
       </c>
       <c r="E93" t="s">
-        <v>389</v>
+        <v>294</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>390</v>
+        <v>295</v>
       </c>
       <c r="G93">
         <v>1</v>
@@ -3764,22 +3764,22 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
       <c r="B94" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
       <c r="C94">
         <v>3</v>
       </c>
       <c r="D94" t="s">
-        <v>308</v>
+        <v>398</v>
       </c>
       <c r="E94" t="s">
-        <v>391</v>
+        <v>296</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>392</v>
+        <v>297</v>
       </c>
       <c r="G94">
         <v>1</v>
@@ -3787,22 +3787,22 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>393</v>
+        <v>298</v>
       </c>
       <c r="B95" t="s">
-        <v>394</v>
+        <v>299</v>
       </c>
       <c r="C95">
         <v>1</v>
       </c>
       <c r="D95" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="E95" t="s">
-        <v>396</v>
+        <v>300</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>397</v>
+        <v>301</v>
       </c>
       <c r="G95">
         <v>1</v>
@@ -3810,10 +3810,10 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>398</v>
+        <v>302</v>
       </c>
       <c r="B96" t="s">
-        <v>399</v>
+        <v>303</v>
       </c>
       <c r="C96">
         <v>2</v>
@@ -3822,10 +3822,10 @@
         <v>400</v>
       </c>
       <c r="E96" t="s">
-        <v>396</v>
+        <v>300</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>397</v>
+        <v>301</v>
       </c>
       <c r="G96">
         <v>1</v>
@@ -3833,22 +3833,22 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>401</v>
+        <v>304</v>
       </c>
       <c r="B97" t="s">
-        <v>402</v>
+        <v>305</v>
       </c>
       <c r="C97">
         <v>2</v>
       </c>
       <c r="D97" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E97" t="s">
-        <v>396</v>
+        <v>300</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>397</v>
+        <v>301</v>
       </c>
       <c r="G97">
         <v>1</v>
@@ -3856,22 +3856,22 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>404</v>
+        <v>306</v>
       </c>
       <c r="B98" t="s">
-        <v>405</v>
+        <v>307</v>
       </c>
       <c r="C98">
         <v>2</v>
       </c>
       <c r="D98" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="E98" t="s">
-        <v>396</v>
+        <v>300</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>397</v>
+        <v>301</v>
       </c>
       <c r="G98">
         <v>1</v>

</xml_diff>

<commit_message>
Added vanilla non-needy modules and improved filter method.
Former-commit-id: 54c48a717579249dba8636729cb6058308e36339
Former-commit-id: b71e3d97d6d17f735adf28c9ea564c23c73c32d1
</commit_message>
<xml_diff>
--- a/resources/modules-config-details-setup.xlsx
+++ b/resources/modules-config-details-setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\IdeaProjects\MakeMyManual\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBF696A-1D1E-473F-9E54-1E1E64D79FE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794F18A1-542D-41B0-A0DE-68DA0EFFFC58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
+    <workbookView xWindow="1320" yWindow="350" windowWidth="12780" windowHeight="6600" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="437">
   <si>
     <t>Colour Flash</t>
   </si>
@@ -1254,6 +1254,96 @@
   </si>
   <si>
     <t>modules/Monsplode Fight.pdf</t>
+  </si>
+  <si>
+    <t>Wires</t>
+  </si>
+  <si>
+    <t>modules/Wires.pdf</t>
+  </si>
+  <si>
+    <t>Steel Crate Games</t>
+  </si>
+  <si>
+    <t>2015-10-08</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>BigButton</t>
+  </si>
+  <si>
+    <t>modules/The Button.pdf</t>
+  </si>
+  <si>
+    <t>Keypad</t>
+  </si>
+  <si>
+    <t>modules/Keypad.pdf</t>
+  </si>
+  <si>
+    <t>Simon Says</t>
+  </si>
+  <si>
+    <t>Simon</t>
+  </si>
+  <si>
+    <t>modules/Simon Says.pdf</t>
+  </si>
+  <si>
+    <t>Who's On First</t>
+  </si>
+  <si>
+    <t>WhosOnFirst</t>
+  </si>
+  <si>
+    <t>modules/Who's On First.pdf</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>modules/Memory.pdf</t>
+  </si>
+  <si>
+    <t>Morse Code</t>
+  </si>
+  <si>
+    <t>Morse</t>
+  </si>
+  <si>
+    <t>modules/Morse Code.pdf</t>
+  </si>
+  <si>
+    <t>Complicated Wires</t>
+  </si>
+  <si>
+    <t>Venn</t>
+  </si>
+  <si>
+    <t>modules/Complicated Wires.pdf</t>
+  </si>
+  <si>
+    <t>Wire Sequence</t>
+  </si>
+  <si>
+    <t>WireSequence</t>
+  </si>
+  <si>
+    <t>modules/Wire Sequence.pdf</t>
+  </si>
+  <si>
+    <t>Maze</t>
+  </si>
+  <si>
+    <t>modules/Maze.pdf</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>modules/Password.pdf</t>
   </si>
 </sst>
 </file>
@@ -1606,10 +1696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC09710-E84E-49A6-94A5-EB5A61B7898A}">
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="72" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="72" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3877,6 +3967,259 @@
         <v>1</v>
       </c>
     </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>407</v>
+      </c>
+      <c r="B99" t="s">
+        <v>407</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99" t="s">
+        <v>408</v>
+      </c>
+      <c r="E99" t="s">
+        <v>409</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>411</v>
+      </c>
+      <c r="B100" t="s">
+        <v>412</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100" t="s">
+        <v>413</v>
+      </c>
+      <c r="E100" t="s">
+        <v>409</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>414</v>
+      </c>
+      <c r="B101" t="s">
+        <v>414</v>
+      </c>
+      <c r="C101">
+        <v>2</v>
+      </c>
+      <c r="D101" t="s">
+        <v>415</v>
+      </c>
+      <c r="E101" t="s">
+        <v>409</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>416</v>
+      </c>
+      <c r="B102" t="s">
+        <v>417</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+      <c r="D102" t="s">
+        <v>418</v>
+      </c>
+      <c r="E102" t="s">
+        <v>409</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>419</v>
+      </c>
+      <c r="B103" t="s">
+        <v>420</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
+      </c>
+      <c r="D103" t="s">
+        <v>421</v>
+      </c>
+      <c r="E103" t="s">
+        <v>409</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>422</v>
+      </c>
+      <c r="B104" t="s">
+        <v>422</v>
+      </c>
+      <c r="C104">
+        <v>2</v>
+      </c>
+      <c r="D104" t="s">
+        <v>423</v>
+      </c>
+      <c r="E104" t="s">
+        <v>409</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>424</v>
+      </c>
+      <c r="B105" t="s">
+        <v>425</v>
+      </c>
+      <c r="C105">
+        <v>3</v>
+      </c>
+      <c r="D105" t="s">
+        <v>426</v>
+      </c>
+      <c r="E105" t="s">
+        <v>409</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>427</v>
+      </c>
+      <c r="B106" t="s">
+        <v>428</v>
+      </c>
+      <c r="C106">
+        <v>3</v>
+      </c>
+      <c r="D106" t="s">
+        <v>429</v>
+      </c>
+      <c r="E106" t="s">
+        <v>409</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>430</v>
+      </c>
+      <c r="B107" t="s">
+        <v>431</v>
+      </c>
+      <c r="C107">
+        <v>3</v>
+      </c>
+      <c r="D107" t="s">
+        <v>432</v>
+      </c>
+      <c r="E107" t="s">
+        <v>409</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>433</v>
+      </c>
+      <c r="B108" t="s">
+        <v>433</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
+      </c>
+      <c r="D108" t="s">
+        <v>434</v>
+      </c>
+      <c r="E108" t="s">
+        <v>409</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>435</v>
+      </c>
+      <c r="B109" t="s">
+        <v>435</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
+      </c>
+      <c r="D109" t="s">
+        <v>436</v>
+      </c>
+      <c r="E109" t="s">
+        <v>409</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added vanilla needy modules
Former-commit-id: 054ff4ef8c847838abd9f8b03f137e5a27094d40
Former-commit-id: 9837844ed6849e9bfde17099076ecc6f8a913c7d
</commit_message>
<xml_diff>
--- a/resources/modules-config-details-setup.xlsx
+++ b/resources/modules-config-details-setup.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\IdeaProjects\MakeMyManual\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794F18A1-542D-41B0-A0DE-68DA0EFFFC58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{03212471-3CDE-45AB-8287-3885681BBD28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="350" windowWidth="12780" windowHeight="6600" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="modules-config-details" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="446">
   <si>
     <t>Colour Flash</t>
   </si>
@@ -1344,6 +1344,33 @@
   </si>
   <si>
     <t>modules/Password.pdf</t>
+  </si>
+  <si>
+    <t>Capacitor Discharge</t>
+  </si>
+  <si>
+    <t>NeedyCapacitor</t>
+  </si>
+  <si>
+    <t>modules/Capacitor Discharge.pdf</t>
+  </si>
+  <si>
+    <t>Knob</t>
+  </si>
+  <si>
+    <t>NeedyKnob</t>
+  </si>
+  <si>
+    <t>modules/Knob.pdf</t>
+  </si>
+  <si>
+    <t>Venting Gas</t>
+  </si>
+  <si>
+    <t>NeedyVentGas</t>
+  </si>
+  <si>
+    <t>modules/Venting Gas.pdf</t>
   </si>
 </sst>
 </file>
@@ -1696,10 +1723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC09710-E84E-49A6-94A5-EB5A61B7898A}">
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="72" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="72" workbookViewId="0">
+      <selection activeCell="J99" sqref="J99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4220,6 +4247,75 @@
         <v>0</v>
       </c>
     </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>437</v>
+      </c>
+      <c r="B110" t="s">
+        <v>438</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="D110" t="s">
+        <v>439</v>
+      </c>
+      <c r="E110" t="s">
+        <v>409</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>440</v>
+      </c>
+      <c r="B111" t="s">
+        <v>441</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+      <c r="D111" t="s">
+        <v>442</v>
+      </c>
+      <c r="E111" t="s">
+        <v>409</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>443</v>
+      </c>
+      <c r="B112" t="s">
+        <v>444</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+      <c r="D112" t="s">
+        <v>445</v>
+      </c>
+      <c r="E112" t="s">
+        <v>409</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G112">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added two extra needy modules for a centurion manual
Former-commit-id: 438657188b70be04bb555bdd10d0b580bbf55f4e
Former-commit-id: 1bdfd2a345c7f6c299e1280b0b4252b2327c2a07
</commit_message>
<xml_diff>
--- a/resources/modules-config-details-setup.xlsx
+++ b/resources/modules-config-details-setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\IdeaProjects\MakeMyManual\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03212471-3CDE-45AB-8287-3885681BBD28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08A4B26-D8DB-437C-990A-D1E5C13D08DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="454">
   <si>
     <t>Colour Flash</t>
   </si>
@@ -1371,6 +1371,30 @@
   </si>
   <si>
     <t>modules/Venting Gas.pdf</t>
+  </si>
+  <si>
+    <t>German Venting Gas</t>
+  </si>
+  <si>
+    <t>VentGasTranslated</t>
+  </si>
+  <si>
+    <t>modules/German Venting Gas.pdf</t>
+  </si>
+  <si>
+    <t>Refill That Beer!</t>
+  </si>
+  <si>
+    <t>NeedyBeer</t>
+  </si>
+  <si>
+    <t>modules/Refill That Beer!.pdf</t>
+  </si>
+  <si>
+    <t>scripto</t>
+  </si>
+  <si>
+    <t>2017-09-23</t>
   </si>
 </sst>
 </file>
@@ -1723,10 +1747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC09710-E84E-49A6-94A5-EB5A61B7898A}">
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="72" workbookViewId="0">
-      <selection activeCell="J99" sqref="J99"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="72" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4316,6 +4340,52 @@
         <v>2</v>
       </c>
     </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>446</v>
+      </c>
+      <c r="B113" t="s">
+        <v>447</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113" t="s">
+        <v>448</v>
+      </c>
+      <c r="E113" t="s">
+        <v>300</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="G113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>449</v>
+      </c>
+      <c r="B114" t="s">
+        <v>450</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+      <c r="D114" t="s">
+        <v>451</v>
+      </c>
+      <c r="E114" t="s">
+        <v>452</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="G114">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed pdf compilation so the pdf is compiled to the right place. Other files could do with a tidy.
Former-commit-id: cb4a7158931fa6c1a12b3490a403037050f7114c
Former-commit-id: a3d384a79a1742fc846dd7ccf990a7e806ab6fa1
</commit_message>
<xml_diff>
--- a/resources/modules-config-details-setup.xlsx
+++ b/resources/modules-config-details-setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\IdeaProjects\MakeMyManual\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08A4B26-D8DB-437C-990A-D1E5C13D08DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341C5256-315A-406A-83CD-8D11AE5800E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
   </bookViews>
@@ -1388,13 +1388,13 @@
     <t>NeedyBeer</t>
   </si>
   <si>
-    <t>modules/Refill That Beer!.pdf</t>
-  </si>
-  <si>
     <t>scripto</t>
   </si>
   <si>
     <t>2017-09-23</t>
+  </si>
+  <si>
+    <t>modules/Refill That Beer.pdf</t>
   </si>
 </sst>
 </file>
@@ -1750,7 +1750,7 @@
   <dimension ref="A1:G114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" zoomScale="72" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116"/>
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4374,13 +4374,13 @@
         <v>1</v>
       </c>
       <c r="D114" t="s">
+        <v>453</v>
+      </c>
+      <c r="E114" t="s">
         <v>451</v>
       </c>
-      <c r="E114" t="s">
+      <c r="F114" s="1" t="s">
         <v>452</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>453</v>
       </c>
       <c r="G114">
         <v>2</v>

</xml_diff>

<commit_message>
Added 10 more modules.
Former-commit-id: 152b7d61a0aa0116ede68c4a704621c990737371
Former-commit-id: b3f8ef05359660787f9578beca230443c184e6a1
</commit_message>
<xml_diff>
--- a/resources/modules-config-details-setup.xlsx
+++ b/resources/modules-config-details-setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\IdeaProjects\MakeMyManual\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341C5256-315A-406A-83CD-8D11AE5800E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B87D66-0579-466B-96FA-3ED57C6F8E5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
+    <workbookView xWindow="-6340" yWindow="3000" windowWidth="12780" windowHeight="6600" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
   </bookViews>
   <sheets>
     <sheet name="modules-config-details" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="578">
   <si>
     <t>Colour Flash</t>
   </si>
@@ -1395,6 +1395,378 @@
   </si>
   <si>
     <t>modules/Refill That Beer.pdf</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Needy Math</t>
+  </si>
+  <si>
+    <t>modules/Math.pdf</t>
+  </si>
+  <si>
+    <t>Lights Out</t>
+  </si>
+  <si>
+    <t>LightsOut</t>
+  </si>
+  <si>
+    <t>modules/Lights Out.pdf</t>
+  </si>
+  <si>
+    <t>2016-07-22</t>
+  </si>
+  <si>
+    <t>Filibuster</t>
+  </si>
+  <si>
+    <t>modules/Filibuster.pdf</t>
+  </si>
+  <si>
+    <t>2016-08-07</t>
+  </si>
+  <si>
+    <t>Motion Sense</t>
+  </si>
+  <si>
+    <t>MotionSense</t>
+  </si>
+  <si>
+    <t>modules/Motion Sense.pdf</t>
+  </si>
+  <si>
+    <t>2016-08-11</t>
+  </si>
+  <si>
+    <t>Answering Questions</t>
+  </si>
+  <si>
+    <t>NeedyVentV2</t>
+  </si>
+  <si>
+    <t>modules/Answering Questions.pdf</t>
+  </si>
+  <si>
+    <t>Rotary Phone</t>
+  </si>
+  <si>
+    <t>NeedyKnobV2</t>
+  </si>
+  <si>
+    <t>modules/Rotary Phone.pdf</t>
+  </si>
+  <si>
+    <t>Cruel Piano Keys</t>
+  </si>
+  <si>
+    <t>CruelPianoKeys</t>
+  </si>
+  <si>
+    <t>modules/Cruel Piano Keys.pdf</t>
+  </si>
+  <si>
+    <t>Tetris</t>
+  </si>
+  <si>
+    <t>spwizTetris</t>
+  </si>
+  <si>
+    <t>modules/Tetris.pdf</t>
+  </si>
+  <si>
+    <t>2016-08-23</t>
+  </si>
+  <si>
+    <t>Who's That Monsplode</t>
+  </si>
+  <si>
+    <t>monsplodeWho</t>
+  </si>
+  <si>
+    <t>modules/Who's That Monsplode.pdf</t>
+  </si>
+  <si>
+    <t>HTTP Response</t>
+  </si>
+  <si>
+    <t>http</t>
+  </si>
+  <si>
+    <t>modules/HTTP Response.pdf</t>
+  </si>
+  <si>
+    <t>2017-01-24</t>
+  </si>
+  <si>
+    <t>Edgework</t>
+  </si>
+  <si>
+    <t>EdgeworkModule</t>
+  </si>
+  <si>
+    <t>modules/Edgework.pdf</t>
+  </si>
+  <si>
+    <t>Ion Lee, ZekNikZ</t>
+  </si>
+  <si>
+    <t>Hex To Decimal</t>
+  </si>
+  <si>
+    <t>EternitySDec</t>
+  </si>
+  <si>
+    <t>modules/Hex To Decimal.pdf</t>
+  </si>
+  <si>
+    <t>EternityShack</t>
+  </si>
+  <si>
+    <t>2017-06-30</t>
+  </si>
+  <si>
+    <t>X-Ray</t>
+  </si>
+  <si>
+    <t>XRayModule</t>
+  </si>
+  <si>
+    <t>modules/X-Ray.pdf</t>
+  </si>
+  <si>
+    <t>2017-07-14</t>
+  </si>
+  <si>
+    <t>QR Code</t>
+  </si>
+  <si>
+    <t>QRCode</t>
+  </si>
+  <si>
+    <t>modules/QR Code.pdf</t>
+  </si>
+  <si>
+    <t>2017-07-17</t>
+  </si>
+  <si>
+    <t>Button Masher</t>
+  </si>
+  <si>
+    <t>buttonMasherNeedy</t>
+  </si>
+  <si>
+    <t>modules/Button Masher.pdf</t>
+  </si>
+  <si>
+    <t>McDude73</t>
+  </si>
+  <si>
+    <t>2017-07-19</t>
+  </si>
+  <si>
+    <t>Random Number Generator</t>
+  </si>
+  <si>
+    <t>rng</t>
+  </si>
+  <si>
+    <t>modules/Random Number Generator.pdf</t>
+  </si>
+  <si>
+    <t>Lumbud84, McDude73</t>
+  </si>
+  <si>
+    <t>2017-07-21</t>
+  </si>
+  <si>
+    <t>Color Morse</t>
+  </si>
+  <si>
+    <t>ColorMorseModule</t>
+  </si>
+  <si>
+    <t>modules/Color Morse.pdf</t>
+  </si>
+  <si>
+    <t>SKiPP, Ezekiel, ZekNikZ</t>
+  </si>
+  <si>
+    <t>2017-07-31</t>
+  </si>
+  <si>
+    <t>Mastermind Simple</t>
+  </si>
+  <si>
+    <t>modules/Mastermind Simple.pdf</t>
+  </si>
+  <si>
+    <t>Eotall</t>
+  </si>
+  <si>
+    <t>2017-08-06</t>
+  </si>
+  <si>
+    <t>Mastermind Cruel</t>
+  </si>
+  <si>
+    <t>modules/Mastermind Cruel.pdf</t>
+  </si>
+  <si>
+    <t>Gridlock</t>
+  </si>
+  <si>
+    <t>GridlockModule</t>
+  </si>
+  <si>
+    <t>modules/Gridlock.pdf</t>
+  </si>
+  <si>
+    <t>Elias, Timwi</t>
+  </si>
+  <si>
+    <t>2017-08-11</t>
+  </si>
+  <si>
+    <t>Big Circle</t>
+  </si>
+  <si>
+    <t>BigCircle</t>
+  </si>
+  <si>
+    <t>modules/Big Circle.pdf</t>
+  </si>
+  <si>
+    <t>Ezekiel, Hendruid, CaitSith2</t>
+  </si>
+  <si>
+    <t>2017-08-14</t>
+  </si>
+  <si>
+    <t>Morse-A-Maze</t>
+  </si>
+  <si>
+    <t>MorseAMaze</t>
+  </si>
+  <si>
+    <t>modules/Morse-A-Maze.pdf</t>
+  </si>
+  <si>
+    <t>CaitSith2</t>
+  </si>
+  <si>
+    <t>2017-08-21</t>
+  </si>
+  <si>
+    <t>Colored Switches</t>
+  </si>
+  <si>
+    <t>ColoredSwitchesModule</t>
+  </si>
+  <si>
+    <t>modules/Colored Switches.pdf</t>
+  </si>
+  <si>
+    <t>2017-09-03</t>
+  </si>
+  <si>
+    <t>Perplexing Wires</t>
+  </si>
+  <si>
+    <t>PerplexingWiresModule</t>
+  </si>
+  <si>
+    <t>modules/Perplexing Wires.pdf</t>
+  </si>
+  <si>
+    <t>MarAyzex, Ezekiel, Timwi</t>
+  </si>
+  <si>
+    <t>2017-09-06</t>
+  </si>
+  <si>
+    <t>Monsplode Trading Cards</t>
+  </si>
+  <si>
+    <t>monsplodeCards</t>
+  </si>
+  <si>
+    <t>modules/Monsplode Trading Cards.pdf</t>
+  </si>
+  <si>
+    <t>clutterArranger, Grybo</t>
+  </si>
+  <si>
+    <t>2017-09-10</t>
+  </si>
+  <si>
+    <t>Game Of Life Simple</t>
+  </si>
+  <si>
+    <t>GameOfLifeSimple</t>
+  </si>
+  <si>
+    <t>GameOfLifeCruel</t>
+  </si>
+  <si>
+    <t>modules/Game Of Life Simple.pdf</t>
+  </si>
+  <si>
+    <t>modules/Game Of Life Cruel.pdf</t>
+  </si>
+  <si>
+    <t>Eotall, WarioLGP, samfun123</t>
+  </si>
+  <si>
+    <t>Game Of Life Cruel</t>
+  </si>
+  <si>
+    <t>Nonogram</t>
+  </si>
+  <si>
+    <t>NonogramModule</t>
+  </si>
+  <si>
+    <t>modules/Nonogram.pdf</t>
+  </si>
+  <si>
+    <t>Piggered</t>
+  </si>
+  <si>
+    <t>2017-09-12</t>
+  </si>
+  <si>
+    <t>2017-09-19</t>
+  </si>
+  <si>
+    <t>S.E.T.</t>
+  </si>
+  <si>
+    <t>SetModule</t>
+  </si>
+  <si>
+    <t>modules/SET.pdf</t>
+  </si>
+  <si>
+    <t>Zawu, Timwi</t>
+  </si>
+  <si>
+    <t>Painting</t>
+  </si>
+  <si>
+    <t>modules/Painting.pdf</t>
+  </si>
+  <si>
+    <t>Hendruid, Bashly</t>
+  </si>
+  <si>
+    <t>2017-09-24</t>
+  </si>
+  <si>
+    <t>Color Generator</t>
+  </si>
+  <si>
+    <t>modules/Color Generator.pdf</t>
   </si>
 </sst>
 </file>
@@ -1747,10 +2119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC09710-E84E-49A6-94A5-EB5A61B7898A}">
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="72" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="72" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4386,6 +4758,719 @@
         <v>2</v>
       </c>
     </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>454</v>
+      </c>
+      <c r="B115" t="s">
+        <v>455</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="D115" t="s">
+        <v>456</v>
+      </c>
+      <c r="E115" t="s">
+        <v>10</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>457</v>
+      </c>
+      <c r="B116" t="s">
+        <v>458</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116" t="s">
+        <v>459</v>
+      </c>
+      <c r="E116" t="s">
+        <v>2</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="G116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>461</v>
+      </c>
+      <c r="B117" t="s">
+        <v>461</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
+      <c r="D117" t="s">
+        <v>462</v>
+      </c>
+      <c r="E117" t="s">
+        <v>10</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="G117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>464</v>
+      </c>
+      <c r="B118" t="s">
+        <v>465</v>
+      </c>
+      <c r="C118">
+        <v>1</v>
+      </c>
+      <c r="D118" t="s">
+        <v>466</v>
+      </c>
+      <c r="E118" t="s">
+        <v>2</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="G118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>468</v>
+      </c>
+      <c r="B119" t="s">
+        <v>469</v>
+      </c>
+      <c r="C119">
+        <v>1</v>
+      </c>
+      <c r="D119" t="s">
+        <v>470</v>
+      </c>
+      <c r="E119" t="s">
+        <v>30</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>471</v>
+      </c>
+      <c r="B120" t="s">
+        <v>472</v>
+      </c>
+      <c r="C120">
+        <v>2</v>
+      </c>
+      <c r="D120" t="s">
+        <v>473</v>
+      </c>
+      <c r="E120" t="s">
+        <v>30</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>474</v>
+      </c>
+      <c r="B121" t="s">
+        <v>475</v>
+      </c>
+      <c r="C121">
+        <v>4</v>
+      </c>
+      <c r="D121" t="s">
+        <v>476</v>
+      </c>
+      <c r="E121" t="s">
+        <v>2</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>477</v>
+      </c>
+      <c r="B122" t="s">
+        <v>478</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
+      <c r="D122" t="s">
+        <v>479</v>
+      </c>
+      <c r="E122" t="s">
+        <v>56</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="G122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>481</v>
+      </c>
+      <c r="B123" t="s">
+        <v>482</v>
+      </c>
+      <c r="C123">
+        <v>2</v>
+      </c>
+      <c r="D123" t="s">
+        <v>483</v>
+      </c>
+      <c r="E123" t="s">
+        <v>47</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="G123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>484</v>
+      </c>
+      <c r="B124" t="s">
+        <v>485</v>
+      </c>
+      <c r="C124">
+        <v>1</v>
+      </c>
+      <c r="D124" t="s">
+        <v>486</v>
+      </c>
+      <c r="E124" t="s">
+        <v>59</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="G124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>488</v>
+      </c>
+      <c r="B125" t="s">
+        <v>489</v>
+      </c>
+      <c r="C125">
+        <v>1</v>
+      </c>
+      <c r="D125" t="s">
+        <v>490</v>
+      </c>
+      <c r="E125" t="s">
+        <v>491</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>492</v>
+      </c>
+      <c r="B126" t="s">
+        <v>493</v>
+      </c>
+      <c r="C126">
+        <v>3</v>
+      </c>
+      <c r="D126" t="s">
+        <v>494</v>
+      </c>
+      <c r="E126" t="s">
+        <v>495</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="G126">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>497</v>
+      </c>
+      <c r="B127" t="s">
+        <v>498</v>
+      </c>
+      <c r="C127">
+        <v>2</v>
+      </c>
+      <c r="D127" t="s">
+        <v>499</v>
+      </c>
+      <c r="E127" t="s">
+        <v>235</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="G127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>501</v>
+      </c>
+      <c r="B128" t="s">
+        <v>502</v>
+      </c>
+      <c r="C128">
+        <v>1</v>
+      </c>
+      <c r="D128" t="s">
+        <v>503</v>
+      </c>
+      <c r="E128" t="s">
+        <v>59</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="G128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>505</v>
+      </c>
+      <c r="B129" t="s">
+        <v>506</v>
+      </c>
+      <c r="C129">
+        <v>1</v>
+      </c>
+      <c r="D129" t="s">
+        <v>507</v>
+      </c>
+      <c r="E129" t="s">
+        <v>508</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>510</v>
+      </c>
+      <c r="B130" t="s">
+        <v>511</v>
+      </c>
+      <c r="C130">
+        <v>1</v>
+      </c>
+      <c r="D130" t="s">
+        <v>512</v>
+      </c>
+      <c r="E130" t="s">
+        <v>513</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="G130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>515</v>
+      </c>
+      <c r="B131" t="s">
+        <v>516</v>
+      </c>
+      <c r="C131">
+        <v>3</v>
+      </c>
+      <c r="D131" t="s">
+        <v>517</v>
+      </c>
+      <c r="E131" t="s">
+        <v>518</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="G131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>520</v>
+      </c>
+      <c r="B132" t="s">
+        <v>520</v>
+      </c>
+      <c r="C132">
+        <v>1</v>
+      </c>
+      <c r="D132" t="s">
+        <v>521</v>
+      </c>
+      <c r="E132" t="s">
+        <v>522</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="G132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>524</v>
+      </c>
+      <c r="B133" t="s">
+        <v>524</v>
+      </c>
+      <c r="C133">
+        <v>5</v>
+      </c>
+      <c r="D133" t="s">
+        <v>525</v>
+      </c>
+      <c r="E133" t="s">
+        <v>522</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="G133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>526</v>
+      </c>
+      <c r="B134" t="s">
+        <v>527</v>
+      </c>
+      <c r="C134">
+        <v>3</v>
+      </c>
+      <c r="D134" t="s">
+        <v>528</v>
+      </c>
+      <c r="E134" t="s">
+        <v>529</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="G134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>531</v>
+      </c>
+      <c r="B135" t="s">
+        <v>532</v>
+      </c>
+      <c r="C135">
+        <v>3</v>
+      </c>
+      <c r="D135" t="s">
+        <v>533</v>
+      </c>
+      <c r="E135" t="s">
+        <v>534</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="G135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>536</v>
+      </c>
+      <c r="B136" t="s">
+        <v>537</v>
+      </c>
+      <c r="C136">
+        <v>3</v>
+      </c>
+      <c r="D136" t="s">
+        <v>538</v>
+      </c>
+      <c r="E136" t="s">
+        <v>539</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="G136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>541</v>
+      </c>
+      <c r="B137" t="s">
+        <v>542</v>
+      </c>
+      <c r="C137">
+        <v>3</v>
+      </c>
+      <c r="D137" t="s">
+        <v>543</v>
+      </c>
+      <c r="E137" t="s">
+        <v>235</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="G137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>545</v>
+      </c>
+      <c r="B138" t="s">
+        <v>546</v>
+      </c>
+      <c r="C138">
+        <v>4</v>
+      </c>
+      <c r="D138" t="s">
+        <v>547</v>
+      </c>
+      <c r="E138" t="s">
+        <v>548</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="G138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>550</v>
+      </c>
+      <c r="B139" t="s">
+        <v>551</v>
+      </c>
+      <c r="C139">
+        <v>4</v>
+      </c>
+      <c r="D139" t="s">
+        <v>552</v>
+      </c>
+      <c r="E139" t="s">
+        <v>553</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="G139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>555</v>
+      </c>
+      <c r="B140" t="s">
+        <v>556</v>
+      </c>
+      <c r="C140">
+        <v>4</v>
+      </c>
+      <c r="D140" t="s">
+        <v>558</v>
+      </c>
+      <c r="E140" t="s">
+        <v>560</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="G140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>561</v>
+      </c>
+      <c r="B141" t="s">
+        <v>557</v>
+      </c>
+      <c r="C141">
+        <v>5</v>
+      </c>
+      <c r="D141" t="s">
+        <v>559</v>
+      </c>
+      <c r="E141" t="s">
+        <v>560</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="G141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>562</v>
+      </c>
+      <c r="B142" t="s">
+        <v>563</v>
+      </c>
+      <c r="C142">
+        <v>4</v>
+      </c>
+      <c r="D142" t="s">
+        <v>564</v>
+      </c>
+      <c r="E142" t="s">
+        <v>565</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="G142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>568</v>
+      </c>
+      <c r="B143" t="s">
+        <v>569</v>
+      </c>
+      <c r="C143">
+        <v>4</v>
+      </c>
+      <c r="D143" t="s">
+        <v>570</v>
+      </c>
+      <c r="E143" t="s">
+        <v>571</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>572</v>
+      </c>
+      <c r="B144" t="s">
+        <v>572</v>
+      </c>
+      <c r="C144">
+        <v>2</v>
+      </c>
+      <c r="D144" t="s">
+        <v>573</v>
+      </c>
+      <c r="E144" t="s">
+        <v>574</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="G144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>576</v>
+      </c>
+      <c r="B145" t="s">
+        <v>576</v>
+      </c>
+      <c r="C145">
+        <v>3</v>
+      </c>
+      <c r="D145" t="s">
+        <v>577</v>
+      </c>
+      <c r="E145" t="s">
+        <v>495</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="G145">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added 10 more modules. All modules released prior to 2018 now available.
Former-commit-id: df1b579c067f5efb98783e85880a2c784f29a958
Former-commit-id: e253ab8079d307cbc3c43afee415e94ee2f66a0e
</commit_message>
<xml_diff>
--- a/resources/modules-config-details-setup.xlsx
+++ b/resources/modules-config-details-setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\IdeaProjects\MakeMyManual\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B87D66-0579-466B-96FA-3ED57C6F8E5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB359DFD-B9EC-4275-B88C-E0F6B35EB859}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6340" yWindow="3000" windowWidth="12780" windowHeight="6600" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="12780" windowHeight="6600" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
   </bookViews>
   <sheets>
     <sheet name="modules-config-details" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="625">
   <si>
     <t>Colour Flash</t>
   </si>
@@ -1767,6 +1767,147 @@
   </si>
   <si>
     <t>modules/Color Generator.pdf</t>
+  </si>
+  <si>
+    <t>Shape Memory</t>
+  </si>
+  <si>
+    <t>needyShapeMemory</t>
+  </si>
+  <si>
+    <t>modules/Shape Memory.pdf</t>
+  </si>
+  <si>
+    <t>UltraCboy</t>
+  </si>
+  <si>
+    <t>2017-09-28</t>
+  </si>
+  <si>
+    <t>Symbol Cycle</t>
+  </si>
+  <si>
+    <t>SymbolCycleModule</t>
+  </si>
+  <si>
+    <t>modules/Symbol Cycle.pdf</t>
+  </si>
+  <si>
+    <t>2017-10-05</t>
+  </si>
+  <si>
+    <t>Hunting</t>
+  </si>
+  <si>
+    <t>hunting</t>
+  </si>
+  <si>
+    <t>modules/Hunting.pdf</t>
+  </si>
+  <si>
+    <t>taggedjc</t>
+  </si>
+  <si>
+    <t>2017-10-09</t>
+  </si>
+  <si>
+    <t>Extended Password</t>
+  </si>
+  <si>
+    <t>ExtendedPassword</t>
+  </si>
+  <si>
+    <t>modules/Extended Password.pdf</t>
+  </si>
+  <si>
+    <t>taggedjc, TWGaming</t>
+  </si>
+  <si>
+    <t>2017-10-24</t>
+  </si>
+  <si>
+    <t>Curriculum</t>
+  </si>
+  <si>
+    <t>curriculum</t>
+  </si>
+  <si>
+    <t>modules/Curriculum.pdf</t>
+  </si>
+  <si>
+    <t>Fixdoll</t>
+  </si>
+  <si>
+    <t>2017-10-30</t>
+  </si>
+  <si>
+    <t>Braille</t>
+  </si>
+  <si>
+    <t>BrailleModule</t>
+  </si>
+  <si>
+    <t>modules/Braille.pdf</t>
+  </si>
+  <si>
+    <t>2017-10-31</t>
+  </si>
+  <si>
+    <t>Mafia</t>
+  </si>
+  <si>
+    <t>MafiaModule</t>
+  </si>
+  <si>
+    <t>modules/Mafia.pdf</t>
+  </si>
+  <si>
+    <t>MarioXTurn, Ezekiel, Timwi</t>
+  </si>
+  <si>
+    <t>2017-11-04</t>
+  </si>
+  <si>
+    <t>Festive Piano Keys</t>
+  </si>
+  <si>
+    <t>FestivePianoKeys</t>
+  </si>
+  <si>
+    <t>modules/Festive Piano Keys.pdf</t>
+  </si>
+  <si>
+    <t>2017-12-07</t>
+  </si>
+  <si>
+    <t>Flags</t>
+  </si>
+  <si>
+    <t>FlagsModule</t>
+  </si>
+  <si>
+    <t>modules/Flags.pdf</t>
+  </si>
+  <si>
+    <t>Monopoly, Piggered</t>
+  </si>
+  <si>
+    <t>2017-12-24</t>
+  </si>
+  <si>
+    <t>Timezone</t>
+  </si>
+  <si>
+    <t>timezone</t>
+  </si>
+  <si>
+    <t>modules/Timezone.pdf</t>
+  </si>
+  <si>
+    <t>federan</t>
+  </si>
+  <si>
+    <t>2017-12-30</t>
   </si>
 </sst>
 </file>
@@ -2119,10 +2260,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC09710-E84E-49A6-94A5-EB5A61B7898A}">
-  <dimension ref="A1:G145"/>
+  <dimension ref="A1:G155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="72" workbookViewId="0">
-      <selection activeCell="A146" sqref="A146"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="72" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5471,6 +5612,236 @@
         <v>1</v>
       </c>
     </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>578</v>
+      </c>
+      <c r="B146" t="s">
+        <v>579</v>
+      </c>
+      <c r="C146">
+        <v>1</v>
+      </c>
+      <c r="D146" t="s">
+        <v>580</v>
+      </c>
+      <c r="E146" t="s">
+        <v>581</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="G146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>583</v>
+      </c>
+      <c r="B147" t="s">
+        <v>584</v>
+      </c>
+      <c r="C147">
+        <v>4</v>
+      </c>
+      <c r="D147" t="s">
+        <v>585</v>
+      </c>
+      <c r="E147" t="s">
+        <v>235</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="G147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>587</v>
+      </c>
+      <c r="B148" t="s">
+        <v>588</v>
+      </c>
+      <c r="C148">
+        <v>3</v>
+      </c>
+      <c r="D148" t="s">
+        <v>589</v>
+      </c>
+      <c r="E148" t="s">
+        <v>590</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="G148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>592</v>
+      </c>
+      <c r="B149" t="s">
+        <v>593</v>
+      </c>
+      <c r="C149">
+        <v>3</v>
+      </c>
+      <c r="D149" t="s">
+        <v>594</v>
+      </c>
+      <c r="E149" t="s">
+        <v>595</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="G149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>597</v>
+      </c>
+      <c r="B150" t="s">
+        <v>598</v>
+      </c>
+      <c r="C150">
+        <v>3</v>
+      </c>
+      <c r="D150" t="s">
+        <v>599</v>
+      </c>
+      <c r="E150" t="s">
+        <v>600</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="G150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>602</v>
+      </c>
+      <c r="B151" t="s">
+        <v>603</v>
+      </c>
+      <c r="C151">
+        <v>4</v>
+      </c>
+      <c r="D151" t="s">
+        <v>604</v>
+      </c>
+      <c r="E151" t="s">
+        <v>235</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="G151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>606</v>
+      </c>
+      <c r="B152" t="s">
+        <v>607</v>
+      </c>
+      <c r="C152">
+        <v>4</v>
+      </c>
+      <c r="D152" t="s">
+        <v>608</v>
+      </c>
+      <c r="E152" t="s">
+        <v>609</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="G152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>611</v>
+      </c>
+      <c r="B153" t="s">
+        <v>612</v>
+      </c>
+      <c r="C153">
+        <v>2</v>
+      </c>
+      <c r="D153" t="s">
+        <v>613</v>
+      </c>
+      <c r="E153" t="s">
+        <v>2</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="G153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>615</v>
+      </c>
+      <c r="B154" t="s">
+        <v>616</v>
+      </c>
+      <c r="C154">
+        <v>3</v>
+      </c>
+      <c r="D154" t="s">
+        <v>617</v>
+      </c>
+      <c r="E154" t="s">
+        <v>618</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="G154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>620</v>
+      </c>
+      <c r="B155" t="s">
+        <v>621</v>
+      </c>
+      <c r="C155">
+        <v>3</v>
+      </c>
+      <c r="D155" t="s">
+        <v>622</v>
+      </c>
+      <c r="E155" t="s">
+        <v>623</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="G155">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add all pre-2018 modules to the linking system. German Venting Gas temporarily removed - will probably have to host it myself. Need to properly thread the file downloading process at some point.
Former-commit-id: 2c3d6209556111ffeedc7051fe7021db52235667
Former-commit-id: 699e9767c4fcc2aca672bcdf35c5a2a1b1d5efc0
</commit_message>
<xml_diff>
--- a/resources/modules-config-details-setup.xlsx
+++ b/resources/modules-config-details-setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\IdeaProjects\MakeMyManual\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB359DFD-B9EC-4275-B88C-E0F6B35EB859}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9A2850-2971-4C92-AE8F-691A439D6A4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="12780" windowHeight="6600" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
+    <workbookView xWindow="340" yWindow="3340" windowWidth="12780" windowHeight="6600" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
   </bookViews>
   <sheets>
     <sheet name="modules-config-details" sheetId="1" r:id="rId1"/>
@@ -959,309 +959,12 @@
     <t>WhosOnFirstTranslated</t>
   </si>
   <si>
-    <t>modules/Colour Flash.pdf</t>
-  </si>
-  <si>
-    <t>modules/Piano Keys.pdf</t>
-  </si>
-  <si>
-    <t>modules/Semaphore.pdf</t>
-  </si>
-  <si>
-    <t>modules/Emoji Math.pdf</t>
-  </si>
-  <si>
-    <t>modules/Switches.pdf</t>
-  </si>
-  <si>
-    <t>modules/Two Bits.pdf</t>
-  </si>
-  <si>
-    <t>modules/Anagrams.pdf</t>
-  </si>
-  <si>
-    <t>modules/Word Scramble.pdf</t>
-  </si>
-  <si>
-    <t>modules/Combination Lock.pdf</t>
-  </si>
-  <si>
-    <t>modules/Square Button.pdf</t>
-  </si>
-  <si>
-    <t>modules/Simon States.pdf</t>
-  </si>
-  <si>
-    <t>modules/Round Keypad.pdf</t>
-  </si>
-  <si>
-    <t>modules/Listening.pdf</t>
-  </si>
-  <si>
-    <t>modules/Foreign Exchange Rates.pdf</t>
-  </si>
-  <si>
-    <t>modules/Orientation Cube.pdf</t>
-  </si>
-  <si>
-    <t>modules/Morsematics.pdf</t>
-  </si>
-  <si>
-    <t>modules/Connection Check.pdf</t>
-  </si>
-  <si>
-    <t>modules/Letter Keys.pdf</t>
-  </si>
-  <si>
-    <t>modules/Forget Me Not.pdf</t>
-  </si>
-  <si>
-    <t>modules/Astrology.pdf</t>
-  </si>
-  <si>
-    <t>modules/Logic.pdf</t>
-  </si>
-  <si>
-    <t>modules/Crazy Talk.pdf</t>
-  </si>
-  <si>
-    <t>modules/Adventure Game.pdf</t>
-  </si>
-  <si>
-    <t>modules/Turn The Key.pdf</t>
-  </si>
-  <si>
-    <t>modules/Turn The Keys.pdf</t>
-  </si>
-  <si>
-    <t>modules/Mystic Square.pdf</t>
-  </si>
-  <si>
-    <t>modules/Plumbing.pdf</t>
-  </si>
-  <si>
-    <t>modules/Safety Safe.pdf</t>
-  </si>
-  <si>
-    <t>modules/Cryptography.pdf</t>
-  </si>
-  <si>
-    <t>modules/Chess.pdf</t>
-  </si>
-  <si>
-    <t>modules/Mouse In The Maze.pdf</t>
-  </si>
-  <si>
-    <t>modules/3D Maze.pdf</t>
-  </si>
-  <si>
-    <t>modules/Silly Slots.pdf</t>
-  </si>
-  <si>
-    <t>modules/Number Pad.pdf</t>
-  </si>
-  <si>
-    <t>modules/Laundry.pdf</t>
-  </si>
-  <si>
-    <t>modules/Probing.pdf</t>
-  </si>
-  <si>
-    <t>modules/Resistors.pdf</t>
-  </si>
-  <si>
-    <t>modules/Skewed Slots.pdf</t>
-  </si>
-  <si>
-    <t>modules/Caesar Cipher.pdf</t>
-  </si>
-  <si>
-    <t>modules/Perspective Pegs.pdf</t>
-  </si>
-  <si>
-    <t>modules/Microcontroller.pdf</t>
-  </si>
-  <si>
-    <t>modules/Murder.pdf</t>
-  </si>
-  <si>
-    <t>modules/Tic-Tac-Toe.pdf</t>
-  </si>
-  <si>
-    <t>modules/Shape Shift.pdf</t>
-  </si>
-  <si>
-    <t>modules/Follow The Leader.pdf</t>
-  </si>
-  <si>
-    <t>modules/Friendship.pdf</t>
-  </si>
-  <si>
-    <t>modules/The Bulb.pdf</t>
-  </si>
-  <si>
-    <t>modules/Alphabet.pdf</t>
-  </si>
-  <si>
-    <t>modules/Blind Alley.pdf</t>
-  </si>
-  <si>
-    <t>modules/Sea Shells.pdf</t>
-  </si>
-  <si>
-    <t>modules/English Test.pdf</t>
-  </si>
-  <si>
-    <t>modules/Rock-Paper-Scissors-Lizard-Spock.pdf</t>
-  </si>
-  <si>
-    <t>modules/Hexamaze.pdf</t>
-  </si>
-  <si>
-    <t>modules/Bitmaps.pdf</t>
-  </si>
-  <si>
-    <t>modules/Colored Squares.pdf</t>
-  </si>
-  <si>
-    <t>modules/Adjacent Letters.pdf</t>
-  </si>
-  <si>
-    <t>modules/Third Base.pdf</t>
-  </si>
-  <si>
-    <t>modules/Souvenir.pdf</t>
-  </si>
-  <si>
-    <t>modules/Word Search.pdf</t>
-  </si>
-  <si>
-    <t>modules/Broken Buttons.pdf</t>
-  </si>
-  <si>
-    <t>modules/Simon Screams.pdf</t>
-  </si>
-  <si>
-    <t>modules/Modules Against Humanity.pdf</t>
-  </si>
-  <si>
-    <t>modules/Complicated Buttons.pdf</t>
-  </si>
-  <si>
-    <t>modules/Battleship.pdf</t>
-  </si>
-  <si>
-    <t>modules/Text Field.pdf</t>
-  </si>
-  <si>
-    <t>modules/Symbolic Password.pdf</t>
-  </si>
-  <si>
-    <t>modules/Wire Placement.pdf</t>
-  </si>
-  <si>
-    <t>modules/Double-Oh.pdf</t>
-  </si>
-  <si>
-    <t>modules/Cheap Checkout.pdf</t>
-  </si>
-  <si>
-    <t>modules/Coordinates.pdf</t>
-  </si>
-  <si>
-    <t>modules/Light Cycle.pdf</t>
-  </si>
-  <si>
-    <t>modules/Rhythms.pdf</t>
-  </si>
-  <si>
-    <t>modules/Color Math.pdf</t>
-  </si>
-  <si>
-    <t>modules/Only Connect.pdf</t>
-  </si>
-  <si>
-    <t>modules/Neutralization.pdf</t>
-  </si>
-  <si>
-    <t>modules/Web Design.pdf</t>
-  </si>
-  <si>
-    <t>modules/Chord Qualities.pdf</t>
-  </si>
-  <si>
-    <t>modules/Creation.pdf</t>
-  </si>
-  <si>
-    <t>modules/Rubik's Cube.pdf</t>
-  </si>
-  <si>
-    <t>modules/FizzBuzz.pdf</t>
-  </si>
-  <si>
-    <t>modules/The Clock.pdf</t>
-  </si>
-  <si>
-    <t>modules/LED Encryption.pdf</t>
-  </si>
-  <si>
-    <t>modules/Bitwise Operations.pdf</t>
-  </si>
-  <si>
-    <t>modules/Fast Math.pdf</t>
-  </si>
-  <si>
-    <t>modules/Minesweeper.pdf</t>
-  </si>
-  <si>
-    <t>modules/Zoo.pdf</t>
-  </si>
-  <si>
-    <t>modules/Binary LEDs.pdf</t>
-  </si>
-  <si>
-    <t>modules/Point Of Order.pdf</t>
-  </si>
-  <si>
-    <t>modules/Ice Cream.pdf</t>
-  </si>
-  <si>
-    <t>modules/The Screw.pdf</t>
-  </si>
-  <si>
-    <t>modules/Yahtzee.pdf</t>
-  </si>
-  <si>
-    <t>modules/German Button.pdf</t>
-  </si>
-  <si>
-    <t>modules/German Morse Code.pdf</t>
-  </si>
-  <si>
-    <t>modules/German Password.pdf</t>
-  </si>
-  <si>
-    <t>modules/German Who's On First.pdf</t>
-  </si>
-  <si>
     <t>Boolean Venn Diagrams</t>
   </si>
   <si>
-    <t>modules/Boolean Venn Diagram.pdf</t>
-  </si>
-  <si>
-    <t>modules/The Gamepad.pdf</t>
-  </si>
-  <si>
-    <t>modules/Monsplode Fight.pdf</t>
-  </si>
-  <si>
     <t>Wires</t>
   </si>
   <si>
-    <t>modules/Wires.pdf</t>
-  </si>
-  <si>
     <t>Steel Crate Games</t>
   </si>
   <si>
@@ -1274,105 +977,66 @@
     <t>BigButton</t>
   </si>
   <si>
-    <t>modules/The Button.pdf</t>
-  </si>
-  <si>
     <t>Keypad</t>
   </si>
   <si>
-    <t>modules/Keypad.pdf</t>
-  </si>
-  <si>
     <t>Simon Says</t>
   </si>
   <si>
     <t>Simon</t>
   </si>
   <si>
-    <t>modules/Simon Says.pdf</t>
-  </si>
-  <si>
     <t>Who's On First</t>
   </si>
   <si>
     <t>WhosOnFirst</t>
   </si>
   <si>
-    <t>modules/Who's On First.pdf</t>
-  </si>
-  <si>
     <t>Memory</t>
   </si>
   <si>
-    <t>modules/Memory.pdf</t>
-  </si>
-  <si>
     <t>Morse Code</t>
   </si>
   <si>
     <t>Morse</t>
   </si>
   <si>
-    <t>modules/Morse Code.pdf</t>
-  </si>
-  <si>
     <t>Complicated Wires</t>
   </si>
   <si>
     <t>Venn</t>
   </si>
   <si>
-    <t>modules/Complicated Wires.pdf</t>
-  </si>
-  <si>
     <t>Wire Sequence</t>
   </si>
   <si>
     <t>WireSequence</t>
   </si>
   <si>
-    <t>modules/Wire Sequence.pdf</t>
-  </si>
-  <si>
     <t>Maze</t>
   </si>
   <si>
-    <t>modules/Maze.pdf</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
-    <t>modules/Password.pdf</t>
-  </si>
-  <si>
     <t>Capacitor Discharge</t>
   </si>
   <si>
     <t>NeedyCapacitor</t>
   </si>
   <si>
-    <t>modules/Capacitor Discharge.pdf</t>
-  </si>
-  <si>
     <t>Knob</t>
   </si>
   <si>
     <t>NeedyKnob</t>
   </si>
   <si>
-    <t>modules/Knob.pdf</t>
-  </si>
-  <si>
     <t>Venting Gas</t>
   </si>
   <si>
     <t>NeedyVentGas</t>
   </si>
   <si>
-    <t>modules/Venting Gas.pdf</t>
-  </si>
-  <si>
     <t>German Venting Gas</t>
   </si>
   <si>
@@ -1394,36 +1058,24 @@
     <t>2017-09-23</t>
   </si>
   <si>
-    <t>modules/Refill That Beer.pdf</t>
-  </si>
-  <si>
     <t>Math</t>
   </si>
   <si>
     <t>Needy Math</t>
   </si>
   <si>
-    <t>modules/Math.pdf</t>
-  </si>
-  <si>
     <t>Lights Out</t>
   </si>
   <si>
     <t>LightsOut</t>
   </si>
   <si>
-    <t>modules/Lights Out.pdf</t>
-  </si>
-  <si>
     <t>2016-07-22</t>
   </si>
   <si>
     <t>Filibuster</t>
   </si>
   <si>
-    <t>modules/Filibuster.pdf</t>
-  </si>
-  <si>
     <t>2016-08-07</t>
   </si>
   <si>
@@ -1433,9 +1085,6 @@
     <t>MotionSense</t>
   </si>
   <si>
-    <t>modules/Motion Sense.pdf</t>
-  </si>
-  <si>
     <t>2016-08-11</t>
   </si>
   <si>
@@ -1445,36 +1094,24 @@
     <t>NeedyVentV2</t>
   </si>
   <si>
-    <t>modules/Answering Questions.pdf</t>
-  </si>
-  <si>
     <t>Rotary Phone</t>
   </si>
   <si>
     <t>NeedyKnobV2</t>
   </si>
   <si>
-    <t>modules/Rotary Phone.pdf</t>
-  </si>
-  <si>
     <t>Cruel Piano Keys</t>
   </si>
   <si>
     <t>CruelPianoKeys</t>
   </si>
   <si>
-    <t>modules/Cruel Piano Keys.pdf</t>
-  </si>
-  <si>
     <t>Tetris</t>
   </si>
   <si>
     <t>spwizTetris</t>
   </si>
   <si>
-    <t>modules/Tetris.pdf</t>
-  </si>
-  <si>
     <t>2016-08-23</t>
   </si>
   <si>
@@ -1484,18 +1121,12 @@
     <t>monsplodeWho</t>
   </si>
   <si>
-    <t>modules/Who's That Monsplode.pdf</t>
-  </si>
-  <si>
     <t>HTTP Response</t>
   </si>
   <si>
     <t>http</t>
   </si>
   <si>
-    <t>modules/HTTP Response.pdf</t>
-  </si>
-  <si>
     <t>2017-01-24</t>
   </si>
   <si>
@@ -1505,9 +1136,6 @@
     <t>EdgeworkModule</t>
   </si>
   <si>
-    <t>modules/Edgework.pdf</t>
-  </si>
-  <si>
     <t>Ion Lee, ZekNikZ</t>
   </si>
   <si>
@@ -1517,9 +1145,6 @@
     <t>EternitySDec</t>
   </si>
   <si>
-    <t>modules/Hex To Decimal.pdf</t>
-  </si>
-  <si>
     <t>EternityShack</t>
   </si>
   <si>
@@ -1532,9 +1157,6 @@
     <t>XRayModule</t>
   </si>
   <si>
-    <t>modules/X-Ray.pdf</t>
-  </si>
-  <si>
     <t>2017-07-14</t>
   </si>
   <si>
@@ -1544,9 +1166,6 @@
     <t>QRCode</t>
   </si>
   <si>
-    <t>modules/QR Code.pdf</t>
-  </si>
-  <si>
     <t>2017-07-17</t>
   </si>
   <si>
@@ -1556,9 +1175,6 @@
     <t>buttonMasherNeedy</t>
   </si>
   <si>
-    <t>modules/Button Masher.pdf</t>
-  </si>
-  <si>
     <t>McDude73</t>
   </si>
   <si>
@@ -1571,9 +1187,6 @@
     <t>rng</t>
   </si>
   <si>
-    <t>modules/Random Number Generator.pdf</t>
-  </si>
-  <si>
     <t>Lumbud84, McDude73</t>
   </si>
   <si>
@@ -1586,9 +1199,6 @@
     <t>ColorMorseModule</t>
   </si>
   <si>
-    <t>modules/Color Morse.pdf</t>
-  </si>
-  <si>
     <t>SKiPP, Ezekiel, ZekNikZ</t>
   </si>
   <si>
@@ -1598,9 +1208,6 @@
     <t>Mastermind Simple</t>
   </si>
   <si>
-    <t>modules/Mastermind Simple.pdf</t>
-  </si>
-  <si>
     <t>Eotall</t>
   </si>
   <si>
@@ -1610,18 +1217,12 @@
     <t>Mastermind Cruel</t>
   </si>
   <si>
-    <t>modules/Mastermind Cruel.pdf</t>
-  </si>
-  <si>
     <t>Gridlock</t>
   </si>
   <si>
     <t>GridlockModule</t>
   </si>
   <si>
-    <t>modules/Gridlock.pdf</t>
-  </si>
-  <si>
     <t>Elias, Timwi</t>
   </si>
   <si>
@@ -1634,9 +1235,6 @@
     <t>BigCircle</t>
   </si>
   <si>
-    <t>modules/Big Circle.pdf</t>
-  </si>
-  <si>
     <t>Ezekiel, Hendruid, CaitSith2</t>
   </si>
   <si>
@@ -1649,9 +1247,6 @@
     <t>MorseAMaze</t>
   </si>
   <si>
-    <t>modules/Morse-A-Maze.pdf</t>
-  </si>
-  <si>
     <t>CaitSith2</t>
   </si>
   <si>
@@ -1664,9 +1259,6 @@
     <t>ColoredSwitchesModule</t>
   </si>
   <si>
-    <t>modules/Colored Switches.pdf</t>
-  </si>
-  <si>
     <t>2017-09-03</t>
   </si>
   <si>
@@ -1676,9 +1268,6 @@
     <t>PerplexingWiresModule</t>
   </si>
   <si>
-    <t>modules/Perplexing Wires.pdf</t>
-  </si>
-  <si>
     <t>MarAyzex, Ezekiel, Timwi</t>
   </si>
   <si>
@@ -1691,9 +1280,6 @@
     <t>monsplodeCards</t>
   </si>
   <si>
-    <t>modules/Monsplode Trading Cards.pdf</t>
-  </si>
-  <si>
     <t>clutterArranger, Grybo</t>
   </si>
   <si>
@@ -1709,12 +1295,6 @@
     <t>GameOfLifeCruel</t>
   </si>
   <si>
-    <t>modules/Game Of Life Simple.pdf</t>
-  </si>
-  <si>
-    <t>modules/Game Of Life Cruel.pdf</t>
-  </si>
-  <si>
     <t>Eotall, WarioLGP, samfun123</t>
   </si>
   <si>
@@ -1727,9 +1307,6 @@
     <t>NonogramModule</t>
   </si>
   <si>
-    <t>modules/Nonogram.pdf</t>
-  </si>
-  <si>
     <t>Piggered</t>
   </si>
   <si>
@@ -1745,18 +1322,12 @@
     <t>SetModule</t>
   </si>
   <si>
-    <t>modules/SET.pdf</t>
-  </si>
-  <si>
     <t>Zawu, Timwi</t>
   </si>
   <si>
     <t>Painting</t>
   </si>
   <si>
-    <t>modules/Painting.pdf</t>
-  </si>
-  <si>
     <t>Hendruid, Bashly</t>
   </si>
   <si>
@@ -1766,18 +1337,12 @@
     <t>Color Generator</t>
   </si>
   <si>
-    <t>modules/Color Generator.pdf</t>
-  </si>
-  <si>
     <t>Shape Memory</t>
   </si>
   <si>
     <t>needyShapeMemory</t>
   </si>
   <si>
-    <t>modules/Shape Memory.pdf</t>
-  </si>
-  <si>
     <t>UltraCboy</t>
   </si>
   <si>
@@ -1790,9 +1355,6 @@
     <t>SymbolCycleModule</t>
   </si>
   <si>
-    <t>modules/Symbol Cycle.pdf</t>
-  </si>
-  <si>
     <t>2017-10-05</t>
   </si>
   <si>
@@ -1802,9 +1364,6 @@
     <t>hunting</t>
   </si>
   <si>
-    <t>modules/Hunting.pdf</t>
-  </si>
-  <si>
     <t>taggedjc</t>
   </si>
   <si>
@@ -1817,9 +1376,6 @@
     <t>ExtendedPassword</t>
   </si>
   <si>
-    <t>modules/Extended Password.pdf</t>
-  </si>
-  <si>
     <t>taggedjc, TWGaming</t>
   </si>
   <si>
@@ -1832,9 +1388,6 @@
     <t>curriculum</t>
   </si>
   <si>
-    <t>modules/Curriculum.pdf</t>
-  </si>
-  <si>
     <t>Fixdoll</t>
   </si>
   <si>
@@ -1847,9 +1400,6 @@
     <t>BrailleModule</t>
   </si>
   <si>
-    <t>modules/Braille.pdf</t>
-  </si>
-  <si>
     <t>2017-10-31</t>
   </si>
   <si>
@@ -1859,9 +1409,6 @@
     <t>MafiaModule</t>
   </si>
   <si>
-    <t>modules/Mafia.pdf</t>
-  </si>
-  <si>
     <t>MarioXTurn, Ezekiel, Timwi</t>
   </si>
   <si>
@@ -1874,9 +1421,6 @@
     <t>FestivePianoKeys</t>
   </si>
   <si>
-    <t>modules/Festive Piano Keys.pdf</t>
-  </si>
-  <si>
     <t>2017-12-07</t>
   </si>
   <si>
@@ -1886,9 +1430,6 @@
     <t>FlagsModule</t>
   </si>
   <si>
-    <t>modules/Flags.pdf</t>
-  </si>
-  <si>
     <t>Monopoly, Piggered</t>
   </si>
   <si>
@@ -1901,23 +1442,490 @@
     <t>timezone</t>
   </si>
   <si>
-    <t>modules/Timezone.pdf</t>
-  </si>
-  <si>
     <t>federan</t>
   </si>
   <si>
     <t>2017-12-30</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Colour%20Flash.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Piano%20Keys.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Semaphore.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Emoji%20Math.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Switches.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Two%20Bits.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Anagrams.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Word%20Scramble.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Combination%20Lock.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Square%20Button.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Simon%20States.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Round%20Keypad.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Listening.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Foreign%20Exchange%20Rates.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Orientation%20Cube.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Morsematics.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Connection%20Check.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Letter%20Keys.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Forget%20Me%20Not.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Astrology.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Logic.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Crazy%20Talk.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Adventure%20Game.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Turn%20The%20Key.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Turn%20The%20Keys.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Mystic%20Square.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Plumbing.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Safety%20Safe.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Cryptography.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Chess.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Mouse%20In%20The%20Maze.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/3D%20Maze.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Silly%20Slots.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Number%20Pad.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Laundry.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Probing.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Resistors.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Skewed%20Slots.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Caesar%20Cipher.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Perspective%20Pegs.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Microcontroller.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Murder.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/The%20Gamepad.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Tic-Tac-Toe.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Monsplode%2C%20Fight!.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Shape%20Shift.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Follow%20the%20Leader.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Friendship.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/The%20Bulb.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Alphabet.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Blind%20Alley.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Sea%20Shells.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/English%20Test.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Rock-Paper-Scissors-Lizard-Spock.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Hexamaze.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Bitmaps.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Colored%20Squares.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Adjacent%20Letters.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Third%20Base.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Souvenir.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Word%20Search.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Broken%20Buttons.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Simon%20Screams.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Modules%20Against%20Humanity.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Complicated%20Buttons.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Battleship.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Text%20Field.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Symbolic%20Password.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Wire%20Placement.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Double-Oh.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Cheap%20Checkout.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Coordinates.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Light%20Cycle.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Rhythms.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Color%20Math.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Only%20Connect.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Neutralization.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Web%20Design.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Chord%20Qualities.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Creation.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Rubik%E2%80%99s%20Cube.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/FizzBuzz.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/The%20Clock.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/LED%20Encryption.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Bitwise%20Operations.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Fast%20Math.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Minesweeper.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Zoo.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Binary%20LEDs.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Boolean%20Venn%20Diagram.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Point%20of%20Order.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Ice%20Cream.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/The%20Screw.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Yahtzee.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/The%20Button%20translated%20(Deutsch%20%E2%80%94%20Der%20Knopf).pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Morse%20Code%20translated%20(Deutsch%20%E2%80%94%20Morsecode).pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Password%20translated%20(Deutsch%20%E2%80%94%20Passw%C3%B6rter).pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Who%E2%80%99s%20on%20First%20translated%20(Deutsch%20%E2%80%94%20Who%E2%80%99s%20on%20First).pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Wires.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/The%20Button.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Keypad.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Simon%20Says.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Who%E2%80%99s%20on%20First.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Memory.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Morse%20Code.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Complicated%20Wires.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Wire%20Sequence.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Maze.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Password.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Capacitor%20Discharge.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Knob.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Venting%20Gas.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Refill%20that%20Beer!.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Math.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Lights%20Out.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Filibuster.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Motion%20Sense.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Answering%20Questions.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Rotary%20Phone.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Cruel%20Piano%20Keys.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Tetris.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Who%E2%80%99s%20That%20Monsplode.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/HTTP%20Response.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Edgework.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Hex%20To%20Decimal.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/X-Ray.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/QR%20Code.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Button%20Masher.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Random%20Number%20Generator.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Color%20Morse.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Mastermind%20Simple.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Mastermind%20Cruel.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Gridlock.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Big%20Circle.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Morse-A-Maze.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Colored%20Switches.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Perplexing%20Wires.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Monsplode%20Trading%20Cards.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Game%20of%20Life%20Simple.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Game%20of%20Life%20Cruel.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Nonogram.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/S.E.T..pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Painting.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Color%20Generator.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Shape%20Memory.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Symbol%20Cycle.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Hunting.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Extended%20Password.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Curriculum.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Braille.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Mafia.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Festive%20Piano%20Keys.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Flags.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Timezone.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1940,14 +1948,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2262,8 +2273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC09710-E84E-49A6-94A5-EB5A61B7898A}">
   <dimension ref="A1:G155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="72" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156"/>
+    <sheetView tabSelected="1" topLeftCell="C136" zoomScale="72" workbookViewId="0">
+      <selection activeCell="E154" sqref="E154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2287,8 +2298,8 @@
       <c r="C1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>308</v>
+      <c r="D1" s="2" t="s">
+        <v>471</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -2310,8 +2321,8 @@
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>309</v>
+      <c r="D2" s="2" t="s">
+        <v>472</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -2333,8 +2344,8 @@
       <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>310</v>
+      <c r="D3" s="2" t="s">
+        <v>473</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -2356,8 +2367,8 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>311</v>
+      <c r="D4" s="2" t="s">
+        <v>474</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -2380,7 +2391,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>312</v>
+        <v>475</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -2403,7 +2414,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>313</v>
+        <v>476</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
@@ -2426,7 +2437,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>314</v>
+        <v>477</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -2449,7 +2460,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>315</v>
+        <v>478</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -2472,7 +2483,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>316</v>
+        <v>479</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -2495,7 +2506,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>317</v>
+        <v>480</v>
       </c>
       <c r="E10" t="s">
         <v>30</v>
@@ -2518,7 +2529,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>318</v>
+        <v>481</v>
       </c>
       <c r="E11" t="s">
         <v>30</v>
@@ -2541,7 +2552,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>319</v>
+        <v>482</v>
       </c>
       <c r="E12" t="s">
         <v>30</v>
@@ -2564,7 +2575,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>320</v>
+        <v>483</v>
       </c>
       <c r="E13" t="s">
         <v>37</v>
@@ -2587,7 +2598,7 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>321</v>
+        <v>484</v>
       </c>
       <c r="E14" t="s">
         <v>37</v>
@@ -2610,7 +2621,7 @@
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>322</v>
+        <v>485</v>
       </c>
       <c r="E15" t="s">
         <v>37</v>
@@ -2633,7 +2644,7 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>323</v>
+        <v>486</v>
       </c>
       <c r="E16" t="s">
         <v>30</v>
@@ -2656,7 +2667,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>324</v>
+        <v>487</v>
       </c>
       <c r="E17" t="s">
         <v>47</v>
@@ -2679,7 +2690,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>325</v>
+        <v>488</v>
       </c>
       <c r="E18" t="s">
         <v>50</v>
@@ -2702,7 +2713,7 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>326</v>
+        <v>489</v>
       </c>
       <c r="E19" t="s">
         <v>30</v>
@@ -2724,8 +2735,8 @@
       <c r="C20">
         <v>3</v>
       </c>
-      <c r="D20" t="s">
-        <v>327</v>
+      <c r="D20" s="2" t="s">
+        <v>490</v>
       </c>
       <c r="E20" t="s">
         <v>56</v>
@@ -2748,7 +2759,7 @@
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>328</v>
+        <v>491</v>
       </c>
       <c r="E21" t="s">
         <v>59</v>
@@ -2771,7 +2782,7 @@
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>329</v>
+        <v>492</v>
       </c>
       <c r="E22" t="s">
         <v>37</v>
@@ -2794,7 +2805,7 @@
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>330</v>
+        <v>493</v>
       </c>
       <c r="E23" t="s">
         <v>56</v>
@@ -2817,7 +2828,7 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>331</v>
+        <v>494</v>
       </c>
       <c r="E24" t="s">
         <v>37</v>
@@ -2840,7 +2851,7 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>332</v>
+        <v>495</v>
       </c>
       <c r="E25" t="s">
         <v>37</v>
@@ -2863,7 +2874,7 @@
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>333</v>
+        <v>496</v>
       </c>
       <c r="E26" t="s">
         <v>73</v>
@@ -2886,7 +2897,7 @@
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>334</v>
+        <v>497</v>
       </c>
       <c r="E27" t="s">
         <v>30</v>
@@ -2909,7 +2920,7 @@
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>335</v>
+        <v>498</v>
       </c>
       <c r="E28" t="s">
         <v>30</v>
@@ -2932,7 +2943,7 @@
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>336</v>
+        <v>499</v>
       </c>
       <c r="E29" t="s">
         <v>37</v>
@@ -2955,7 +2966,7 @@
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>337</v>
+        <v>500</v>
       </c>
       <c r="E30" t="s">
         <v>85</v>
@@ -2978,7 +2989,7 @@
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>338</v>
+        <v>501</v>
       </c>
       <c r="E31" t="s">
         <v>73</v>
@@ -3001,7 +3012,7 @@
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>339</v>
+        <v>502</v>
       </c>
       <c r="E32" t="s">
         <v>56</v>
@@ -3024,7 +3035,7 @@
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>340</v>
+        <v>503</v>
       </c>
       <c r="E33" t="s">
         <v>37</v>
@@ -3047,7 +3058,7 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>341</v>
+        <v>504</v>
       </c>
       <c r="E34" t="s">
         <v>96</v>
@@ -3070,7 +3081,7 @@
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>342</v>
+        <v>505</v>
       </c>
       <c r="E35" t="s">
         <v>99</v>
@@ -3093,7 +3104,7 @@
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>343</v>
+        <v>506</v>
       </c>
       <c r="E36" t="s">
         <v>37</v>
@@ -3116,7 +3127,7 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>344</v>
+        <v>507</v>
       </c>
       <c r="E37" t="s">
         <v>217</v>
@@ -3139,7 +3150,7 @@
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>345</v>
+        <v>508</v>
       </c>
       <c r="E38" t="s">
         <v>219</v>
@@ -3162,7 +3173,7 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>346</v>
+        <v>509</v>
       </c>
       <c r="E39" t="s">
         <v>221</v>
@@ -3185,7 +3196,7 @@
         <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>347</v>
+        <v>510</v>
       </c>
       <c r="E40" t="s">
         <v>56</v>
@@ -3208,7 +3219,7 @@
         <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>348</v>
+        <v>511</v>
       </c>
       <c r="E41" t="s">
         <v>224</v>
@@ -3231,7 +3242,7 @@
         <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>349</v>
+        <v>512</v>
       </c>
       <c r="E42" t="s">
         <v>225</v>
@@ -3254,7 +3265,7 @@
         <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>405</v>
+        <v>513</v>
       </c>
       <c r="E43" t="s">
         <v>227</v>
@@ -3277,7 +3288,7 @@
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>350</v>
+        <v>514</v>
       </c>
       <c r="E44" t="s">
         <v>229</v>
@@ -3300,7 +3311,7 @@
         <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>406</v>
+        <v>515</v>
       </c>
       <c r="E45" t="s">
         <v>47</v>
@@ -3323,7 +3334,7 @@
         <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>351</v>
+        <v>516</v>
       </c>
       <c r="E46" t="s">
         <v>225</v>
@@ -3346,7 +3357,7 @@
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>352</v>
+        <v>517</v>
       </c>
       <c r="E47" t="s">
         <v>233</v>
@@ -3369,7 +3380,7 @@
         <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>353</v>
+        <v>518</v>
       </c>
       <c r="E48" t="s">
         <v>235</v>
@@ -3392,7 +3403,7 @@
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>354</v>
+        <v>519</v>
       </c>
       <c r="E49" t="s">
         <v>235</v>
@@ -3415,7 +3426,7 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>355</v>
+        <v>520</v>
       </c>
       <c r="E50" t="s">
         <v>96</v>
@@ -3438,7 +3449,7 @@
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>356</v>
+        <v>521</v>
       </c>
       <c r="E51" t="s">
         <v>235</v>
@@ -3461,7 +3472,7 @@
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>357</v>
+        <v>522</v>
       </c>
       <c r="E52" t="s">
         <v>225</v>
@@ -3484,7 +3495,7 @@
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>358</v>
+        <v>523</v>
       </c>
       <c r="E53" t="s">
         <v>241</v>
@@ -3507,7 +3518,7 @@
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>359</v>
+        <v>524</v>
       </c>
       <c r="E54" t="s">
         <v>235</v>
@@ -3530,7 +3541,7 @@
         <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>360</v>
+        <v>525</v>
       </c>
       <c r="E55" t="s">
         <v>235</v>
@@ -3553,7 +3564,7 @@
         <v>4</v>
       </c>
       <c r="D56" t="s">
-        <v>361</v>
+        <v>526</v>
       </c>
       <c r="E56" t="s">
         <v>244</v>
@@ -3576,7 +3587,7 @@
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>362</v>
+        <v>527</v>
       </c>
       <c r="E57" t="s">
         <v>233</v>
@@ -3599,7 +3610,7 @@
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>363</v>
+        <v>528</v>
       </c>
       <c r="E58" t="s">
         <v>247</v>
@@ -3622,7 +3633,7 @@
         <v>4</v>
       </c>
       <c r="D59" t="s">
-        <v>364</v>
+        <v>529</v>
       </c>
       <c r="E59" t="s">
         <v>225</v>
@@ -3645,7 +3656,7 @@
         <v>4</v>
       </c>
       <c r="D60" t="s">
-        <v>365</v>
+        <v>530</v>
       </c>
       <c r="E60" t="s">
         <v>250</v>
@@ -3668,7 +3679,7 @@
         <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>366</v>
+        <v>531</v>
       </c>
       <c r="E61" t="s">
         <v>233</v>
@@ -3691,7 +3702,7 @@
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>367</v>
+        <v>532</v>
       </c>
       <c r="E62" t="s">
         <v>219</v>
@@ -3714,7 +3725,7 @@
         <v>4</v>
       </c>
       <c r="D63" t="s">
-        <v>368</v>
+        <v>533</v>
       </c>
       <c r="E63" t="s">
         <v>235</v>
@@ -3737,7 +3748,7 @@
         <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>369</v>
+        <v>534</v>
       </c>
       <c r="E64" t="s">
         <v>255</v>
@@ -3760,7 +3771,7 @@
         <v>2</v>
       </c>
       <c r="D65" t="s">
-        <v>370</v>
+        <v>535</v>
       </c>
       <c r="E65" t="s">
         <v>257</v>
@@ -3783,7 +3794,7 @@
         <v>4</v>
       </c>
       <c r="D66" t="s">
-        <v>371</v>
+        <v>536</v>
       </c>
       <c r="E66" t="s">
         <v>235</v>
@@ -3806,7 +3817,7 @@
         <v>2</v>
       </c>
       <c r="D67" t="s">
-        <v>372</v>
+        <v>537</v>
       </c>
       <c r="E67" t="s">
         <v>59</v>
@@ -3829,7 +3840,7 @@
         <v>2</v>
       </c>
       <c r="D68" t="s">
-        <v>373</v>
+        <v>538</v>
       </c>
       <c r="E68" t="s">
         <v>257</v>
@@ -3851,8 +3862,8 @@
       <c r="C69">
         <v>2</v>
       </c>
-      <c r="D69" t="s">
-        <v>374</v>
+      <c r="D69" s="2" t="s">
+        <v>539</v>
       </c>
       <c r="E69" t="s">
         <v>247</v>
@@ -3875,7 +3886,7 @@
         <v>2</v>
       </c>
       <c r="D70" t="s">
-        <v>375</v>
+        <v>540</v>
       </c>
       <c r="E70" t="s">
         <v>257</v>
@@ -3898,7 +3909,7 @@
         <v>4</v>
       </c>
       <c r="D71" t="s">
-        <v>376</v>
+        <v>541</v>
       </c>
       <c r="E71" t="s">
         <v>219</v>
@@ -3921,7 +3932,7 @@
         <v>4</v>
       </c>
       <c r="D72" t="s">
-        <v>377</v>
+        <v>542</v>
       </c>
       <c r="E72" t="s">
         <v>235</v>
@@ -3944,7 +3955,7 @@
         <v>4</v>
       </c>
       <c r="D73" t="s">
-        <v>378</v>
+        <v>543</v>
       </c>
       <c r="E73" t="s">
         <v>265</v>
@@ -3967,7 +3978,7 @@
         <v>3</v>
       </c>
       <c r="D74" t="s">
-        <v>379</v>
+        <v>544</v>
       </c>
       <c r="E74" t="s">
         <v>267</v>
@@ -3990,7 +4001,7 @@
         <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>380</v>
+        <v>545</v>
       </c>
       <c r="E75" t="s">
         <v>59</v>
@@ -4013,7 +4024,7 @@
         <v>4</v>
       </c>
       <c r="D76" t="s">
-        <v>381</v>
+        <v>546</v>
       </c>
       <c r="E76" t="s">
         <v>235</v>
@@ -4036,7 +4047,7 @@
         <v>4</v>
       </c>
       <c r="D77" t="s">
-        <v>382</v>
+        <v>547</v>
       </c>
       <c r="E77" t="s">
         <v>270</v>
@@ -4059,7 +4070,7 @@
         <v>4</v>
       </c>
       <c r="D78" t="s">
-        <v>383</v>
+        <v>548</v>
       </c>
       <c r="E78" t="s">
         <v>272</v>
@@ -4082,7 +4093,7 @@
         <v>4</v>
       </c>
       <c r="D79" t="s">
-        <v>384</v>
+        <v>549</v>
       </c>
       <c r="E79" t="s">
         <v>267</v>
@@ -4105,7 +4116,7 @@
         <v>3</v>
       </c>
       <c r="D80" t="s">
-        <v>385</v>
+        <v>550</v>
       </c>
       <c r="E80" t="s">
         <v>275</v>
@@ -4128,7 +4139,7 @@
         <v>4</v>
       </c>
       <c r="D81" t="s">
-        <v>386</v>
+        <v>551</v>
       </c>
       <c r="E81" t="s">
         <v>277</v>
@@ -4151,7 +4162,7 @@
         <v>4</v>
       </c>
       <c r="D82" t="s">
-        <v>387</v>
+        <v>552</v>
       </c>
       <c r="E82" t="s">
         <v>257</v>
@@ -4174,7 +4185,7 @@
         <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>388</v>
+        <v>553</v>
       </c>
       <c r="E83" t="s">
         <v>233</v>
@@ -4197,7 +4208,7 @@
         <v>3</v>
       </c>
       <c r="D84" t="s">
-        <v>389</v>
+        <v>554</v>
       </c>
       <c r="E84" t="s">
         <v>281</v>
@@ -4220,7 +4231,7 @@
         <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>390</v>
+        <v>555</v>
       </c>
       <c r="E85" t="s">
         <v>281</v>
@@ -4243,7 +4254,7 @@
         <v>4</v>
       </c>
       <c r="D86" t="s">
-        <v>391</v>
+        <v>556</v>
       </c>
       <c r="E86" t="s">
         <v>284</v>
@@ -4266,7 +4277,7 @@
         <v>2</v>
       </c>
       <c r="D87" t="s">
-        <v>392</v>
+        <v>557</v>
       </c>
       <c r="E87" t="s">
         <v>219</v>
@@ -4289,7 +4300,7 @@
         <v>4</v>
       </c>
       <c r="D88" t="s">
-        <v>393</v>
+        <v>558</v>
       </c>
       <c r="E88" t="s">
         <v>235</v>
@@ -4312,7 +4323,7 @@
         <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>394</v>
+        <v>559</v>
       </c>
       <c r="E89" t="s">
         <v>288</v>
@@ -4326,7 +4337,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>403</v>
+        <v>308</v>
       </c>
       <c r="B90" t="s">
         <v>155</v>
@@ -4335,7 +4346,7 @@
         <v>4</v>
       </c>
       <c r="D90" t="s">
-        <v>404</v>
+        <v>560</v>
       </c>
       <c r="E90" t="s">
         <v>257</v>
@@ -4358,7 +4369,7 @@
         <v>4</v>
       </c>
       <c r="D91" t="s">
-        <v>395</v>
+        <v>561</v>
       </c>
       <c r="E91" t="s">
         <v>235</v>
@@ -4381,7 +4392,7 @@
         <v>3</v>
       </c>
       <c r="D92" t="s">
-        <v>396</v>
+        <v>562</v>
       </c>
       <c r="E92" t="s">
         <v>292</v>
@@ -4404,7 +4415,7 @@
         <v>3</v>
       </c>
       <c r="D93" t="s">
-        <v>397</v>
+        <v>563</v>
       </c>
       <c r="E93" t="s">
         <v>294</v>
@@ -4427,7 +4438,7 @@
         <v>3</v>
       </c>
       <c r="D94" t="s">
-        <v>398</v>
+        <v>564</v>
       </c>
       <c r="E94" t="s">
         <v>296</v>
@@ -4449,8 +4460,8 @@
       <c r="C95">
         <v>1</v>
       </c>
-      <c r="D95" t="s">
-        <v>399</v>
+      <c r="D95" s="2" t="s">
+        <v>565</v>
       </c>
       <c r="E95" t="s">
         <v>300</v>
@@ -4473,7 +4484,7 @@
         <v>2</v>
       </c>
       <c r="D96" t="s">
-        <v>400</v>
+        <v>566</v>
       </c>
       <c r="E96" t="s">
         <v>300</v>
@@ -4496,7 +4507,7 @@
         <v>2</v>
       </c>
       <c r="D97" t="s">
-        <v>401</v>
+        <v>567</v>
       </c>
       <c r="E97" t="s">
         <v>300</v>
@@ -4519,7 +4530,7 @@
         <v>2</v>
       </c>
       <c r="D98" t="s">
-        <v>402</v>
+        <v>568</v>
       </c>
       <c r="E98" t="s">
         <v>300</v>
@@ -4533,22 +4544,22 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>407</v>
+        <v>309</v>
       </c>
       <c r="B99" t="s">
-        <v>407</v>
+        <v>309</v>
       </c>
       <c r="C99">
         <v>1</v>
       </c>
       <c r="D99" t="s">
-        <v>408</v>
+        <v>569</v>
       </c>
       <c r="E99" t="s">
-        <v>409</v>
+        <v>310</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>410</v>
+        <v>311</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -4556,22 +4567,22 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>411</v>
+        <v>312</v>
       </c>
       <c r="B100" t="s">
-        <v>412</v>
+        <v>313</v>
       </c>
       <c r="C100">
         <v>1</v>
       </c>
       <c r="D100" t="s">
-        <v>413</v>
+        <v>570</v>
       </c>
       <c r="E100" t="s">
-        <v>409</v>
+        <v>310</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>410</v>
+        <v>311</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -4579,22 +4590,22 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>414</v>
+        <v>314</v>
       </c>
       <c r="B101" t="s">
-        <v>414</v>
+        <v>314</v>
       </c>
       <c r="C101">
         <v>2</v>
       </c>
       <c r="D101" t="s">
-        <v>415</v>
+        <v>571</v>
       </c>
       <c r="E101" t="s">
-        <v>409</v>
+        <v>310</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>410</v>
+        <v>311</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -4602,22 +4613,22 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>416</v>
+        <v>315</v>
       </c>
       <c r="B102" t="s">
-        <v>417</v>
+        <v>316</v>
       </c>
       <c r="C102">
         <v>1</v>
       </c>
-      <c r="D102" t="s">
-        <v>418</v>
+      <c r="D102" s="2" t="s">
+        <v>572</v>
       </c>
       <c r="E102" t="s">
-        <v>409</v>
+        <v>310</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>410</v>
+        <v>311</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -4625,22 +4636,22 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>419</v>
+        <v>317</v>
       </c>
       <c r="B103" t="s">
-        <v>420</v>
+        <v>318</v>
       </c>
       <c r="C103">
         <v>2</v>
       </c>
       <c r="D103" t="s">
-        <v>421</v>
+        <v>573</v>
       </c>
       <c r="E103" t="s">
-        <v>409</v>
+        <v>310</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>410</v>
+        <v>311</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -4648,22 +4659,22 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>422</v>
+        <v>319</v>
       </c>
       <c r="B104" t="s">
-        <v>422</v>
+        <v>319</v>
       </c>
       <c r="C104">
         <v>2</v>
       </c>
       <c r="D104" t="s">
-        <v>423</v>
+        <v>574</v>
       </c>
       <c r="E104" t="s">
-        <v>409</v>
+        <v>310</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>410</v>
+        <v>311</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -4671,22 +4682,22 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>424</v>
+        <v>320</v>
       </c>
       <c r="B105" t="s">
-        <v>425</v>
+        <v>321</v>
       </c>
       <c r="C105">
         <v>3</v>
       </c>
       <c r="D105" t="s">
-        <v>426</v>
+        <v>575</v>
       </c>
       <c r="E105" t="s">
-        <v>409</v>
+        <v>310</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>410</v>
+        <v>311</v>
       </c>
       <c r="G105">
         <v>0</v>
@@ -4694,22 +4705,22 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>427</v>
+        <v>322</v>
       </c>
       <c r="B106" t="s">
-        <v>428</v>
+        <v>323</v>
       </c>
       <c r="C106">
         <v>3</v>
       </c>
-      <c r="D106" t="s">
-        <v>429</v>
+      <c r="D106" s="2" t="s">
+        <v>576</v>
       </c>
       <c r="E106" t="s">
-        <v>409</v>
+        <v>310</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>410</v>
+        <v>311</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -4717,22 +4728,22 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>430</v>
+        <v>324</v>
       </c>
       <c r="B107" t="s">
-        <v>431</v>
+        <v>325</v>
       </c>
       <c r="C107">
         <v>3</v>
       </c>
       <c r="D107" t="s">
-        <v>432</v>
+        <v>577</v>
       </c>
       <c r="E107" t="s">
-        <v>409</v>
+        <v>310</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>410</v>
+        <v>311</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -4740,22 +4751,22 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>433</v>
+        <v>326</v>
       </c>
       <c r="B108" t="s">
-        <v>433</v>
+        <v>326</v>
       </c>
       <c r="C108">
         <v>2</v>
       </c>
       <c r="D108" t="s">
-        <v>434</v>
+        <v>578</v>
       </c>
       <c r="E108" t="s">
-        <v>409</v>
+        <v>310</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>410</v>
+        <v>311</v>
       </c>
       <c r="G108">
         <v>0</v>
@@ -4763,22 +4774,22 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>435</v>
+        <v>327</v>
       </c>
       <c r="B109" t="s">
-        <v>435</v>
+        <v>327</v>
       </c>
       <c r="C109">
         <v>2</v>
       </c>
-      <c r="D109" t="s">
-        <v>436</v>
+      <c r="D109" s="2" t="s">
+        <v>579</v>
       </c>
       <c r="E109" t="s">
-        <v>409</v>
+        <v>310</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>410</v>
+        <v>311</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -4786,22 +4797,22 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>437</v>
+        <v>328</v>
       </c>
       <c r="B110" t="s">
-        <v>438</v>
+        <v>329</v>
       </c>
       <c r="C110">
         <v>1</v>
       </c>
       <c r="D110" t="s">
-        <v>439</v>
+        <v>580</v>
       </c>
       <c r="E110" t="s">
-        <v>409</v>
+        <v>310</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>410</v>
+        <v>311</v>
       </c>
       <c r="G110">
         <v>2</v>
@@ -4809,22 +4820,22 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>440</v>
+        <v>330</v>
       </c>
       <c r="B111" t="s">
-        <v>441</v>
+        <v>331</v>
       </c>
       <c r="C111">
         <v>1</v>
       </c>
       <c r="D111" t="s">
-        <v>442</v>
+        <v>581</v>
       </c>
       <c r="E111" t="s">
-        <v>409</v>
+        <v>310</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>410</v>
+        <v>311</v>
       </c>
       <c r="G111">
         <v>2</v>
@@ -4832,22 +4843,22 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>443</v>
+        <v>332</v>
       </c>
       <c r="B112" t="s">
-        <v>444</v>
+        <v>333</v>
       </c>
       <c r="C112">
         <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>445</v>
+        <v>582</v>
       </c>
       <c r="E112" t="s">
-        <v>409</v>
+        <v>310</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>410</v>
+        <v>311</v>
       </c>
       <c r="G112">
         <v>2</v>
@@ -4855,16 +4866,16 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>446</v>
+        <v>334</v>
       </c>
       <c r="B113" t="s">
-        <v>447</v>
+        <v>335</v>
       </c>
       <c r="C113">
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>448</v>
+        <v>336</v>
       </c>
       <c r="E113" t="s">
         <v>300</v>
@@ -4878,22 +4889,22 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>449</v>
+        <v>337</v>
       </c>
       <c r="B114" t="s">
-        <v>450</v>
+        <v>338</v>
       </c>
       <c r="C114">
         <v>1</v>
       </c>
       <c r="D114" t="s">
-        <v>453</v>
+        <v>583</v>
       </c>
       <c r="E114" t="s">
-        <v>451</v>
+        <v>339</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>452</v>
+        <v>340</v>
       </c>
       <c r="G114">
         <v>2</v>
@@ -4901,16 +4912,16 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>454</v>
+        <v>341</v>
       </c>
       <c r="B115" t="s">
-        <v>455</v>
+        <v>342</v>
       </c>
       <c r="C115">
         <v>1</v>
       </c>
       <c r="D115" t="s">
-        <v>456</v>
+        <v>584</v>
       </c>
       <c r="E115" t="s">
         <v>10</v>
@@ -4924,22 +4935,22 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>457</v>
+        <v>343</v>
       </c>
       <c r="B116" t="s">
-        <v>458</v>
+        <v>344</v>
       </c>
       <c r="C116">
         <v>1</v>
       </c>
       <c r="D116" t="s">
-        <v>459</v>
+        <v>585</v>
       </c>
       <c r="E116" t="s">
         <v>2</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>460</v>
+        <v>345</v>
       </c>
       <c r="G116">
         <v>2</v>
@@ -4947,22 +4958,22 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>461</v>
+        <v>346</v>
       </c>
       <c r="B117" t="s">
-        <v>461</v>
+        <v>346</v>
       </c>
       <c r="C117">
         <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>462</v>
+        <v>586</v>
       </c>
       <c r="E117" t="s">
         <v>10</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>463</v>
+        <v>347</v>
       </c>
       <c r="G117">
         <v>2</v>
@@ -4970,22 +4981,22 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>464</v>
+        <v>348</v>
       </c>
       <c r="B118" t="s">
-        <v>465</v>
+        <v>349</v>
       </c>
       <c r="C118">
         <v>1</v>
       </c>
       <c r="D118" t="s">
-        <v>466</v>
+        <v>587</v>
       </c>
       <c r="E118" t="s">
         <v>2</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>467</v>
+        <v>350</v>
       </c>
       <c r="G118">
         <v>2</v>
@@ -4993,16 +5004,16 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>468</v>
+        <v>351</v>
       </c>
       <c r="B119" t="s">
-        <v>469</v>
+        <v>352</v>
       </c>
       <c r="C119">
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>470</v>
+        <v>588</v>
       </c>
       <c r="E119" t="s">
         <v>30</v>
@@ -5016,16 +5027,16 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>471</v>
+        <v>353</v>
       </c>
       <c r="B120" t="s">
-        <v>472</v>
+        <v>354</v>
       </c>
       <c r="C120">
         <v>2</v>
       </c>
       <c r="D120" t="s">
-        <v>473</v>
+        <v>589</v>
       </c>
       <c r="E120" t="s">
         <v>30</v>
@@ -5039,16 +5050,16 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>474</v>
+        <v>355</v>
       </c>
       <c r="B121" t="s">
-        <v>475</v>
+        <v>356</v>
       </c>
       <c r="C121">
         <v>4</v>
       </c>
       <c r="D121" t="s">
-        <v>476</v>
+        <v>590</v>
       </c>
       <c r="E121" t="s">
         <v>2</v>
@@ -5062,22 +5073,22 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>477</v>
+        <v>357</v>
       </c>
       <c r="B122" t="s">
-        <v>478</v>
+        <v>358</v>
       </c>
       <c r="C122">
         <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>479</v>
+        <v>591</v>
       </c>
       <c r="E122" t="s">
         <v>56</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>480</v>
+        <v>359</v>
       </c>
       <c r="G122">
         <v>2</v>
@@ -5085,16 +5096,16 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>481</v>
+        <v>360</v>
       </c>
       <c r="B123" t="s">
-        <v>482</v>
+        <v>361</v>
       </c>
       <c r="C123">
         <v>2</v>
       </c>
-      <c r="D123" t="s">
-        <v>483</v>
+      <c r="D123" s="2" t="s">
+        <v>592</v>
       </c>
       <c r="E123" t="s">
         <v>47</v>
@@ -5108,22 +5119,22 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>484</v>
+        <v>362</v>
       </c>
       <c r="B124" t="s">
-        <v>485</v>
+        <v>363</v>
       </c>
       <c r="C124">
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>486</v>
+        <v>593</v>
       </c>
       <c r="E124" t="s">
         <v>59</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>487</v>
+        <v>364</v>
       </c>
       <c r="G124">
         <v>2</v>
@@ -5131,19 +5142,19 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>488</v>
+        <v>365</v>
       </c>
       <c r="B125" t="s">
-        <v>489</v>
+        <v>366</v>
       </c>
       <c r="C125">
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>490</v>
+        <v>594</v>
       </c>
       <c r="E125" t="s">
-        <v>491</v>
+        <v>367</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>283</v>
@@ -5154,22 +5165,22 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>492</v>
+        <v>368</v>
       </c>
       <c r="B126" t="s">
-        <v>493</v>
+        <v>369</v>
       </c>
       <c r="C126">
         <v>3</v>
       </c>
       <c r="D126" t="s">
-        <v>494</v>
+        <v>595</v>
       </c>
       <c r="E126" t="s">
-        <v>495</v>
+        <v>370</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>496</v>
+        <v>371</v>
       </c>
       <c r="G126">
         <v>2</v>
@@ -5177,22 +5188,22 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>497</v>
+        <v>372</v>
       </c>
       <c r="B127" t="s">
-        <v>498</v>
+        <v>373</v>
       </c>
       <c r="C127">
         <v>2</v>
       </c>
       <c r="D127" t="s">
-        <v>499</v>
+        <v>596</v>
       </c>
       <c r="E127" t="s">
         <v>235</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>500</v>
+        <v>374</v>
       </c>
       <c r="G127">
         <v>1</v>
@@ -5200,22 +5211,22 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>501</v>
+        <v>375</v>
       </c>
       <c r="B128" t="s">
-        <v>502</v>
+        <v>376</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
-      <c r="D128" t="s">
-        <v>503</v>
+      <c r="D128" s="2" t="s">
+        <v>597</v>
       </c>
       <c r="E128" t="s">
         <v>59</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>504</v>
+        <v>377</v>
       </c>
       <c r="G128">
         <v>2</v>
@@ -5223,22 +5234,22 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>505</v>
+        <v>378</v>
       </c>
       <c r="B129" t="s">
-        <v>506</v>
+        <v>379</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>507</v>
+        <v>598</v>
       </c>
       <c r="E129" t="s">
-        <v>508</v>
+        <v>380</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>509</v>
+        <v>381</v>
       </c>
       <c r="G129">
         <v>2</v>
@@ -5246,22 +5257,22 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>510</v>
+        <v>382</v>
       </c>
       <c r="B130" t="s">
-        <v>511</v>
+        <v>383</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>512</v>
+        <v>599</v>
       </c>
       <c r="E130" t="s">
-        <v>513</v>
+        <v>384</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>514</v>
+        <v>385</v>
       </c>
       <c r="G130">
         <v>2</v>
@@ -5269,22 +5280,22 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>515</v>
+        <v>386</v>
       </c>
       <c r="B131" t="s">
-        <v>516</v>
+        <v>387</v>
       </c>
       <c r="C131">
         <v>3</v>
       </c>
       <c r="D131" t="s">
-        <v>517</v>
+        <v>600</v>
       </c>
       <c r="E131" t="s">
-        <v>518</v>
+        <v>388</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>519</v>
+        <v>389</v>
       </c>
       <c r="G131">
         <v>1</v>
@@ -5292,22 +5303,22 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>520</v>
+        <v>390</v>
       </c>
       <c r="B132" t="s">
-        <v>520</v>
+        <v>390</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>521</v>
+        <v>601</v>
       </c>
       <c r="E132" t="s">
-        <v>522</v>
+        <v>391</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>523</v>
+        <v>392</v>
       </c>
       <c r="G132">
         <v>1</v>
@@ -5315,22 +5326,22 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>524</v>
+        <v>393</v>
       </c>
       <c r="B133" t="s">
-        <v>524</v>
+        <v>393</v>
       </c>
       <c r="C133">
         <v>5</v>
       </c>
-      <c r="D133" t="s">
-        <v>525</v>
+      <c r="D133" s="2" t="s">
+        <v>602</v>
       </c>
       <c r="E133" t="s">
-        <v>522</v>
+        <v>391</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>523</v>
+        <v>392</v>
       </c>
       <c r="G133">
         <v>1</v>
@@ -5338,22 +5349,22 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>526</v>
+        <v>394</v>
       </c>
       <c r="B134" t="s">
-        <v>527</v>
+        <v>395</v>
       </c>
       <c r="C134">
         <v>3</v>
       </c>
       <c r="D134" t="s">
-        <v>528</v>
+        <v>603</v>
       </c>
       <c r="E134" t="s">
-        <v>529</v>
+        <v>396</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>530</v>
+        <v>397</v>
       </c>
       <c r="G134">
         <v>1</v>
@@ -5361,22 +5372,22 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>531</v>
+        <v>398</v>
       </c>
       <c r="B135" t="s">
-        <v>532</v>
+        <v>399</v>
       </c>
       <c r="C135">
         <v>3</v>
       </c>
       <c r="D135" t="s">
-        <v>533</v>
+        <v>604</v>
       </c>
       <c r="E135" t="s">
-        <v>534</v>
+        <v>400</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>535</v>
+        <v>401</v>
       </c>
       <c r="G135">
         <v>1</v>
@@ -5384,22 +5395,22 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>536</v>
+        <v>402</v>
       </c>
       <c r="B136" t="s">
-        <v>537</v>
+        <v>403</v>
       </c>
       <c r="C136">
         <v>3</v>
       </c>
       <c r="D136" t="s">
-        <v>538</v>
+        <v>605</v>
       </c>
       <c r="E136" t="s">
-        <v>539</v>
+        <v>404</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>540</v>
+        <v>405</v>
       </c>
       <c r="G136">
         <v>1</v>
@@ -5407,22 +5418,22 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>541</v>
+        <v>406</v>
       </c>
       <c r="B137" t="s">
-        <v>542</v>
+        <v>407</v>
       </c>
       <c r="C137">
         <v>3</v>
       </c>
       <c r="D137" t="s">
-        <v>543</v>
+        <v>606</v>
       </c>
       <c r="E137" t="s">
         <v>235</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>544</v>
+        <v>408</v>
       </c>
       <c r="G137">
         <v>1</v>
@@ -5430,22 +5441,22 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>545</v>
+        <v>409</v>
       </c>
       <c r="B138" t="s">
-        <v>546</v>
+        <v>410</v>
       </c>
       <c r="C138">
         <v>4</v>
       </c>
-      <c r="D138" t="s">
-        <v>547</v>
+      <c r="D138" s="2" t="s">
+        <v>607</v>
       </c>
       <c r="E138" t="s">
-        <v>548</v>
+        <v>411</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>549</v>
+        <v>412</v>
       </c>
       <c r="G138">
         <v>1</v>
@@ -5453,22 +5464,22 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>550</v>
+        <v>413</v>
       </c>
       <c r="B139" t="s">
-        <v>551</v>
+        <v>414</v>
       </c>
       <c r="C139">
         <v>4</v>
       </c>
       <c r="D139" t="s">
-        <v>552</v>
+        <v>608</v>
       </c>
       <c r="E139" t="s">
-        <v>553</v>
+        <v>415</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>554</v>
+        <v>416</v>
       </c>
       <c r="G139">
         <v>1</v>
@@ -5476,22 +5487,22 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>555</v>
+        <v>417</v>
       </c>
       <c r="B140" t="s">
-        <v>556</v>
+        <v>418</v>
       </c>
       <c r="C140">
         <v>4</v>
       </c>
       <c r="D140" t="s">
-        <v>558</v>
+        <v>609</v>
       </c>
       <c r="E140" t="s">
-        <v>560</v>
+        <v>420</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>566</v>
+        <v>425</v>
       </c>
       <c r="G140">
         <v>1</v>
@@ -5499,22 +5510,22 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>561</v>
+        <v>421</v>
       </c>
       <c r="B141" t="s">
-        <v>557</v>
+        <v>419</v>
       </c>
       <c r="C141">
         <v>5</v>
       </c>
       <c r="D141" t="s">
-        <v>559</v>
+        <v>610</v>
       </c>
       <c r="E141" t="s">
-        <v>560</v>
+        <v>420</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>566</v>
+        <v>425</v>
       </c>
       <c r="G141">
         <v>1</v>
@@ -5522,22 +5533,22 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>562</v>
+        <v>422</v>
       </c>
       <c r="B142" t="s">
-        <v>563</v>
+        <v>423</v>
       </c>
       <c r="C142">
         <v>4</v>
       </c>
       <c r="D142" t="s">
-        <v>564</v>
+        <v>611</v>
       </c>
       <c r="E142" t="s">
-        <v>565</v>
+        <v>424</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>567</v>
+        <v>426</v>
       </c>
       <c r="G142">
         <v>1</v>
@@ -5545,22 +5556,22 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>568</v>
+        <v>427</v>
       </c>
       <c r="B143" t="s">
-        <v>569</v>
+        <v>428</v>
       </c>
       <c r="C143">
         <v>4</v>
       </c>
       <c r="D143" t="s">
-        <v>570</v>
+        <v>612</v>
       </c>
       <c r="E143" t="s">
-        <v>571</v>
+        <v>429</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>452</v>
+        <v>340</v>
       </c>
       <c r="G143">
         <v>1</v>
@@ -5568,22 +5579,22 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>572</v>
+        <v>430</v>
       </c>
       <c r="B144" t="s">
-        <v>572</v>
+        <v>430</v>
       </c>
       <c r="C144">
         <v>2</v>
       </c>
       <c r="D144" t="s">
-        <v>573</v>
+        <v>613</v>
       </c>
       <c r="E144" t="s">
-        <v>574</v>
+        <v>431</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>575</v>
+        <v>432</v>
       </c>
       <c r="G144">
         <v>1</v>
@@ -5591,22 +5602,22 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>576</v>
+        <v>433</v>
       </c>
       <c r="B145" t="s">
-        <v>576</v>
+        <v>433</v>
       </c>
       <c r="C145">
         <v>3</v>
       </c>
       <c r="D145" t="s">
-        <v>577</v>
+        <v>614</v>
       </c>
       <c r="E145" t="s">
-        <v>495</v>
+        <v>370</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>575</v>
+        <v>432</v>
       </c>
       <c r="G145">
         <v>1</v>
@@ -5614,22 +5625,22 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>578</v>
+        <v>434</v>
       </c>
       <c r="B146" t="s">
-        <v>579</v>
+        <v>435</v>
       </c>
       <c r="C146">
         <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>580</v>
+        <v>615</v>
       </c>
       <c r="E146" t="s">
-        <v>581</v>
+        <v>436</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>582</v>
+        <v>437</v>
       </c>
       <c r="G146">
         <v>2</v>
@@ -5637,22 +5648,22 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>583</v>
+        <v>438</v>
       </c>
       <c r="B147" t="s">
-        <v>584</v>
+        <v>439</v>
       </c>
       <c r="C147">
         <v>4</v>
       </c>
       <c r="D147" t="s">
-        <v>585</v>
+        <v>616</v>
       </c>
       <c r="E147" t="s">
         <v>235</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>586</v>
+        <v>440</v>
       </c>
       <c r="G147">
         <v>1</v>
@@ -5660,22 +5671,22 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>587</v>
+        <v>441</v>
       </c>
       <c r="B148" t="s">
-        <v>588</v>
+        <v>442</v>
       </c>
       <c r="C148">
         <v>3</v>
       </c>
       <c r="D148" t="s">
-        <v>589</v>
+        <v>617</v>
       </c>
       <c r="E148" t="s">
-        <v>590</v>
+        <v>443</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>591</v>
+        <v>444</v>
       </c>
       <c r="G148">
         <v>1</v>
@@ -5683,22 +5694,22 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>592</v>
+        <v>445</v>
       </c>
       <c r="B149" t="s">
-        <v>593</v>
+        <v>446</v>
       </c>
       <c r="C149">
         <v>3</v>
       </c>
       <c r="D149" t="s">
-        <v>594</v>
+        <v>618</v>
       </c>
       <c r="E149" t="s">
-        <v>595</v>
+        <v>447</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>596</v>
+        <v>448</v>
       </c>
       <c r="G149">
         <v>1</v>
@@ -5706,22 +5717,22 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>597</v>
+        <v>449</v>
       </c>
       <c r="B150" t="s">
-        <v>598</v>
+        <v>450</v>
       </c>
       <c r="C150">
         <v>3</v>
       </c>
       <c r="D150" t="s">
-        <v>599</v>
+        <v>619</v>
       </c>
       <c r="E150" t="s">
-        <v>600</v>
+        <v>451</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>601</v>
+        <v>452</v>
       </c>
       <c r="G150">
         <v>1</v>
@@ -5729,22 +5740,22 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>602</v>
+        <v>453</v>
       </c>
       <c r="B151" t="s">
-        <v>603</v>
+        <v>454</v>
       </c>
       <c r="C151">
         <v>4</v>
       </c>
       <c r="D151" t="s">
-        <v>604</v>
+        <v>620</v>
       </c>
       <c r="E151" t="s">
         <v>235</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>605</v>
+        <v>455</v>
       </c>
       <c r="G151">
         <v>1</v>
@@ -5752,22 +5763,22 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>606</v>
+        <v>456</v>
       </c>
       <c r="B152" t="s">
-        <v>607</v>
+        <v>457</v>
       </c>
       <c r="C152">
         <v>4</v>
       </c>
       <c r="D152" t="s">
-        <v>608</v>
+        <v>621</v>
       </c>
       <c r="E152" t="s">
-        <v>609</v>
+        <v>458</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>610</v>
+        <v>459</v>
       </c>
       <c r="G152">
         <v>1</v>
@@ -5775,22 +5786,22 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>611</v>
+        <v>460</v>
       </c>
       <c r="B153" t="s">
-        <v>612</v>
+        <v>461</v>
       </c>
       <c r="C153">
         <v>2</v>
       </c>
       <c r="D153" t="s">
-        <v>613</v>
+        <v>622</v>
       </c>
       <c r="E153" t="s">
         <v>2</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>614</v>
+        <v>462</v>
       </c>
       <c r="G153">
         <v>1</v>
@@ -5798,22 +5809,22 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>615</v>
+        <v>463</v>
       </c>
       <c r="B154" t="s">
-        <v>616</v>
+        <v>464</v>
       </c>
       <c r="C154">
         <v>3</v>
       </c>
       <c r="D154" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="E154" t="s">
-        <v>618</v>
+        <v>465</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>619</v>
+        <v>466</v>
       </c>
       <c r="G154">
         <v>1</v>
@@ -5821,29 +5832,45 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>620</v>
+        <v>467</v>
       </c>
       <c r="B155" t="s">
-        <v>621</v>
+        <v>468</v>
       </c>
       <c r="C155">
         <v>3</v>
       </c>
       <c r="D155" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="E155" t="s">
-        <v>623</v>
+        <v>469</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>624</v>
+        <v>470</v>
       </c>
       <c r="G155">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D1" r:id="rId1" xr:uid="{899C9EC5-539F-4BDB-9A2D-F7C918AB9EEE}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{827FD9E7-4529-4E89-9463-C24DDB2C8493}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{8B62675E-6826-4687-A9C1-2849CA967275}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{0CE9FE1E-D06C-4820-95F9-A64934E84449}"/>
+    <hyperlink ref="D20" r:id="rId5" xr:uid="{073CF697-87CF-4B15-897E-87F283C07ED9}"/>
+    <hyperlink ref="D69" r:id="rId6" xr:uid="{9ED88FAB-9A21-4B5D-B569-B1CC41B93004}"/>
+    <hyperlink ref="D95" r:id="rId7" xr:uid="{2686521B-F340-4E51-BA70-8E0EBFC4FD55}"/>
+    <hyperlink ref="D102" r:id="rId8" xr:uid="{B1C1C455-40F5-40EE-A262-823F3E505DBF}"/>
+    <hyperlink ref="D106" r:id="rId9" xr:uid="{5ED76D23-4021-4CF4-AFAD-4B6FCD5FEE8B}"/>
+    <hyperlink ref="D109" r:id="rId10" xr:uid="{156C7FA4-7F1A-43A6-ADC7-4A2A79F1521A}"/>
+    <hyperlink ref="D123" r:id="rId11" xr:uid="{4FF446EB-2121-41E9-8CCE-DD52240BE193}"/>
+    <hyperlink ref="D128" r:id="rId12" xr:uid="{011A385D-83C1-49F3-94A8-2D57AB8D51DF}"/>
+    <hyperlink ref="D133" r:id="rId13" xr:uid="{E7D95AC4-DDCF-42F1-B07F-DE761BAA8A6A}"/>
+    <hyperlink ref="D138" r:id="rId14" xr:uid="{F6402070-B9B1-454F-9BA1-B301D9287D55}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add 26 more modules. Up to Praetorian.
Former-commit-id: ab2d50b01dc1c71503f9bb5fab0fe2f5f90d2b28
Former-commit-id: b02bd9dd8e51467c2539867674594026719beeaa
</commit_message>
<xml_diff>
--- a/resources/modules-config-details-setup.xlsx
+++ b/resources/modules-config-details-setup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\IdeaProjects\MakeMyManual\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9A2850-2971-4C92-AE8F-691A439D6A4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36102B42-F469-48E8-911C-DB505023C75C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="3340" windowWidth="12780" windowHeight="6600" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
+    <workbookView xWindow="-14320" yWindow="1350" windowWidth="19200" windowHeight="10200" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
   </bookViews>
   <sheets>
     <sheet name="modules-config-details" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="726">
   <si>
     <t>Colour Flash</t>
   </si>
@@ -1908,6 +1908,309 @@
   </si>
   <si>
     <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Timezone.pdf</t>
+  </si>
+  <si>
+    <t>Polyhedral Maze</t>
+  </si>
+  <si>
+    <t>PolyhedralMazeModule</t>
+  </si>
+  <si>
+    <t>2018-01-01</t>
+  </si>
+  <si>
+    <t>Symbolic Coordinates</t>
+  </si>
+  <si>
+    <t>symbolicCoordinates</t>
+  </si>
+  <si>
+    <t>Royal_Flu$h</t>
+  </si>
+  <si>
+    <t>2018-01-09</t>
+  </si>
+  <si>
+    <t>Poker</t>
+  </si>
+  <si>
+    <t>2018-01-14</t>
+  </si>
+  <si>
+    <t>Sonic the Hedgehog</t>
+  </si>
+  <si>
+    <t>sonic</t>
+  </si>
+  <si>
+    <t>Poetry</t>
+  </si>
+  <si>
+    <t>poetry</t>
+  </si>
+  <si>
+    <t>Button Sequence</t>
+  </si>
+  <si>
+    <t>buttonSequencesModule</t>
+  </si>
+  <si>
+    <t>2018-01-15</t>
+  </si>
+  <si>
+    <t>Algebra</t>
+  </si>
+  <si>
+    <t>algebra</t>
+  </si>
+  <si>
+    <t>2018-01-17</t>
+  </si>
+  <si>
+    <t>Visual Impairment</t>
+  </si>
+  <si>
+    <t>visual_impairment</t>
+  </si>
+  <si>
+    <t>KingBranBran</t>
+  </si>
+  <si>
+    <t>2018-01-20</t>
+  </si>
+  <si>
+    <t>Jukebox</t>
+  </si>
+  <si>
+    <t>jukebox</t>
+  </si>
+  <si>
+    <t>2018-01-23</t>
+  </si>
+  <si>
+    <t>Identity Parade</t>
+  </si>
+  <si>
+    <t>identityParade</t>
+  </si>
+  <si>
+    <t>2018-01-25</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>maintenance</t>
+  </si>
+  <si>
+    <t>2018-01-30</t>
+  </si>
+  <si>
+    <t>Blind Maze</t>
+  </si>
+  <si>
+    <t>BlindMaze</t>
+  </si>
+  <si>
+    <t>Riverbui, McNiko67</t>
+  </si>
+  <si>
+    <t>Backgrounds</t>
+  </si>
+  <si>
+    <t>McNiko67</t>
+  </si>
+  <si>
+    <t>Mortal Kombat</t>
+  </si>
+  <si>
+    <t>2018-02-02</t>
+  </si>
+  <si>
+    <t>Mashematics</t>
+  </si>
+  <si>
+    <t>Marksam32</t>
+  </si>
+  <si>
+    <t>2018-02-03</t>
+  </si>
+  <si>
+    <t>Faulty Backgrounds</t>
+  </si>
+  <si>
+    <t>Radiator</t>
+  </si>
+  <si>
+    <t>red031000, Inova</t>
+  </si>
+  <si>
+    <t>2018-02-04</t>
+  </si>
+  <si>
+    <t>Modern Cipher</t>
+  </si>
+  <si>
+    <t>TheFe</t>
+  </si>
+  <si>
+    <t>LED Grid</t>
+  </si>
+  <si>
+    <t>2018-02-06</t>
+  </si>
+  <si>
+    <t>Sink</t>
+  </si>
+  <si>
+    <t>2018-02-09</t>
+  </si>
+  <si>
+    <t>iPhone</t>
+  </si>
+  <si>
+    <t>2018-02-20</t>
+  </si>
+  <si>
+    <t>Swan</t>
+  </si>
+  <si>
+    <t>2018-02-22</t>
+  </si>
+  <si>
+    <t>Waste Management</t>
+  </si>
+  <si>
+    <t>red031000, Inova, AppleSlice</t>
+  </si>
+  <si>
+    <t>2018-02-23</t>
+  </si>
+  <si>
+    <t>Human Resources</t>
+  </si>
+  <si>
+    <t>2018-02-26</t>
+  </si>
+  <si>
+    <t>Skyrim</t>
+  </si>
+  <si>
+    <t>2018-03-02</t>
+  </si>
+  <si>
+    <t>Burglar Alarm</t>
+  </si>
+  <si>
+    <t>2018-03-03</t>
+  </si>
+  <si>
+    <t>mortalKombat</t>
+  </si>
+  <si>
+    <t>modernCipher</t>
+  </si>
+  <si>
+    <t>burglarAlarm</t>
+  </si>
+  <si>
+    <t>mashematics</t>
+  </si>
+  <si>
+    <t>FaultyBackgrounds</t>
+  </si>
+  <si>
+    <t>radiator</t>
+  </si>
+  <si>
+    <t>theSwan</t>
+  </si>
+  <si>
+    <t>wastemanagement</t>
+  </si>
+  <si>
+    <t>HumanResourcesModule</t>
+  </si>
+  <si>
+    <t>skyrim</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Polyhedral%20Maze.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Symbolic%20Coordinates.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Poker.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Sonic%20the%20Hedgehog.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Poetry.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Button%20Sequence.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Algebra.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Visual%20Impairment.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/The%20Jukebox.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Identity%20Parade.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Maintenance.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Blind%20Maze.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Backgrounds.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Mortal%20Kombat.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Mashematics.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Faulty%20Backgrounds.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Radiator.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Modern%20Cipher.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/LED%20Grid.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Sink.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/The%20iPhone.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/The%20Swan.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Waste%20Management.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Human%20Resources.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Skyrim.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Timwi/KtaneContent/master/PDF/Burglar%20Alarm.pdf</t>
   </si>
 </sst>
 </file>
@@ -2271,10 +2574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC09710-E84E-49A6-94A5-EB5A61B7898A}">
-  <dimension ref="A1:G155"/>
+  <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C136" zoomScale="72" workbookViewId="0">
-      <selection activeCell="E154" sqref="E154"/>
+    <sheetView tabSelected="1" topLeftCell="B158" zoomScale="72" workbookViewId="0">
+      <selection activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5850,6 +6153,604 @@
         <v>470</v>
       </c>
       <c r="G155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>625</v>
+      </c>
+      <c r="B156" t="s">
+        <v>626</v>
+      </c>
+      <c r="C156">
+        <v>5</v>
+      </c>
+      <c r="D156" t="s">
+        <v>700</v>
+      </c>
+      <c r="E156" t="s">
+        <v>235</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="G156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>628</v>
+      </c>
+      <c r="B157" t="s">
+        <v>629</v>
+      </c>
+      <c r="C157">
+        <v>2</v>
+      </c>
+      <c r="D157" t="s">
+        <v>701</v>
+      </c>
+      <c r="E157" t="s">
+        <v>630</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="G157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>632</v>
+      </c>
+      <c r="B158" t="s">
+        <v>632</v>
+      </c>
+      <c r="C158">
+        <v>3</v>
+      </c>
+      <c r="D158" t="s">
+        <v>702</v>
+      </c>
+      <c r="E158" t="s">
+        <v>630</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="G158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>634</v>
+      </c>
+      <c r="B159" t="s">
+        <v>635</v>
+      </c>
+      <c r="C159">
+        <v>3</v>
+      </c>
+      <c r="D159" t="s">
+        <v>703</v>
+      </c>
+      <c r="E159" t="s">
+        <v>630</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="G159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>636</v>
+      </c>
+      <c r="B160" t="s">
+        <v>637</v>
+      </c>
+      <c r="C160">
+        <v>3</v>
+      </c>
+      <c r="D160" t="s">
+        <v>704</v>
+      </c>
+      <c r="E160" t="s">
+        <v>47</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="G160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>638</v>
+      </c>
+      <c r="B161" t="s">
+        <v>639</v>
+      </c>
+      <c r="C161">
+        <v>3</v>
+      </c>
+      <c r="D161" t="s">
+        <v>705</v>
+      </c>
+      <c r="E161" t="s">
+        <v>257</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="G161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>641</v>
+      </c>
+      <c r="B162" t="s">
+        <v>642</v>
+      </c>
+      <c r="C162">
+        <v>3</v>
+      </c>
+      <c r="D162" t="s">
+        <v>706</v>
+      </c>
+      <c r="E162" t="s">
+        <v>630</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="G162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>644</v>
+      </c>
+      <c r="B163" t="s">
+        <v>645</v>
+      </c>
+      <c r="C163">
+        <v>3</v>
+      </c>
+      <c r="D163" t="s">
+        <v>707</v>
+      </c>
+      <c r="E163" t="s">
+        <v>646</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="G163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>648</v>
+      </c>
+      <c r="B164" t="s">
+        <v>649</v>
+      </c>
+      <c r="C164">
+        <v>2</v>
+      </c>
+      <c r="D164" t="s">
+        <v>708</v>
+      </c>
+      <c r="E164" t="s">
+        <v>630</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="G164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>651</v>
+      </c>
+      <c r="B165" t="s">
+        <v>652</v>
+      </c>
+      <c r="C165">
+        <v>2</v>
+      </c>
+      <c r="D165" t="s">
+        <v>709</v>
+      </c>
+      <c r="E165" t="s">
+        <v>630</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="G165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>654</v>
+      </c>
+      <c r="B166" t="s">
+        <v>655</v>
+      </c>
+      <c r="C166">
+        <v>4</v>
+      </c>
+      <c r="D166" t="s">
+        <v>710</v>
+      </c>
+      <c r="E166" t="s">
+        <v>630</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="G166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>657</v>
+      </c>
+      <c r="B167" t="s">
+        <v>658</v>
+      </c>
+      <c r="C167">
+        <v>4</v>
+      </c>
+      <c r="D167" t="s">
+        <v>711</v>
+      </c>
+      <c r="E167" t="s">
+        <v>659</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="G167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>660</v>
+      </c>
+      <c r="B168" t="s">
+        <v>660</v>
+      </c>
+      <c r="C168">
+        <v>2</v>
+      </c>
+      <c r="D168" t="s">
+        <v>712</v>
+      </c>
+      <c r="E168" t="s">
+        <v>661</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="G168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>662</v>
+      </c>
+      <c r="B169" t="s">
+        <v>690</v>
+      </c>
+      <c r="C169">
+        <v>3</v>
+      </c>
+      <c r="D169" t="s">
+        <v>713</v>
+      </c>
+      <c r="E169" t="s">
+        <v>630</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="G169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>664</v>
+      </c>
+      <c r="B170" t="s">
+        <v>693</v>
+      </c>
+      <c r="C170">
+        <v>2</v>
+      </c>
+      <c r="D170" t="s">
+        <v>714</v>
+      </c>
+      <c r="E170" t="s">
+        <v>665</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="G170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>667</v>
+      </c>
+      <c r="B171" t="s">
+        <v>694</v>
+      </c>
+      <c r="C171">
+        <v>2</v>
+      </c>
+      <c r="D171" t="s">
+        <v>715</v>
+      </c>
+      <c r="E171" t="s">
+        <v>661</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="G171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>668</v>
+      </c>
+      <c r="B172" t="s">
+        <v>695</v>
+      </c>
+      <c r="C172">
+        <v>2</v>
+      </c>
+      <c r="D172" t="s">
+        <v>716</v>
+      </c>
+      <c r="E172" t="s">
+        <v>669</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="G172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>671</v>
+      </c>
+      <c r="B173" t="s">
+        <v>691</v>
+      </c>
+      <c r="C173">
+        <v>3</v>
+      </c>
+      <c r="D173" t="s">
+        <v>717</v>
+      </c>
+      <c r="E173" t="s">
+        <v>672</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="G173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>673</v>
+      </c>
+      <c r="B174" t="s">
+        <v>673</v>
+      </c>
+      <c r="C174">
+        <v>2</v>
+      </c>
+      <c r="D174" t="s">
+        <v>718</v>
+      </c>
+      <c r="E174" t="s">
+        <v>630</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="G174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>675</v>
+      </c>
+      <c r="B175" t="s">
+        <v>675</v>
+      </c>
+      <c r="C175">
+        <v>2</v>
+      </c>
+      <c r="D175" t="s">
+        <v>719</v>
+      </c>
+      <c r="E175" t="s">
+        <v>661</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="G175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>677</v>
+      </c>
+      <c r="B176" t="s">
+        <v>677</v>
+      </c>
+      <c r="C176">
+        <v>4</v>
+      </c>
+      <c r="D176" t="s">
+        <v>720</v>
+      </c>
+      <c r="E176" t="s">
+        <v>630</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="G176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>679</v>
+      </c>
+      <c r="B177" t="s">
+        <v>696</v>
+      </c>
+      <c r="C177">
+        <v>4</v>
+      </c>
+      <c r="D177" t="s">
+        <v>721</v>
+      </c>
+      <c r="E177" t="s">
+        <v>630</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="G177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>681</v>
+      </c>
+      <c r="B178" t="s">
+        <v>697</v>
+      </c>
+      <c r="C178">
+        <v>4</v>
+      </c>
+      <c r="D178" t="s">
+        <v>722</v>
+      </c>
+      <c r="E178" t="s">
+        <v>682</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="G178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>684</v>
+      </c>
+      <c r="B179" t="s">
+        <v>698</v>
+      </c>
+      <c r="C179">
+        <v>3</v>
+      </c>
+      <c r="D179" t="s">
+        <v>723</v>
+      </c>
+      <c r="E179" t="s">
+        <v>396</v>
+      </c>
+      <c r="F179" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="G179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>686</v>
+      </c>
+      <c r="B180" t="s">
+        <v>699</v>
+      </c>
+      <c r="C180">
+        <v>4</v>
+      </c>
+      <c r="D180" t="s">
+        <v>724</v>
+      </c>
+      <c r="E180" t="s">
+        <v>630</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="G180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>688</v>
+      </c>
+      <c r="B181" t="s">
+        <v>692</v>
+      </c>
+      <c r="C181">
+        <v>3</v>
+      </c>
+      <c r="D181" t="s">
+        <v>725</v>
+      </c>
+      <c r="E181" t="s">
+        <v>665</v>
+      </c>
+      <c r="F181" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="G181">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Temporarily remove German Vent Gas
Former-commit-id: 81aa7c31681199da0b1692c85ab2d052caa45e0d
Former-commit-id: 414f74f33e85e5236961be0e7daf92c3c810bea6
</commit_message>
<xml_diff>
--- a/resources/modules-config-details-setup.xlsx
+++ b/resources/modules-config-details-setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\IdeaProjects\MakeMyManual\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36102B42-F469-48E8-911C-DB505023C75C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDF5CBB-090E-44D7-AF2F-8BDD4BAAE1C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14320" yWindow="1350" windowWidth="19200" windowHeight="10200" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{8FDEE611-CDBB-4BAD-AA96-AFBFDE129191}"/>
   </bookViews>
   <sheets>
     <sheet name="modules-config-details" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="723">
   <si>
     <t>Colour Flash</t>
   </si>
@@ -1035,15 +1035,6 @@
   </si>
   <si>
     <t>NeedyVentGas</t>
-  </si>
-  <si>
-    <t>German Venting Gas</t>
-  </si>
-  <si>
-    <t>VentGasTranslated</t>
-  </si>
-  <si>
-    <t>modules/German Venting Gas.pdf</t>
   </si>
   <si>
     <t>Refill That Beer!</t>
@@ -2574,10 +2565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC09710-E84E-49A6-94A5-EB5A61B7898A}">
-  <dimension ref="A1:G181"/>
+  <dimension ref="A1:G180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B158" zoomScale="72" workbookViewId="0">
-      <selection activeCell="D182" sqref="D182"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="72" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2602,7 +2593,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -2625,7 +2616,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -2648,7 +2639,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -2671,7 +2662,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -2694,7 +2685,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -2717,7 +2708,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
@@ -2740,7 +2731,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -2763,7 +2754,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -2786,7 +2777,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -2809,7 +2800,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="E10" t="s">
         <v>30</v>
@@ -2832,7 +2823,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="E11" t="s">
         <v>30</v>
@@ -2855,7 +2846,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="E12" t="s">
         <v>30</v>
@@ -2878,7 +2869,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="E13" t="s">
         <v>37</v>
@@ -2901,7 +2892,7 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="E14" t="s">
         <v>37</v>
@@ -2924,7 +2915,7 @@
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="E15" t="s">
         <v>37</v>
@@ -2947,7 +2938,7 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="E16" t="s">
         <v>30</v>
@@ -2970,7 +2961,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="E17" t="s">
         <v>47</v>
@@ -2993,7 +2984,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="E18" t="s">
         <v>50</v>
@@ -3016,7 +3007,7 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="E19" t="s">
         <v>30</v>
@@ -3039,7 +3030,7 @@
         <v>3</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="E20" t="s">
         <v>56</v>
@@ -3062,7 +3053,7 @@
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E21" t="s">
         <v>59</v>
@@ -3085,7 +3076,7 @@
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="E22" t="s">
         <v>37</v>
@@ -3108,7 +3099,7 @@
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="E23" t="s">
         <v>56</v>
@@ -3131,7 +3122,7 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="E24" t="s">
         <v>37</v>
@@ -3154,7 +3145,7 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="E25" t="s">
         <v>37</v>
@@ -3177,7 +3168,7 @@
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="E26" t="s">
         <v>73</v>
@@ -3200,7 +3191,7 @@
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="E27" t="s">
         <v>30</v>
@@ -3223,7 +3214,7 @@
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="E28" t="s">
         <v>30</v>
@@ -3246,7 +3237,7 @@
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="E29" t="s">
         <v>37</v>
@@ -3269,7 +3260,7 @@
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="E30" t="s">
         <v>85</v>
@@ -3292,7 +3283,7 @@
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="E31" t="s">
         <v>73</v>
@@ -3315,7 +3306,7 @@
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="E32" t="s">
         <v>56</v>
@@ -3338,7 +3329,7 @@
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E33" t="s">
         <v>37</v>
@@ -3361,7 +3352,7 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="E34" t="s">
         <v>96</v>
@@ -3384,7 +3375,7 @@
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="E35" t="s">
         <v>99</v>
@@ -3407,7 +3398,7 @@
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="E36" t="s">
         <v>37</v>
@@ -3430,7 +3421,7 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="E37" t="s">
         <v>217</v>
@@ -3453,7 +3444,7 @@
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="E38" t="s">
         <v>219</v>
@@ -3476,7 +3467,7 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="E39" t="s">
         <v>221</v>
@@ -3499,7 +3490,7 @@
         <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="E40" t="s">
         <v>56</v>
@@ -3522,7 +3513,7 @@
         <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E41" t="s">
         <v>224</v>
@@ -3545,7 +3536,7 @@
         <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="E42" t="s">
         <v>225</v>
@@ -3568,7 +3559,7 @@
         <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="E43" t="s">
         <v>227</v>
@@ -3591,7 +3582,7 @@
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E44" t="s">
         <v>229</v>
@@ -3614,7 +3605,7 @@
         <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="E45" t="s">
         <v>47</v>
@@ -3637,7 +3628,7 @@
         <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E46" t="s">
         <v>225</v>
@@ -3660,7 +3651,7 @@
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="E47" t="s">
         <v>233</v>
@@ -3683,7 +3674,7 @@
         <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E48" t="s">
         <v>235</v>
@@ -3706,7 +3697,7 @@
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="E49" t="s">
         <v>235</v>
@@ -3729,7 +3720,7 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="E50" t="s">
         <v>96</v>
@@ -3752,7 +3743,7 @@
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E51" t="s">
         <v>235</v>
@@ -3775,7 +3766,7 @@
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="E52" t="s">
         <v>225</v>
@@ -3798,7 +3789,7 @@
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E53" t="s">
         <v>241</v>
@@ -3821,7 +3812,7 @@
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="E54" t="s">
         <v>235</v>
@@ -3844,7 +3835,7 @@
         <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="E55" t="s">
         <v>235</v>
@@ -3867,7 +3858,7 @@
         <v>4</v>
       </c>
       <c r="D56" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="E56" t="s">
         <v>244</v>
@@ -3890,7 +3881,7 @@
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="E57" t="s">
         <v>233</v>
@@ -3913,7 +3904,7 @@
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="E58" t="s">
         <v>247</v>
@@ -3936,7 +3927,7 @@
         <v>4</v>
       </c>
       <c r="D59" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="E59" t="s">
         <v>225</v>
@@ -3959,7 +3950,7 @@
         <v>4</v>
       </c>
       <c r="D60" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="E60" t="s">
         <v>250</v>
@@ -3982,7 +3973,7 @@
         <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="E61" t="s">
         <v>233</v>
@@ -4005,7 +3996,7 @@
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="E62" t="s">
         <v>219</v>
@@ -4028,7 +4019,7 @@
         <v>4</v>
       </c>
       <c r="D63" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="E63" t="s">
         <v>235</v>
@@ -4051,7 +4042,7 @@
         <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="E64" t="s">
         <v>255</v>
@@ -4074,7 +4065,7 @@
         <v>2</v>
       </c>
       <c r="D65" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="E65" t="s">
         <v>257</v>
@@ -4097,7 +4088,7 @@
         <v>4</v>
       </c>
       <c r="D66" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E66" t="s">
         <v>235</v>
@@ -4120,7 +4111,7 @@
         <v>2</v>
       </c>
       <c r="D67" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E67" t="s">
         <v>59</v>
@@ -4143,7 +4134,7 @@
         <v>2</v>
       </c>
       <c r="D68" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="E68" t="s">
         <v>257</v>
@@ -4166,7 +4157,7 @@
         <v>2</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="E69" t="s">
         <v>247</v>
@@ -4189,7 +4180,7 @@
         <v>2</v>
       </c>
       <c r="D70" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="E70" t="s">
         <v>257</v>
@@ -4212,7 +4203,7 @@
         <v>4</v>
       </c>
       <c r="D71" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E71" t="s">
         <v>219</v>
@@ -4235,7 +4226,7 @@
         <v>4</v>
       </c>
       <c r="D72" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E72" t="s">
         <v>235</v>
@@ -4258,7 +4249,7 @@
         <v>4</v>
       </c>
       <c r="D73" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E73" t="s">
         <v>265</v>
@@ -4281,7 +4272,7 @@
         <v>3</v>
       </c>
       <c r="D74" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="E74" t="s">
         <v>267</v>
@@ -4304,7 +4295,7 @@
         <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="E75" t="s">
         <v>59</v>
@@ -4327,7 +4318,7 @@
         <v>4</v>
       </c>
       <c r="D76" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="E76" t="s">
         <v>235</v>
@@ -4350,7 +4341,7 @@
         <v>4</v>
       </c>
       <c r="D77" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="E77" t="s">
         <v>270</v>
@@ -4373,7 +4364,7 @@
         <v>4</v>
       </c>
       <c r="D78" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="E78" t="s">
         <v>272</v>
@@ -4396,7 +4387,7 @@
         <v>4</v>
       </c>
       <c r="D79" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E79" t="s">
         <v>267</v>
@@ -4419,7 +4410,7 @@
         <v>3</v>
       </c>
       <c r="D80" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="E80" t="s">
         <v>275</v>
@@ -4442,7 +4433,7 @@
         <v>4</v>
       </c>
       <c r="D81" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E81" t="s">
         <v>277</v>
@@ -4465,7 +4456,7 @@
         <v>4</v>
       </c>
       <c r="D82" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E82" t="s">
         <v>257</v>
@@ -4488,7 +4479,7 @@
         <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="E83" t="s">
         <v>233</v>
@@ -4511,7 +4502,7 @@
         <v>3</v>
       </c>
       <c r="D84" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="E84" t="s">
         <v>281</v>
@@ -4534,7 +4525,7 @@
         <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="E85" t="s">
         <v>281</v>
@@ -4557,7 +4548,7 @@
         <v>4</v>
       </c>
       <c r="D86" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E86" t="s">
         <v>284</v>
@@ -4580,7 +4571,7 @@
         <v>2</v>
       </c>
       <c r="D87" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="E87" t="s">
         <v>219</v>
@@ -4603,7 +4594,7 @@
         <v>4</v>
       </c>
       <c r="D88" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E88" t="s">
         <v>235</v>
@@ -4626,7 +4617,7 @@
         <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="E89" t="s">
         <v>288</v>
@@ -4649,7 +4640,7 @@
         <v>4</v>
       </c>
       <c r="D90" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="E90" t="s">
         <v>257</v>
@@ -4672,7 +4663,7 @@
         <v>4</v>
       </c>
       <c r="D91" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="E91" t="s">
         <v>235</v>
@@ -4695,7 +4686,7 @@
         <v>3</v>
       </c>
       <c r="D92" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="E92" t="s">
         <v>292</v>
@@ -4718,7 +4709,7 @@
         <v>3</v>
       </c>
       <c r="D93" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="E93" t="s">
         <v>294</v>
@@ -4741,7 +4732,7 @@
         <v>3</v>
       </c>
       <c r="D94" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="E94" t="s">
         <v>296</v>
@@ -4764,7 +4755,7 @@
         <v>1</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="E95" t="s">
         <v>300</v>
@@ -4787,7 +4778,7 @@
         <v>2</v>
       </c>
       <c r="D96" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E96" t="s">
         <v>300</v>
@@ -4810,7 +4801,7 @@
         <v>2</v>
       </c>
       <c r="D97" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E97" t="s">
         <v>300</v>
@@ -4833,7 +4824,7 @@
         <v>2</v>
       </c>
       <c r="D98" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="E98" t="s">
         <v>300</v>
@@ -4856,7 +4847,7 @@
         <v>1</v>
       </c>
       <c r="D99" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="E99" t="s">
         <v>310</v>
@@ -4879,7 +4870,7 @@
         <v>1</v>
       </c>
       <c r="D100" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="E100" t="s">
         <v>310</v>
@@ -4902,7 +4893,7 @@
         <v>2</v>
       </c>
       <c r="D101" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="E101" t="s">
         <v>310</v>
@@ -4925,7 +4916,7 @@
         <v>1</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="E102" t="s">
         <v>310</v>
@@ -4948,7 +4939,7 @@
         <v>2</v>
       </c>
       <c r="D103" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E103" t="s">
         <v>310</v>
@@ -4971,7 +4962,7 @@
         <v>2</v>
       </c>
       <c r="D104" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="E104" t="s">
         <v>310</v>
@@ -4994,7 +4985,7 @@
         <v>3</v>
       </c>
       <c r="D105" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="E105" t="s">
         <v>310</v>
@@ -5017,7 +5008,7 @@
         <v>3</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="E106" t="s">
         <v>310</v>
@@ -5040,7 +5031,7 @@
         <v>3</v>
       </c>
       <c r="D107" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E107" t="s">
         <v>310</v>
@@ -5063,7 +5054,7 @@
         <v>2</v>
       </c>
       <c r="D108" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E108" t="s">
         <v>310</v>
@@ -5086,7 +5077,7 @@
         <v>2</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="E109" t="s">
         <v>310</v>
@@ -5109,7 +5100,7 @@
         <v>1</v>
       </c>
       <c r="D110" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="E110" t="s">
         <v>310</v>
@@ -5132,7 +5123,7 @@
         <v>1</v>
       </c>
       <c r="D111" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="E111" t="s">
         <v>310</v>
@@ -5155,7 +5146,7 @@
         <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E112" t="s">
         <v>310</v>
@@ -5178,13 +5169,13 @@
         <v>1</v>
       </c>
       <c r="D113" t="s">
+        <v>580</v>
+      </c>
+      <c r="E113" t="s">
         <v>336</v>
       </c>
-      <c r="E113" t="s">
-        <v>300</v>
-      </c>
       <c r="F113" s="1" t="s">
-        <v>301</v>
+        <v>337</v>
       </c>
       <c r="G113">
         <v>2</v>
@@ -5192,22 +5183,22 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B114" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C114">
         <v>1</v>
       </c>
       <c r="D114" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E114" t="s">
-        <v>339</v>
+        <v>10</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>340</v>
+        <v>11</v>
       </c>
       <c r="G114">
         <v>2</v>
@@ -5215,22 +5206,22 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
+        <v>340</v>
+      </c>
+      <c r="B115" t="s">
         <v>341</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="D115" t="s">
+        <v>582</v>
+      </c>
+      <c r="E115" t="s">
+        <v>2</v>
+      </c>
+      <c r="F115" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="C115">
-        <v>1</v>
-      </c>
-      <c r="D115" t="s">
-        <v>584</v>
-      </c>
-      <c r="E115" t="s">
-        <v>10</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="G115">
         <v>2</v>
@@ -5241,19 +5232,19 @@
         <v>343</v>
       </c>
       <c r="B116" t="s">
+        <v>343</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116" t="s">
+        <v>583</v>
+      </c>
+      <c r="E116" t="s">
+        <v>10</v>
+      </c>
+      <c r="F116" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="C116">
-        <v>1</v>
-      </c>
-      <c r="D116" t="s">
-        <v>585</v>
-      </c>
-      <c r="E116" t="s">
-        <v>2</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>345</v>
       </c>
       <c r="G116">
         <v>2</v>
@@ -5261,7 +5252,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B117" t="s">
         <v>346</v>
@@ -5270,10 +5261,10 @@
         <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E117" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>347</v>
@@ -5293,13 +5284,13 @@
         <v>1</v>
       </c>
       <c r="D118" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E118" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>350</v>
+        <v>31</v>
       </c>
       <c r="G118">
         <v>2</v>
@@ -5307,22 +5298,22 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
+        <v>350</v>
+      </c>
+      <c r="B119" t="s">
         <v>351</v>
       </c>
-      <c r="B119" t="s">
-        <v>352</v>
-      </c>
       <c r="C119">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="E119" t="s">
         <v>30</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="G119">
         <v>2</v>
@@ -5330,48 +5321,48 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
+        <v>352</v>
+      </c>
+      <c r="B120" t="s">
         <v>353</v>
       </c>
-      <c r="B120" t="s">
-        <v>354</v>
-      </c>
       <c r="C120">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D120" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="E120" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="G120">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
+        <v>354</v>
+      </c>
+      <c r="B121" t="s">
         <v>355</v>
       </c>
-      <c r="B121" t="s">
+      <c r="C121">
+        <v>1</v>
+      </c>
+      <c r="D121" t="s">
+        <v>588</v>
+      </c>
+      <c r="E121" t="s">
+        <v>56</v>
+      </c>
+      <c r="F121" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="C121">
-        <v>4</v>
-      </c>
-      <c r="D121" t="s">
-        <v>590</v>
-      </c>
-      <c r="E121" t="s">
-        <v>2</v>
-      </c>
-      <c r="F121" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="G121">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
@@ -5382,16 +5373,16 @@
         <v>358</v>
       </c>
       <c r="C122">
-        <v>1</v>
-      </c>
-      <c r="D122" t="s">
-        <v>591</v>
+        <v>2</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>589</v>
       </c>
       <c r="E122" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>359</v>
+        <v>231</v>
       </c>
       <c r="G122">
         <v>2</v>
@@ -5399,22 +5390,22 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
+        <v>359</v>
+      </c>
+      <c r="B123" t="s">
         <v>360</v>
       </c>
-      <c r="B123" t="s">
+      <c r="C123">
+        <v>1</v>
+      </c>
+      <c r="D123" t="s">
+        <v>590</v>
+      </c>
+      <c r="E123" t="s">
+        <v>59</v>
+      </c>
+      <c r="F123" s="1" t="s">
         <v>361</v>
-      </c>
-      <c r="C123">
-        <v>2</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="E123" t="s">
-        <v>47</v>
-      </c>
-      <c r="F123" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="G123">
         <v>2</v>
@@ -5431,13 +5422,13 @@
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E124" t="s">
-        <v>59</v>
+        <v>364</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>364</v>
+        <v>283</v>
       </c>
       <c r="G124">
         <v>2</v>
@@ -5451,16 +5442,16 @@
         <v>366</v>
       </c>
       <c r="C125">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D125" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E125" t="s">
         <v>367</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>283</v>
+        <v>368</v>
       </c>
       <c r="G125">
         <v>2</v>
@@ -5468,25 +5459,25 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B126" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C126">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D126" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E126" t="s">
-        <v>370</v>
+        <v>235</v>
       </c>
       <c r="F126" s="1" t="s">
         <v>371</v>
       </c>
       <c r="G126">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
@@ -5497,19 +5488,19 @@
         <v>373</v>
       </c>
       <c r="C127">
-        <v>2</v>
-      </c>
-      <c r="D127" t="s">
-        <v>596</v>
+        <v>1</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>594</v>
       </c>
       <c r="E127" t="s">
-        <v>235</v>
+        <v>59</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>374</v>
       </c>
       <c r="G127">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.35">
@@ -5522,14 +5513,14 @@
       <c r="C128">
         <v>1</v>
       </c>
-      <c r="D128" s="2" t="s">
-        <v>597</v>
+      <c r="D128" t="s">
+        <v>595</v>
       </c>
       <c r="E128" t="s">
-        <v>59</v>
+        <v>377</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="G128">
         <v>2</v>
@@ -5537,22 +5528,22 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B129" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="E129" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="G129">
         <v>2</v>
@@ -5560,39 +5551,39 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B130" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C130">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D130" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E130" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="G130">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B131" t="s">
         <v>387</v>
       </c>
       <c r="C131">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E131" t="s">
         <v>388</v>
@@ -5612,16 +5603,16 @@
         <v>390</v>
       </c>
       <c r="C132">
-        <v>1</v>
-      </c>
-      <c r="D132" t="s">
-        <v>601</v>
+        <v>5</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>599</v>
       </c>
       <c r="E132" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G132">
         <v>1</v>
@@ -5629,22 +5620,22 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
+        <v>391</v>
+      </c>
+      <c r="B133" t="s">
+        <v>392</v>
+      </c>
+      <c r="C133">
+        <v>3</v>
+      </c>
+      <c r="D133" t="s">
+        <v>600</v>
+      </c>
+      <c r="E133" t="s">
         <v>393</v>
       </c>
-      <c r="B133" t="s">
-        <v>393</v>
-      </c>
-      <c r="C133">
-        <v>5</v>
-      </c>
-      <c r="D133" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="E133" t="s">
-        <v>391</v>
-      </c>
       <c r="F133" s="1" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="G133">
         <v>1</v>
@@ -5652,22 +5643,22 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B134" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C134">
         <v>3</v>
       </c>
       <c r="D134" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E134" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="G134">
         <v>1</v>
@@ -5675,22 +5666,22 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B135" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C135">
         <v>3</v>
       </c>
       <c r="D135" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E135" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="G135">
         <v>1</v>
@@ -5698,19 +5689,19 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B136" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C136">
         <v>3</v>
       </c>
       <c r="D136" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="E136" t="s">
-        <v>404</v>
+        <v>235</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>405</v>
@@ -5727,16 +5718,16 @@
         <v>407</v>
       </c>
       <c r="C137">
-        <v>3</v>
-      </c>
-      <c r="D137" t="s">
-        <v>606</v>
+        <v>4</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>604</v>
       </c>
       <c r="E137" t="s">
-        <v>235</v>
+        <v>408</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="G137">
         <v>1</v>
@@ -5744,22 +5735,22 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B138" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C138">
         <v>4</v>
       </c>
-      <c r="D138" s="2" t="s">
-        <v>607</v>
+      <c r="D138" t="s">
+        <v>605</v>
       </c>
       <c r="E138" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="G138">
         <v>1</v>
@@ -5767,22 +5758,22 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B139" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C139">
         <v>4</v>
       </c>
       <c r="D139" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="E139" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="G139">
         <v>1</v>
@@ -5790,22 +5781,22 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
+        <v>418</v>
+      </c>
+      <c r="B140" t="s">
+        <v>416</v>
+      </c>
+      <c r="C140">
+        <v>5</v>
+      </c>
+      <c r="D140" t="s">
+        <v>607</v>
+      </c>
+      <c r="E140" t="s">
         <v>417</v>
       </c>
-      <c r="B140" t="s">
-        <v>418</v>
-      </c>
-      <c r="C140">
-        <v>4</v>
-      </c>
-      <c r="D140" t="s">
-        <v>609</v>
-      </c>
-      <c r="E140" t="s">
-        <v>420</v>
-      </c>
       <c r="F140" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G140">
         <v>1</v>
@@ -5813,22 +5804,22 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
+        <v>419</v>
+      </c>
+      <c r="B141" t="s">
+        <v>420</v>
+      </c>
+      <c r="C141">
+        <v>4</v>
+      </c>
+      <c r="D141" t="s">
+        <v>608</v>
+      </c>
+      <c r="E141" t="s">
         <v>421</v>
       </c>
-      <c r="B141" t="s">
-        <v>419</v>
-      </c>
-      <c r="C141">
-        <v>5</v>
-      </c>
-      <c r="D141" t="s">
-        <v>610</v>
-      </c>
-      <c r="E141" t="s">
-        <v>420</v>
-      </c>
       <c r="F141" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G141">
         <v>1</v>
@@ -5836,22 +5827,22 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B142" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C142">
         <v>4</v>
       </c>
       <c r="D142" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="E142" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>426</v>
+        <v>337</v>
       </c>
       <c r="G142">
         <v>1</v>
@@ -5862,19 +5853,19 @@
         <v>427</v>
       </c>
       <c r="B143" t="s">
+        <v>427</v>
+      </c>
+      <c r="C143">
+        <v>2</v>
+      </c>
+      <c r="D143" t="s">
+        <v>610</v>
+      </c>
+      <c r="E143" t="s">
         <v>428</v>
       </c>
-      <c r="C143">
-        <v>4</v>
-      </c>
-      <c r="D143" t="s">
-        <v>612</v>
-      </c>
-      <c r="E143" t="s">
+      <c r="F143" s="1" t="s">
         <v>429</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>340</v>
       </c>
       <c r="G143">
         <v>1</v>
@@ -5888,16 +5879,16 @@
         <v>430</v>
       </c>
       <c r="C144">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D144" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="E144" t="s">
-        <v>431</v>
+        <v>367</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="G144">
         <v>1</v>
@@ -5905,48 +5896,48 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
+        <v>431</v>
+      </c>
+      <c r="B145" t="s">
+        <v>432</v>
+      </c>
+      <c r="C145">
+        <v>1</v>
+      </c>
+      <c r="D145" t="s">
+        <v>612</v>
+      </c>
+      <c r="E145" t="s">
         <v>433</v>
       </c>
-      <c r="B145" t="s">
-        <v>433</v>
-      </c>
-      <c r="C145">
-        <v>3</v>
-      </c>
-      <c r="D145" t="s">
-        <v>614</v>
-      </c>
-      <c r="E145" t="s">
-        <v>370</v>
-      </c>
       <c r="F145" s="1" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="G145">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B146" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C146">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D146" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="E146" t="s">
-        <v>436</v>
+        <v>235</v>
       </c>
       <c r="F146" s="1" t="s">
         <v>437</v>
       </c>
       <c r="G146">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.35">
@@ -5957,16 +5948,16 @@
         <v>439</v>
       </c>
       <c r="C147">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D147" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E147" t="s">
-        <v>235</v>
+        <v>440</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="G147">
         <v>1</v>
@@ -5974,22 +5965,22 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B148" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C148">
         <v>3</v>
       </c>
       <c r="D148" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="E148" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="G148">
         <v>1</v>
@@ -5997,22 +5988,22 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B149" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C149">
         <v>3</v>
       </c>
       <c r="D149" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E149" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="G149">
         <v>1</v>
@@ -6020,19 +6011,19 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B150" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C150">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D150" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E150" t="s">
-        <v>451</v>
+        <v>235</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>452</v>
@@ -6052,13 +6043,13 @@
         <v>4</v>
       </c>
       <c r="D151" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="E151" t="s">
-        <v>235</v>
+        <v>455</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="G151">
         <v>1</v>
@@ -6066,19 +6057,19 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B152" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C152">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D152" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="E152" t="s">
-        <v>458</v>
+        <v>2</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>459</v>
@@ -6095,16 +6086,16 @@
         <v>461</v>
       </c>
       <c r="C153">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D153" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E153" t="s">
-        <v>2</v>
+        <v>462</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="G153">
         <v>1</v>
@@ -6112,22 +6103,22 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B154" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C154">
         <v>3</v>
       </c>
       <c r="D154" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E154" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="G154">
         <v>1</v>
@@ -6135,22 +6126,22 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>467</v>
+        <v>622</v>
       </c>
       <c r="B155" t="s">
-        <v>468</v>
+        <v>623</v>
       </c>
       <c r="C155">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D155" t="s">
+        <v>697</v>
+      </c>
+      <c r="E155" t="s">
+        <v>235</v>
+      </c>
+      <c r="F155" s="1" t="s">
         <v>624</v>
-      </c>
-      <c r="E155" t="s">
-        <v>469</v>
-      </c>
-      <c r="F155" s="1" t="s">
-        <v>470</v>
       </c>
       <c r="G155">
         <v>1</v>
@@ -6164,16 +6155,16 @@
         <v>626</v>
       </c>
       <c r="C156">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D156" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="E156" t="s">
-        <v>235</v>
+        <v>627</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="G156">
         <v>1</v>
@@ -6181,22 +6172,22 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B157" t="s">
         <v>629</v>
       </c>
       <c r="C157">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D157" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="E157" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="G157">
         <v>1</v>
@@ -6204,7 +6195,7 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B158" t="s">
         <v>632</v>
@@ -6213,13 +6204,13 @@
         <v>3</v>
       </c>
       <c r="D158" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="E158" t="s">
+        <v>627</v>
+      </c>
+      <c r="F158" s="1" t="s">
         <v>630</v>
-      </c>
-      <c r="F158" s="1" t="s">
-        <v>631</v>
       </c>
       <c r="G158">
         <v>1</v>
@@ -6227,22 +6218,22 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
+        <v>633</v>
+      </c>
+      <c r="B159" t="s">
         <v>634</v>
-      </c>
-      <c r="B159" t="s">
-        <v>635</v>
       </c>
       <c r="C159">
         <v>3</v>
       </c>
       <c r="D159" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="E159" t="s">
+        <v>47</v>
+      </c>
+      <c r="F159" s="1" t="s">
         <v>630</v>
-      </c>
-      <c r="F159" s="1" t="s">
-        <v>633</v>
       </c>
       <c r="G159">
         <v>1</v>
@@ -6250,22 +6241,22 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
+        <v>635</v>
+      </c>
+      <c r="B160" t="s">
         <v>636</v>
-      </c>
-      <c r="B160" t="s">
-        <v>637</v>
       </c>
       <c r="C160">
         <v>3</v>
       </c>
       <c r="D160" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="E160" t="s">
-        <v>47</v>
+        <v>257</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="G160">
         <v>1</v>
@@ -6282,10 +6273,10 @@
         <v>3</v>
       </c>
       <c r="D161" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="E161" t="s">
-        <v>257</v>
+        <v>627</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>640</v>
@@ -6305,13 +6296,13 @@
         <v>3</v>
       </c>
       <c r="D162" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="E162" t="s">
-        <v>630</v>
+        <v>643</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="G162">
         <v>1</v>
@@ -6319,19 +6310,19 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B163" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="C163">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D163" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="E163" t="s">
-        <v>646</v>
+        <v>627</v>
       </c>
       <c r="F163" s="1" t="s">
         <v>647</v>
@@ -6351,10 +6342,10 @@
         <v>2</v>
       </c>
       <c r="D164" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="E164" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>650</v>
@@ -6371,13 +6362,13 @@
         <v>652</v>
       </c>
       <c r="C165">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D165" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E165" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="F165" s="1" t="s">
         <v>653</v>
@@ -6397,13 +6388,13 @@
         <v>4</v>
       </c>
       <c r="D166" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E166" t="s">
-        <v>630</v>
+        <v>656</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G166">
         <v>1</v>
@@ -6414,19 +6405,19 @@
         <v>657</v>
       </c>
       <c r="B167" t="s">
+        <v>657</v>
+      </c>
+      <c r="C167">
+        <v>2</v>
+      </c>
+      <c r="D167" t="s">
+        <v>709</v>
+      </c>
+      <c r="E167" t="s">
         <v>658</v>
       </c>
-      <c r="C167">
-        <v>4</v>
-      </c>
-      <c r="D167" t="s">
-        <v>711</v>
-      </c>
-      <c r="E167" t="s">
-        <v>659</v>
-      </c>
       <c r="F167" s="1" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G167">
         <v>1</v>
@@ -6434,22 +6425,22 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
+        <v>659</v>
+      </c>
+      <c r="B168" t="s">
+        <v>687</v>
+      </c>
+      <c r="C168">
+        <v>3</v>
+      </c>
+      <c r="D168" t="s">
+        <v>710</v>
+      </c>
+      <c r="E168" t="s">
+        <v>627</v>
+      </c>
+      <c r="F168" s="1" t="s">
         <v>660</v>
-      </c>
-      <c r="B168" t="s">
-        <v>660</v>
-      </c>
-      <c r="C168">
-        <v>2</v>
-      </c>
-      <c r="D168" t="s">
-        <v>712</v>
-      </c>
-      <c r="E168" t="s">
-        <v>661</v>
-      </c>
-      <c r="F168" s="1" t="s">
-        <v>656</v>
       </c>
       <c r="G168">
         <v>1</v>
@@ -6457,19 +6448,19 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B169" t="s">
         <v>690</v>
       </c>
       <c r="C169">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D169" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="E169" t="s">
-        <v>630</v>
+        <v>662</v>
       </c>
       <c r="F169" s="1" t="s">
         <v>663</v>
@@ -6483,19 +6474,19 @@
         <v>664</v>
       </c>
       <c r="B170" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C170">
         <v>2</v>
       </c>
       <c r="D170" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="E170" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="G170">
         <v>1</v>
@@ -6503,22 +6494,22 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
+        <v>665</v>
+      </c>
+      <c r="B171" t="s">
+        <v>692</v>
+      </c>
+      <c r="C171">
+        <v>2</v>
+      </c>
+      <c r="D171" t="s">
+        <v>713</v>
+      </c>
+      <c r="E171" t="s">
+        <v>666</v>
+      </c>
+      <c r="F171" s="1" t="s">
         <v>667</v>
-      </c>
-      <c r="B171" t="s">
-        <v>694</v>
-      </c>
-      <c r="C171">
-        <v>2</v>
-      </c>
-      <c r="D171" t="s">
-        <v>715</v>
-      </c>
-      <c r="E171" t="s">
-        <v>661</v>
-      </c>
-      <c r="F171" s="1" t="s">
-        <v>666</v>
       </c>
       <c r="G171">
         <v>1</v>
@@ -6529,19 +6520,19 @@
         <v>668</v>
       </c>
       <c r="B172" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
       <c r="C172">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D172" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="E172" t="s">
         <v>669</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="G172">
         <v>1</v>
@@ -6549,22 +6540,22 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
+        <v>670</v>
+      </c>
+      <c r="B173" t="s">
+        <v>670</v>
+      </c>
+      <c r="C173">
+        <v>2</v>
+      </c>
+      <c r="D173" t="s">
+        <v>715</v>
+      </c>
+      <c r="E173" t="s">
+        <v>627</v>
+      </c>
+      <c r="F173" s="1" t="s">
         <v>671</v>
-      </c>
-      <c r="B173" t="s">
-        <v>691</v>
-      </c>
-      <c r="C173">
-        <v>3</v>
-      </c>
-      <c r="D173" t="s">
-        <v>717</v>
-      </c>
-      <c r="E173" t="s">
-        <v>672</v>
-      </c>
-      <c r="F173" s="1" t="s">
-        <v>670</v>
       </c>
       <c r="G173">
         <v>1</v>
@@ -6572,22 +6563,22 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
+        <v>672</v>
+      </c>
+      <c r="B174" t="s">
+        <v>672</v>
+      </c>
+      <c r="C174">
+        <v>2</v>
+      </c>
+      <c r="D174" t="s">
+        <v>716</v>
+      </c>
+      <c r="E174" t="s">
+        <v>658</v>
+      </c>
+      <c r="F174" s="1" t="s">
         <v>673</v>
-      </c>
-      <c r="B174" t="s">
-        <v>673</v>
-      </c>
-      <c r="C174">
-        <v>2</v>
-      </c>
-      <c r="D174" t="s">
-        <v>718</v>
-      </c>
-      <c r="E174" t="s">
-        <v>630</v>
-      </c>
-      <c r="F174" s="1" t="s">
-        <v>674</v>
       </c>
       <c r="G174">
         <v>1</v>
@@ -6595,22 +6586,22 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
+        <v>674</v>
+      </c>
+      <c r="B175" t="s">
+        <v>674</v>
+      </c>
+      <c r="C175">
+        <v>4</v>
+      </c>
+      <c r="D175" t="s">
+        <v>717</v>
+      </c>
+      <c r="E175" t="s">
+        <v>627</v>
+      </c>
+      <c r="F175" s="1" t="s">
         <v>675</v>
-      </c>
-      <c r="B175" t="s">
-        <v>675</v>
-      </c>
-      <c r="C175">
-        <v>2</v>
-      </c>
-      <c r="D175" t="s">
-        <v>719</v>
-      </c>
-      <c r="E175" t="s">
-        <v>661</v>
-      </c>
-      <c r="F175" s="1" t="s">
-        <v>676</v>
       </c>
       <c r="G175">
         <v>1</v>
@@ -6618,22 +6609,22 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B176" t="s">
-        <v>677</v>
+        <v>693</v>
       </c>
       <c r="C176">
         <v>4</v>
       </c>
       <c r="D176" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="E176" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G176">
         <v>1</v>
@@ -6641,19 +6632,19 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B177" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C177">
         <v>4</v>
       </c>
       <c r="D177" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="E177" t="s">
-        <v>630</v>
+        <v>679</v>
       </c>
       <c r="F177" s="1" t="s">
         <v>680</v>
@@ -6667,19 +6658,19 @@
         <v>681</v>
       </c>
       <c r="B178" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C178">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D178" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E178" t="s">
+        <v>393</v>
+      </c>
+      <c r="F178" s="1" t="s">
         <v>682</v>
-      </c>
-      <c r="F178" s="1" t="s">
-        <v>683</v>
       </c>
       <c r="G178">
         <v>1</v>
@@ -6687,22 +6678,22 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
+        <v>683</v>
+      </c>
+      <c r="B179" t="s">
+        <v>696</v>
+      </c>
+      <c r="C179">
+        <v>4</v>
+      </c>
+      <c r="D179" t="s">
+        <v>721</v>
+      </c>
+      <c r="E179" t="s">
+        <v>627</v>
+      </c>
+      <c r="F179" s="1" t="s">
         <v>684</v>
-      </c>
-      <c r="B179" t="s">
-        <v>698</v>
-      </c>
-      <c r="C179">
-        <v>3</v>
-      </c>
-      <c r="D179" t="s">
-        <v>723</v>
-      </c>
-      <c r="E179" t="s">
-        <v>396</v>
-      </c>
-      <c r="F179" s="1" t="s">
-        <v>685</v>
       </c>
       <c r="G179">
         <v>1</v>
@@ -6710,47 +6701,24 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
+        <v>685</v>
+      </c>
+      <c r="B180" t="s">
+        <v>689</v>
+      </c>
+      <c r="C180">
+        <v>3</v>
+      </c>
+      <c r="D180" t="s">
+        <v>722</v>
+      </c>
+      <c r="E180" t="s">
+        <v>662</v>
+      </c>
+      <c r="F180" s="1" t="s">
         <v>686</v>
       </c>
-      <c r="B180" t="s">
-        <v>699</v>
-      </c>
-      <c r="C180">
-        <v>4</v>
-      </c>
-      <c r="D180" t="s">
-        <v>724</v>
-      </c>
-      <c r="E180" t="s">
-        <v>630</v>
-      </c>
-      <c r="F180" s="1" t="s">
-        <v>687</v>
-      </c>
       <c r="G180">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A181" t="s">
-        <v>688</v>
-      </c>
-      <c r="B181" t="s">
-        <v>692</v>
-      </c>
-      <c r="C181">
-        <v>3</v>
-      </c>
-      <c r="D181" t="s">
-        <v>725</v>
-      </c>
-      <c r="E181" t="s">
-        <v>665</v>
-      </c>
-      <c r="F181" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="G181">
         <v>1</v>
       </c>
     </row>
@@ -6766,10 +6734,10 @@
     <hyperlink ref="D102" r:id="rId8" xr:uid="{B1C1C455-40F5-40EE-A262-823F3E505DBF}"/>
     <hyperlink ref="D106" r:id="rId9" xr:uid="{5ED76D23-4021-4CF4-AFAD-4B6FCD5FEE8B}"/>
     <hyperlink ref="D109" r:id="rId10" xr:uid="{156C7FA4-7F1A-43A6-ADC7-4A2A79F1521A}"/>
-    <hyperlink ref="D123" r:id="rId11" xr:uid="{4FF446EB-2121-41E9-8CCE-DD52240BE193}"/>
-    <hyperlink ref="D128" r:id="rId12" xr:uid="{011A385D-83C1-49F3-94A8-2D57AB8D51DF}"/>
-    <hyperlink ref="D133" r:id="rId13" xr:uid="{E7D95AC4-DDCF-42F1-B07F-DE761BAA8A6A}"/>
-    <hyperlink ref="D138" r:id="rId14" xr:uid="{F6402070-B9B1-454F-9BA1-B301D9287D55}"/>
+    <hyperlink ref="D122" r:id="rId11" xr:uid="{4FF446EB-2121-41E9-8CCE-DD52240BE193}"/>
+    <hyperlink ref="D127" r:id="rId12" xr:uid="{011A385D-83C1-49F3-94A8-2D57AB8D51DF}"/>
+    <hyperlink ref="D132" r:id="rId13" xr:uid="{E7D95AC4-DDCF-42F1-B07F-DE761BAA8A6A}"/>
+    <hyperlink ref="D137" r:id="rId14" xr:uid="{F6402070-B9B1-454F-9BA1-B301D9287D55}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId15"/>

</xml_diff>